<commit_message>
Update version - 28/12/2023 ~2:00pm
</commit_message>
<xml_diff>
--- a/test_savedata.xlsx
+++ b/test_savedata.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:AK15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -430,11 +430,26 @@
  End day of week: Thursday 11</t>
         </is>
       </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>TOTAL HOURS (ACCUMULATED)</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>REGULAR HOURS</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>OVERTIME HOURS (PER DAY)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Names</t>
+          <t>NAMES</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -485,6 +500,116 @@
       <c r="K2" t="inlineStr">
         <is>
           <t>TOTAL OVERTIME HOURS - WEEKLY</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Friday 5</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Saturday 6</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Sunday 7</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Monday 8</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Tuesday 9</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Wednesday 10</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Thursday 11</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>Friday 5</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>Saturday 6</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>Sunday 7</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>Monday 8</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>Tuesday 9</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>Wednesday 10</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>Thursday 11</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>Friday 5</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>Saturday 6</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>Sunday 7</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>Monday 8</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>Tuesday 9</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>Wednesday 10</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>Thursday 11</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>NAMES</t>
         </is>
       </c>
     </row>
@@ -534,6 +659,95 @@
         <f>I3-J3</f>
         <v/>
       </c>
+      <c r="N3">
+        <f>B3</f>
+        <v/>
+      </c>
+      <c r="O3">
+        <f>C3+N3</f>
+        <v/>
+      </c>
+      <c r="P3">
+        <f>D3+O3</f>
+        <v/>
+      </c>
+      <c r="Q3">
+        <f>E3+P3</f>
+        <v/>
+      </c>
+      <c r="R3">
+        <f>F3+Q3</f>
+        <v/>
+      </c>
+      <c r="S3">
+        <f>G3+R3</f>
+        <v/>
+      </c>
+      <c r="T3">
+        <f>H3+S3</f>
+        <v/>
+      </c>
+      <c r="V3">
+        <f>N3</f>
+        <v/>
+      </c>
+      <c r="W3">
+        <f>IF(O3&lt;=0, 0, IF(O3&lt;=40,O3-N3,IF(O3-N3&lt;=0, 0, ABS(O3-N3-AE3))))</f>
+        <v/>
+      </c>
+      <c r="X3">
+        <f>IF(P3&lt;=0, 0, IF(P3&lt;=40,P3-O3,IF(P3-O3&lt;=0, 0, ABS(P3-O3-AF3))))</f>
+        <v/>
+      </c>
+      <c r="Y3">
+        <f>IF(Q3&lt;=0, 0, IF(Q3&lt;=40,Q3-P3,IF(Q3-P3&lt;=0, 0, ABS(Q3-P3-AG3))))</f>
+        <v/>
+      </c>
+      <c r="Z3">
+        <f>IF(R3&lt;=0, 0, IF(R3&lt;=40,R3-Q3,IF(R3-Q3&lt;=0, 0, ABS(R3-Q3-AH3))))</f>
+        <v/>
+      </c>
+      <c r="AA3">
+        <f>IF(S3&lt;=0, 0, IF(S3&lt;=40,S3-R3,IF(S3-R3&lt;=0, 0, ABS(S3-R3-AI3))))</f>
+        <v/>
+      </c>
+      <c r="AB3">
+        <f>IF(T3&lt;=0, 0, IF(T3&lt;=40,T3-S3,IF(T3-S3&lt;=0, 0, ABS(T3-S3-AJ3))))</f>
+        <v/>
+      </c>
+      <c r="AD3">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE3">
+        <f>IF(O3&lt;=0, 0, IF(O3&lt;=40,0, IF(O3-N3&lt;=0,0,IF(O3&gt;40, O3-40-SUM(AD3:AD3),0))))</f>
+        <v/>
+      </c>
+      <c r="AF3">
+        <f>IF(P3&lt;=0, 0, IF(P3&lt;=40,0, IF(P3-O3&lt;=0,0,IF(P3&gt;40, P3-40-SUM(AD3:AE3),0))))</f>
+        <v/>
+      </c>
+      <c r="AG3">
+        <f>IF(Q3&lt;=0, 0, IF(Q3&lt;=40,0, IF(Q3-P3&lt;=0,0,IF(Q3&gt;40, Q3-40-SUM(AD3:AF3),0))))</f>
+        <v/>
+      </c>
+      <c r="AH3">
+        <f>IF(R3&lt;=0, 0, IF(R3&lt;=40,0, IF(R3-Q3&lt;=0,0,IF(R3&gt;40, R3-40-SUM(AD3:AG3),0))))</f>
+        <v/>
+      </c>
+      <c r="AI3">
+        <f>IF(S3&lt;=0, 0, IF(S3&lt;=40,0, IF(S3-R3&lt;=0,0,IF(S3&gt;40, S3-40-SUM(AD3:AH3),0))))</f>
+        <v/>
+      </c>
+      <c r="AJ3">
+        <f>IF(T3&lt;=0, 0, IF(T3&lt;=40,0, IF(T3-S3&lt;=0,0,IF(T3&gt;40, T3-40-SUM(AD3:AI3),0))))</f>
+        <v/>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>ClaudiaGil</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -581,6 +795,95 @@
         <f>I4-J4</f>
         <v/>
       </c>
+      <c r="N4">
+        <f>B4</f>
+        <v/>
+      </c>
+      <c r="O4">
+        <f>C4+N4</f>
+        <v/>
+      </c>
+      <c r="P4">
+        <f>D4+O4</f>
+        <v/>
+      </c>
+      <c r="Q4">
+        <f>E4+P4</f>
+        <v/>
+      </c>
+      <c r="R4">
+        <f>F4+Q4</f>
+        <v/>
+      </c>
+      <c r="S4">
+        <f>G4+R4</f>
+        <v/>
+      </c>
+      <c r="T4">
+        <f>H4+S4</f>
+        <v/>
+      </c>
+      <c r="V4">
+        <f>N4</f>
+        <v/>
+      </c>
+      <c r="W4">
+        <f>IF(O4&lt;=0, 0, IF(O4&lt;=40,O4-N4,IF(O4-N4&lt;=0, 0, ABS(O4-N4-AE4))))</f>
+        <v/>
+      </c>
+      <c r="X4">
+        <f>IF(P4&lt;=0, 0, IF(P4&lt;=40,P4-O4,IF(P4-O4&lt;=0, 0, ABS(P4-O4-AF4))))</f>
+        <v/>
+      </c>
+      <c r="Y4">
+        <f>IF(Q4&lt;=0, 0, IF(Q4&lt;=40,Q4-P4,IF(Q4-P4&lt;=0, 0, ABS(Q4-P4-AG4))))</f>
+        <v/>
+      </c>
+      <c r="Z4">
+        <f>IF(R4&lt;=0, 0, IF(R4&lt;=40,R4-Q4,IF(R4-Q4&lt;=0, 0, ABS(R4-Q4-AH4))))</f>
+        <v/>
+      </c>
+      <c r="AA4">
+        <f>IF(S4&lt;=0, 0, IF(S4&lt;=40,S4-R4,IF(S4-R4&lt;=0, 0, ABS(S4-R4-AI4))))</f>
+        <v/>
+      </c>
+      <c r="AB4">
+        <f>IF(T4&lt;=0, 0, IF(T4&lt;=40,T4-S4,IF(T4-S4&lt;=0, 0, ABS(T4-S4-AJ4))))</f>
+        <v/>
+      </c>
+      <c r="AD4">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE4">
+        <f>IF(O4&lt;=0, 0, IF(O4&lt;=40,0, IF(O4-N4&lt;=0,0,IF(O4&gt;40, O4-40-SUM(AD4:AD4),0))))</f>
+        <v/>
+      </c>
+      <c r="AF4">
+        <f>IF(P4&lt;=0, 0, IF(P4&lt;=40,0, IF(P4-O4&lt;=0,0,IF(P4&gt;40, P4-40-SUM(AD4:AE4),0))))</f>
+        <v/>
+      </c>
+      <c r="AG4">
+        <f>IF(Q4&lt;=0, 0, IF(Q4&lt;=40,0, IF(Q4-P4&lt;=0,0,IF(Q4&gt;40, Q4-40-SUM(AD4:AF4),0))))</f>
+        <v/>
+      </c>
+      <c r="AH4">
+        <f>IF(R4&lt;=0, 0, IF(R4&lt;=40,0, IF(R4-Q4&lt;=0,0,IF(R4&gt;40, R4-40-SUM(AD4:AG4),0))))</f>
+        <v/>
+      </c>
+      <c r="AI4">
+        <f>IF(S4&lt;=0, 0, IF(S4&lt;=40,0, IF(S4-R4&lt;=0,0,IF(S4&gt;40, S4-40-SUM(AD4:AH4),0))))</f>
+        <v/>
+      </c>
+      <c r="AJ4">
+        <f>IF(T4&lt;=0, 0, IF(T4&lt;=40,0, IF(T4-S4&lt;=0,0,IF(T4&gt;40, T4-40-SUM(AD4:AI4),0))))</f>
+        <v/>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>Darwinparedes</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -628,6 +931,95 @@
         <f>I5-J5</f>
         <v/>
       </c>
+      <c r="N5">
+        <f>B5</f>
+        <v/>
+      </c>
+      <c r="O5">
+        <f>C5+N5</f>
+        <v/>
+      </c>
+      <c r="P5">
+        <f>D5+O5</f>
+        <v/>
+      </c>
+      <c r="Q5">
+        <f>E5+P5</f>
+        <v/>
+      </c>
+      <c r="R5">
+        <f>F5+Q5</f>
+        <v/>
+      </c>
+      <c r="S5">
+        <f>G5+R5</f>
+        <v/>
+      </c>
+      <c r="T5">
+        <f>H5+S5</f>
+        <v/>
+      </c>
+      <c r="V5">
+        <f>N5</f>
+        <v/>
+      </c>
+      <c r="W5">
+        <f>IF(O5&lt;=0, 0, IF(O5&lt;=40,O5-N5,IF(O5-N5&lt;=0, 0, ABS(O5-N5-AE5))))</f>
+        <v/>
+      </c>
+      <c r="X5">
+        <f>IF(P5&lt;=0, 0, IF(P5&lt;=40,P5-O5,IF(P5-O5&lt;=0, 0, ABS(P5-O5-AF5))))</f>
+        <v/>
+      </c>
+      <c r="Y5">
+        <f>IF(Q5&lt;=0, 0, IF(Q5&lt;=40,Q5-P5,IF(Q5-P5&lt;=0, 0, ABS(Q5-P5-AG5))))</f>
+        <v/>
+      </c>
+      <c r="Z5">
+        <f>IF(R5&lt;=0, 0, IF(R5&lt;=40,R5-Q5,IF(R5-Q5&lt;=0, 0, ABS(R5-Q5-AH5))))</f>
+        <v/>
+      </c>
+      <c r="AA5">
+        <f>IF(S5&lt;=0, 0, IF(S5&lt;=40,S5-R5,IF(S5-R5&lt;=0, 0, ABS(S5-R5-AI5))))</f>
+        <v/>
+      </c>
+      <c r="AB5">
+        <f>IF(T5&lt;=0, 0, IF(T5&lt;=40,T5-S5,IF(T5-S5&lt;=0, 0, ABS(T5-S5-AJ5))))</f>
+        <v/>
+      </c>
+      <c r="AD5">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE5">
+        <f>IF(O5&lt;=0, 0, IF(O5&lt;=40,0, IF(O5-N5&lt;=0,0,IF(O5&gt;40, O5-40-SUM(AD5:AD5),0))))</f>
+        <v/>
+      </c>
+      <c r="AF5">
+        <f>IF(P5&lt;=0, 0, IF(P5&lt;=40,0, IF(P5-O5&lt;=0,0,IF(P5&gt;40, P5-40-SUM(AD5:AE5),0))))</f>
+        <v/>
+      </c>
+      <c r="AG5">
+        <f>IF(Q5&lt;=0, 0, IF(Q5&lt;=40,0, IF(Q5-P5&lt;=0,0,IF(Q5&gt;40, Q5-40-SUM(AD5:AF5),0))))</f>
+        <v/>
+      </c>
+      <c r="AH5">
+        <f>IF(R5&lt;=0, 0, IF(R5&lt;=40,0, IF(R5-Q5&lt;=0,0,IF(R5&gt;40, R5-40-SUM(AD5:AG5),0))))</f>
+        <v/>
+      </c>
+      <c r="AI5">
+        <f>IF(S5&lt;=0, 0, IF(S5&lt;=40,0, IF(S5-R5&lt;=0,0,IF(S5&gt;40, S5-40-SUM(AD5:AH5),0))))</f>
+        <v/>
+      </c>
+      <c r="AJ5">
+        <f>IF(T5&lt;=0, 0, IF(T5&lt;=40,0, IF(T5-S5&lt;=0,0,IF(T5&gt;40, T5-40-SUM(AD5:AI5),0))))</f>
+        <v/>
+      </c>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t>EdgarCamacho</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -675,6 +1067,95 @@
         <f>I6-J6</f>
         <v/>
       </c>
+      <c r="N6">
+        <f>B6</f>
+        <v/>
+      </c>
+      <c r="O6">
+        <f>C6+N6</f>
+        <v/>
+      </c>
+      <c r="P6">
+        <f>D6+O6</f>
+        <v/>
+      </c>
+      <c r="Q6">
+        <f>E6+P6</f>
+        <v/>
+      </c>
+      <c r="R6">
+        <f>F6+Q6</f>
+        <v/>
+      </c>
+      <c r="S6">
+        <f>G6+R6</f>
+        <v/>
+      </c>
+      <c r="T6">
+        <f>H6+S6</f>
+        <v/>
+      </c>
+      <c r="V6">
+        <f>N6</f>
+        <v/>
+      </c>
+      <c r="W6">
+        <f>IF(O6&lt;=0, 0, IF(O6&lt;=40,O6-N6,IF(O6-N6&lt;=0, 0, ABS(O6-N6-AE6))))</f>
+        <v/>
+      </c>
+      <c r="X6">
+        <f>IF(P6&lt;=0, 0, IF(P6&lt;=40,P6-O6,IF(P6-O6&lt;=0, 0, ABS(P6-O6-AF6))))</f>
+        <v/>
+      </c>
+      <c r="Y6">
+        <f>IF(Q6&lt;=0, 0, IF(Q6&lt;=40,Q6-P6,IF(Q6-P6&lt;=0, 0, ABS(Q6-P6-AG6))))</f>
+        <v/>
+      </c>
+      <c r="Z6">
+        <f>IF(R6&lt;=0, 0, IF(R6&lt;=40,R6-Q6,IF(R6-Q6&lt;=0, 0, ABS(R6-Q6-AH6))))</f>
+        <v/>
+      </c>
+      <c r="AA6">
+        <f>IF(S6&lt;=0, 0, IF(S6&lt;=40,S6-R6,IF(S6-R6&lt;=0, 0, ABS(S6-R6-AI6))))</f>
+        <v/>
+      </c>
+      <c r="AB6">
+        <f>IF(T6&lt;=0, 0, IF(T6&lt;=40,T6-S6,IF(T6-S6&lt;=0, 0, ABS(T6-S6-AJ6))))</f>
+        <v/>
+      </c>
+      <c r="AD6">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE6">
+        <f>IF(O6&lt;=0, 0, IF(O6&lt;=40,0, IF(O6-N6&lt;=0,0,IF(O6&gt;40, O6-40-SUM(AD6:AD6),0))))</f>
+        <v/>
+      </c>
+      <c r="AF6">
+        <f>IF(P6&lt;=0, 0, IF(P6&lt;=40,0, IF(P6-O6&lt;=0,0,IF(P6&gt;40, P6-40-SUM(AD6:AE6),0))))</f>
+        <v/>
+      </c>
+      <c r="AG6">
+        <f>IF(Q6&lt;=0, 0, IF(Q6&lt;=40,0, IF(Q6-P6&lt;=0,0,IF(Q6&gt;40, Q6-40-SUM(AD6:AF6),0))))</f>
+        <v/>
+      </c>
+      <c r="AH6">
+        <f>IF(R6&lt;=0, 0, IF(R6&lt;=40,0, IF(R6-Q6&lt;=0,0,IF(R6&gt;40, R6-40-SUM(AD6:AG6),0))))</f>
+        <v/>
+      </c>
+      <c r="AI6">
+        <f>IF(S6&lt;=0, 0, IF(S6&lt;=40,0, IF(S6-R6&lt;=0,0,IF(S6&gt;40, S6-40-SUM(AD6:AH6),0))))</f>
+        <v/>
+      </c>
+      <c r="AJ6">
+        <f>IF(T6&lt;=0, 0, IF(T6&lt;=40,0, IF(T6-S6&lt;=0,0,IF(T6&gt;40, T6-40-SUM(AD6:AI6),0))))</f>
+        <v/>
+      </c>
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t>EduardodeSouza</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -722,6 +1203,95 @@
         <f>I7-J7</f>
         <v/>
       </c>
+      <c r="N7">
+        <f>B7</f>
+        <v/>
+      </c>
+      <c r="O7">
+        <f>C7+N7</f>
+        <v/>
+      </c>
+      <c r="P7">
+        <f>D7+O7</f>
+        <v/>
+      </c>
+      <c r="Q7">
+        <f>E7+P7</f>
+        <v/>
+      </c>
+      <c r="R7">
+        <f>F7+Q7</f>
+        <v/>
+      </c>
+      <c r="S7">
+        <f>G7+R7</f>
+        <v/>
+      </c>
+      <c r="T7">
+        <f>H7+S7</f>
+        <v/>
+      </c>
+      <c r="V7">
+        <f>N7</f>
+        <v/>
+      </c>
+      <c r="W7">
+        <f>IF(O7&lt;=0, 0, IF(O7&lt;=40,O7-N7,IF(O7-N7&lt;=0, 0, ABS(O7-N7-AE7))))</f>
+        <v/>
+      </c>
+      <c r="X7">
+        <f>IF(P7&lt;=0, 0, IF(P7&lt;=40,P7-O7,IF(P7-O7&lt;=0, 0, ABS(P7-O7-AF7))))</f>
+        <v/>
+      </c>
+      <c r="Y7">
+        <f>IF(Q7&lt;=0, 0, IF(Q7&lt;=40,Q7-P7,IF(Q7-P7&lt;=0, 0, ABS(Q7-P7-AG7))))</f>
+        <v/>
+      </c>
+      <c r="Z7">
+        <f>IF(R7&lt;=0, 0, IF(R7&lt;=40,R7-Q7,IF(R7-Q7&lt;=0, 0, ABS(R7-Q7-AH7))))</f>
+        <v/>
+      </c>
+      <c r="AA7">
+        <f>IF(S7&lt;=0, 0, IF(S7&lt;=40,S7-R7,IF(S7-R7&lt;=0, 0, ABS(S7-R7-AI7))))</f>
+        <v/>
+      </c>
+      <c r="AB7">
+        <f>IF(T7&lt;=0, 0, IF(T7&lt;=40,T7-S7,IF(T7-S7&lt;=0, 0, ABS(T7-S7-AJ7))))</f>
+        <v/>
+      </c>
+      <c r="AD7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE7">
+        <f>IF(O7&lt;=0, 0, IF(O7&lt;=40,0, IF(O7-N7&lt;=0,0,IF(O7&gt;40, O7-40-SUM(AD7:AD7),0))))</f>
+        <v/>
+      </c>
+      <c r="AF7">
+        <f>IF(P7&lt;=0, 0, IF(P7&lt;=40,0, IF(P7-O7&lt;=0,0,IF(P7&gt;40, P7-40-SUM(AD7:AE7),0))))</f>
+        <v/>
+      </c>
+      <c r="AG7">
+        <f>IF(Q7&lt;=0, 0, IF(Q7&lt;=40,0, IF(Q7-P7&lt;=0,0,IF(Q7&gt;40, Q7-40-SUM(AD7:AF7),0))))</f>
+        <v/>
+      </c>
+      <c r="AH7">
+        <f>IF(R7&lt;=0, 0, IF(R7&lt;=40,0, IF(R7-Q7&lt;=0,0,IF(R7&gt;40, R7-40-SUM(AD7:AG7),0))))</f>
+        <v/>
+      </c>
+      <c r="AI7">
+        <f>IF(S7&lt;=0, 0, IF(S7&lt;=40,0, IF(S7-R7&lt;=0,0,IF(S7&gt;40, S7-40-SUM(AD7:AH7),0))))</f>
+        <v/>
+      </c>
+      <c r="AJ7">
+        <f>IF(T7&lt;=0, 0, IF(T7&lt;=40,0, IF(T7-S7&lt;=0,0,IF(T7&gt;40, T7-40-SUM(AD7:AI7),0))))</f>
+        <v/>
+      </c>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t>Eliasalbornoz</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -769,6 +1339,95 @@
         <f>I8-J8</f>
         <v/>
       </c>
+      <c r="N8">
+        <f>B8</f>
+        <v/>
+      </c>
+      <c r="O8">
+        <f>C8+N8</f>
+        <v/>
+      </c>
+      <c r="P8">
+        <f>D8+O8</f>
+        <v/>
+      </c>
+      <c r="Q8">
+        <f>E8+P8</f>
+        <v/>
+      </c>
+      <c r="R8">
+        <f>F8+Q8</f>
+        <v/>
+      </c>
+      <c r="S8">
+        <f>G8+R8</f>
+        <v/>
+      </c>
+      <c r="T8">
+        <f>H8+S8</f>
+        <v/>
+      </c>
+      <c r="V8">
+        <f>N8</f>
+        <v/>
+      </c>
+      <c r="W8">
+        <f>IF(O8&lt;=0, 0, IF(O8&lt;=40,O8-N8,IF(O8-N8&lt;=0, 0, ABS(O8-N8-AE8))))</f>
+        <v/>
+      </c>
+      <c r="X8">
+        <f>IF(P8&lt;=0, 0, IF(P8&lt;=40,P8-O8,IF(P8-O8&lt;=0, 0, ABS(P8-O8-AF8))))</f>
+        <v/>
+      </c>
+      <c r="Y8">
+        <f>IF(Q8&lt;=0, 0, IF(Q8&lt;=40,Q8-P8,IF(Q8-P8&lt;=0, 0, ABS(Q8-P8-AG8))))</f>
+        <v/>
+      </c>
+      <c r="Z8">
+        <f>IF(R8&lt;=0, 0, IF(R8&lt;=40,R8-Q8,IF(R8-Q8&lt;=0, 0, ABS(R8-Q8-AH8))))</f>
+        <v/>
+      </c>
+      <c r="AA8">
+        <f>IF(S8&lt;=0, 0, IF(S8&lt;=40,S8-R8,IF(S8-R8&lt;=0, 0, ABS(S8-R8-AI8))))</f>
+        <v/>
+      </c>
+      <c r="AB8">
+        <f>IF(T8&lt;=0, 0, IF(T8&lt;=40,T8-S8,IF(T8-S8&lt;=0, 0, ABS(T8-S8-AJ8))))</f>
+        <v/>
+      </c>
+      <c r="AD8">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE8">
+        <f>IF(O8&lt;=0, 0, IF(O8&lt;=40,0, IF(O8-N8&lt;=0,0,IF(O8&gt;40, O8-40-SUM(AD8:AD8),0))))</f>
+        <v/>
+      </c>
+      <c r="AF8">
+        <f>IF(P8&lt;=0, 0, IF(P8&lt;=40,0, IF(P8-O8&lt;=0,0,IF(P8&gt;40, P8-40-SUM(AD8:AE8),0))))</f>
+        <v/>
+      </c>
+      <c r="AG8">
+        <f>IF(Q8&lt;=0, 0, IF(Q8&lt;=40,0, IF(Q8-P8&lt;=0,0,IF(Q8&gt;40, Q8-40-SUM(AD8:AF8),0))))</f>
+        <v/>
+      </c>
+      <c r="AH8">
+        <f>IF(R8&lt;=0, 0, IF(R8&lt;=40,0, IF(R8-Q8&lt;=0,0,IF(R8&gt;40, R8-40-SUM(AD8:AG8),0))))</f>
+        <v/>
+      </c>
+      <c r="AI8">
+        <f>IF(S8&lt;=0, 0, IF(S8&lt;=40,0, IF(S8-R8&lt;=0,0,IF(S8&gt;40, S8-40-SUM(AD8:AH8),0))))</f>
+        <v/>
+      </c>
+      <c r="AJ8">
+        <f>IF(T8&lt;=0, 0, IF(T8&lt;=40,0, IF(T8-S8&lt;=0,0,IF(T8&gt;40, T8-40-SUM(AD8:AI8),0))))</f>
+        <v/>
+      </c>
+      <c r="AK8" t="inlineStr">
+        <is>
+          <t>GermanCastro</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -816,6 +1475,95 @@
         <f>I9-J9</f>
         <v/>
       </c>
+      <c r="N9">
+        <f>B9</f>
+        <v/>
+      </c>
+      <c r="O9">
+        <f>C9+N9</f>
+        <v/>
+      </c>
+      <c r="P9">
+        <f>D9+O9</f>
+        <v/>
+      </c>
+      <c r="Q9">
+        <f>E9+P9</f>
+        <v/>
+      </c>
+      <c r="R9">
+        <f>F9+Q9</f>
+        <v/>
+      </c>
+      <c r="S9">
+        <f>G9+R9</f>
+        <v/>
+      </c>
+      <c r="T9">
+        <f>H9+S9</f>
+        <v/>
+      </c>
+      <c r="V9">
+        <f>N9</f>
+        <v/>
+      </c>
+      <c r="W9">
+        <f>IF(O9&lt;=0, 0, IF(O9&lt;=40,O9-N9,IF(O9-N9&lt;=0, 0, ABS(O9-N9-AE9))))</f>
+        <v/>
+      </c>
+      <c r="X9">
+        <f>IF(P9&lt;=0, 0, IF(P9&lt;=40,P9-O9,IF(P9-O9&lt;=0, 0, ABS(P9-O9-AF9))))</f>
+        <v/>
+      </c>
+      <c r="Y9">
+        <f>IF(Q9&lt;=0, 0, IF(Q9&lt;=40,Q9-P9,IF(Q9-P9&lt;=0, 0, ABS(Q9-P9-AG9))))</f>
+        <v/>
+      </c>
+      <c r="Z9">
+        <f>IF(R9&lt;=0, 0, IF(R9&lt;=40,R9-Q9,IF(R9-Q9&lt;=0, 0, ABS(R9-Q9-AH9))))</f>
+        <v/>
+      </c>
+      <c r="AA9">
+        <f>IF(S9&lt;=0, 0, IF(S9&lt;=40,S9-R9,IF(S9-R9&lt;=0, 0, ABS(S9-R9-AI9))))</f>
+        <v/>
+      </c>
+      <c r="AB9">
+        <f>IF(T9&lt;=0, 0, IF(T9&lt;=40,T9-S9,IF(T9-S9&lt;=0, 0, ABS(T9-S9-AJ9))))</f>
+        <v/>
+      </c>
+      <c r="AD9">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE9">
+        <f>IF(O9&lt;=0, 0, IF(O9&lt;=40,0, IF(O9-N9&lt;=0,0,IF(O9&gt;40, O9-40-SUM(AD9:AD9),0))))</f>
+        <v/>
+      </c>
+      <c r="AF9">
+        <f>IF(P9&lt;=0, 0, IF(P9&lt;=40,0, IF(P9-O9&lt;=0,0,IF(P9&gt;40, P9-40-SUM(AD9:AE9),0))))</f>
+        <v/>
+      </c>
+      <c r="AG9">
+        <f>IF(Q9&lt;=0, 0, IF(Q9&lt;=40,0, IF(Q9-P9&lt;=0,0,IF(Q9&gt;40, Q9-40-SUM(AD9:AF9),0))))</f>
+        <v/>
+      </c>
+      <c r="AH9">
+        <f>IF(R9&lt;=0, 0, IF(R9&lt;=40,0, IF(R9-Q9&lt;=0,0,IF(R9&gt;40, R9-40-SUM(AD9:AG9),0))))</f>
+        <v/>
+      </c>
+      <c r="AI9">
+        <f>IF(S9&lt;=0, 0, IF(S9&lt;=40,0, IF(S9-R9&lt;=0,0,IF(S9&gt;40, S9-40-SUM(AD9:AH9),0))))</f>
+        <v/>
+      </c>
+      <c r="AJ9">
+        <f>IF(T9&lt;=0, 0, IF(T9&lt;=40,0, IF(T9-S9&lt;=0,0,IF(T9&gt;40, T9-40-SUM(AD9:AI9),0))))</f>
+        <v/>
+      </c>
+      <c r="AK9" t="inlineStr">
+        <is>
+          <t>LuisJimenez</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -863,6 +1611,95 @@
         <f>I10-J10</f>
         <v/>
       </c>
+      <c r="N10">
+        <f>B10</f>
+        <v/>
+      </c>
+      <c r="O10">
+        <f>C10+N10</f>
+        <v/>
+      </c>
+      <c r="P10">
+        <f>D10+O10</f>
+        <v/>
+      </c>
+      <c r="Q10">
+        <f>E10+P10</f>
+        <v/>
+      </c>
+      <c r="R10">
+        <f>F10+Q10</f>
+        <v/>
+      </c>
+      <c r="S10">
+        <f>G10+R10</f>
+        <v/>
+      </c>
+      <c r="T10">
+        <f>H10+S10</f>
+        <v/>
+      </c>
+      <c r="V10">
+        <f>N10</f>
+        <v/>
+      </c>
+      <c r="W10">
+        <f>IF(O10&lt;=0, 0, IF(O10&lt;=40,O10-N10,IF(O10-N10&lt;=0, 0, ABS(O10-N10-AE10))))</f>
+        <v/>
+      </c>
+      <c r="X10">
+        <f>IF(P10&lt;=0, 0, IF(P10&lt;=40,P10-O10,IF(P10-O10&lt;=0, 0, ABS(P10-O10-AF10))))</f>
+        <v/>
+      </c>
+      <c r="Y10">
+        <f>IF(Q10&lt;=0, 0, IF(Q10&lt;=40,Q10-P10,IF(Q10-P10&lt;=0, 0, ABS(Q10-P10-AG10))))</f>
+        <v/>
+      </c>
+      <c r="Z10">
+        <f>IF(R10&lt;=0, 0, IF(R10&lt;=40,R10-Q10,IF(R10-Q10&lt;=0, 0, ABS(R10-Q10-AH10))))</f>
+        <v/>
+      </c>
+      <c r="AA10">
+        <f>IF(S10&lt;=0, 0, IF(S10&lt;=40,S10-R10,IF(S10-R10&lt;=0, 0, ABS(S10-R10-AI10))))</f>
+        <v/>
+      </c>
+      <c r="AB10">
+        <f>IF(T10&lt;=0, 0, IF(T10&lt;=40,T10-S10,IF(T10-S10&lt;=0, 0, ABS(T10-S10-AJ10))))</f>
+        <v/>
+      </c>
+      <c r="AD10">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE10">
+        <f>IF(O10&lt;=0, 0, IF(O10&lt;=40,0, IF(O10-N10&lt;=0,0,IF(O10&gt;40, O10-40-SUM(AD10:AD10),0))))</f>
+        <v/>
+      </c>
+      <c r="AF10">
+        <f>IF(P10&lt;=0, 0, IF(P10&lt;=40,0, IF(P10-O10&lt;=0,0,IF(P10&gt;40, P10-40-SUM(AD10:AE10),0))))</f>
+        <v/>
+      </c>
+      <c r="AG10">
+        <f>IF(Q10&lt;=0, 0, IF(Q10&lt;=40,0, IF(Q10-P10&lt;=0,0,IF(Q10&gt;40, Q10-40-SUM(AD10:AF10),0))))</f>
+        <v/>
+      </c>
+      <c r="AH10">
+        <f>IF(R10&lt;=0, 0, IF(R10&lt;=40,0, IF(R10-Q10&lt;=0,0,IF(R10&gt;40, R10-40-SUM(AD10:AG10),0))))</f>
+        <v/>
+      </c>
+      <c r="AI10">
+        <f>IF(S10&lt;=0, 0, IF(S10&lt;=40,0, IF(S10-R10&lt;=0,0,IF(S10&gt;40, S10-40-SUM(AD10:AH10),0))))</f>
+        <v/>
+      </c>
+      <c r="AJ10">
+        <f>IF(T10&lt;=0, 0, IF(T10&lt;=40,0, IF(T10-S10&lt;=0,0,IF(T10&gt;40, T10-40-SUM(AD10:AI10),0))))</f>
+        <v/>
+      </c>
+      <c r="AK10" t="inlineStr">
+        <is>
+          <t>ManuelLopez</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -910,6 +1747,95 @@
         <f>I11-J11</f>
         <v/>
       </c>
+      <c r="N11">
+        <f>B11</f>
+        <v/>
+      </c>
+      <c r="O11">
+        <f>C11+N11</f>
+        <v/>
+      </c>
+      <c r="P11">
+        <f>D11+O11</f>
+        <v/>
+      </c>
+      <c r="Q11">
+        <f>E11+P11</f>
+        <v/>
+      </c>
+      <c r="R11">
+        <f>F11+Q11</f>
+        <v/>
+      </c>
+      <c r="S11">
+        <f>G11+R11</f>
+        <v/>
+      </c>
+      <c r="T11">
+        <f>H11+S11</f>
+        <v/>
+      </c>
+      <c r="V11">
+        <f>N11</f>
+        <v/>
+      </c>
+      <c r="W11">
+        <f>IF(O11&lt;=0, 0, IF(O11&lt;=40,O11-N11,IF(O11-N11&lt;=0, 0, ABS(O11-N11-AE11))))</f>
+        <v/>
+      </c>
+      <c r="X11">
+        <f>IF(P11&lt;=0, 0, IF(P11&lt;=40,P11-O11,IF(P11-O11&lt;=0, 0, ABS(P11-O11-AF11))))</f>
+        <v/>
+      </c>
+      <c r="Y11">
+        <f>IF(Q11&lt;=0, 0, IF(Q11&lt;=40,Q11-P11,IF(Q11-P11&lt;=0, 0, ABS(Q11-P11-AG11))))</f>
+        <v/>
+      </c>
+      <c r="Z11">
+        <f>IF(R11&lt;=0, 0, IF(R11&lt;=40,R11-Q11,IF(R11-Q11&lt;=0, 0, ABS(R11-Q11-AH11))))</f>
+        <v/>
+      </c>
+      <c r="AA11">
+        <f>IF(S11&lt;=0, 0, IF(S11&lt;=40,S11-R11,IF(S11-R11&lt;=0, 0, ABS(S11-R11-AI11))))</f>
+        <v/>
+      </c>
+      <c r="AB11">
+        <f>IF(T11&lt;=0, 0, IF(T11&lt;=40,T11-S11,IF(T11-S11&lt;=0, 0, ABS(T11-S11-AJ11))))</f>
+        <v/>
+      </c>
+      <c r="AD11">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE11">
+        <f>IF(O11&lt;=0, 0, IF(O11&lt;=40,0, IF(O11-N11&lt;=0,0,IF(O11&gt;40, O11-40-SUM(AD11:AD11),0))))</f>
+        <v/>
+      </c>
+      <c r="AF11">
+        <f>IF(P11&lt;=0, 0, IF(P11&lt;=40,0, IF(P11-O11&lt;=0,0,IF(P11&gt;40, P11-40-SUM(AD11:AE11),0))))</f>
+        <v/>
+      </c>
+      <c r="AG11">
+        <f>IF(Q11&lt;=0, 0, IF(Q11&lt;=40,0, IF(Q11-P11&lt;=0,0,IF(Q11&gt;40, Q11-40-SUM(AD11:AF11),0))))</f>
+        <v/>
+      </c>
+      <c r="AH11">
+        <f>IF(R11&lt;=0, 0, IF(R11&lt;=40,0, IF(R11-Q11&lt;=0,0,IF(R11&gt;40, R11-40-SUM(AD11:AG11),0))))</f>
+        <v/>
+      </c>
+      <c r="AI11">
+        <f>IF(S11&lt;=0, 0, IF(S11&lt;=40,0, IF(S11-R11&lt;=0,0,IF(S11&gt;40, S11-40-SUM(AD11:AH11),0))))</f>
+        <v/>
+      </c>
+      <c r="AJ11">
+        <f>IF(T11&lt;=0, 0, IF(T11&lt;=40,0, IF(T11-S11&lt;=0,0,IF(T11&gt;40, T11-40-SUM(AD11:AI11),0))))</f>
+        <v/>
+      </c>
+      <c r="AK11" t="inlineStr">
+        <is>
+          <t>SaraOrtiz</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -957,6 +1883,95 @@
         <f>I12-J12</f>
         <v/>
       </c>
+      <c r="N12">
+        <f>B12</f>
+        <v/>
+      </c>
+      <c r="O12">
+        <f>C12+N12</f>
+        <v/>
+      </c>
+      <c r="P12">
+        <f>D12+O12</f>
+        <v/>
+      </c>
+      <c r="Q12">
+        <f>E12+P12</f>
+        <v/>
+      </c>
+      <c r="R12">
+        <f>F12+Q12</f>
+        <v/>
+      </c>
+      <c r="S12">
+        <f>G12+R12</f>
+        <v/>
+      </c>
+      <c r="T12">
+        <f>H12+S12</f>
+        <v/>
+      </c>
+      <c r="V12">
+        <f>N12</f>
+        <v/>
+      </c>
+      <c r="W12">
+        <f>IF(O12&lt;=0, 0, IF(O12&lt;=40,O12-N12,IF(O12-N12&lt;=0, 0, ABS(O12-N12-AE12))))</f>
+        <v/>
+      </c>
+      <c r="X12">
+        <f>IF(P12&lt;=0, 0, IF(P12&lt;=40,P12-O12,IF(P12-O12&lt;=0, 0, ABS(P12-O12-AF12))))</f>
+        <v/>
+      </c>
+      <c r="Y12">
+        <f>IF(Q12&lt;=0, 0, IF(Q12&lt;=40,Q12-P12,IF(Q12-P12&lt;=0, 0, ABS(Q12-P12-AG12))))</f>
+        <v/>
+      </c>
+      <c r="Z12">
+        <f>IF(R12&lt;=0, 0, IF(R12&lt;=40,R12-Q12,IF(R12-Q12&lt;=0, 0, ABS(R12-Q12-AH12))))</f>
+        <v/>
+      </c>
+      <c r="AA12">
+        <f>IF(S12&lt;=0, 0, IF(S12&lt;=40,S12-R12,IF(S12-R12&lt;=0, 0, ABS(S12-R12-AI12))))</f>
+        <v/>
+      </c>
+      <c r="AB12">
+        <f>IF(T12&lt;=0, 0, IF(T12&lt;=40,T12-S12,IF(T12-S12&lt;=0, 0, ABS(T12-S12-AJ12))))</f>
+        <v/>
+      </c>
+      <c r="AD12">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE12">
+        <f>IF(O12&lt;=0, 0, IF(O12&lt;=40,0, IF(O12-N12&lt;=0,0,IF(O12&gt;40, O12-40-SUM(AD12:AD12),0))))</f>
+        <v/>
+      </c>
+      <c r="AF12">
+        <f>IF(P12&lt;=0, 0, IF(P12&lt;=40,0, IF(P12-O12&lt;=0,0,IF(P12&gt;40, P12-40-SUM(AD12:AE12),0))))</f>
+        <v/>
+      </c>
+      <c r="AG12">
+        <f>IF(Q12&lt;=0, 0, IF(Q12&lt;=40,0, IF(Q12-P12&lt;=0,0,IF(Q12&gt;40, Q12-40-SUM(AD12:AF12),0))))</f>
+        <v/>
+      </c>
+      <c r="AH12">
+        <f>IF(R12&lt;=0, 0, IF(R12&lt;=40,0, IF(R12-Q12&lt;=0,0,IF(R12&gt;40, R12-40-SUM(AD12:AG12),0))))</f>
+        <v/>
+      </c>
+      <c r="AI12">
+        <f>IF(S12&lt;=0, 0, IF(S12&lt;=40,0, IF(S12-R12&lt;=0,0,IF(S12&gt;40, S12-40-SUM(AD12:AH12),0))))</f>
+        <v/>
+      </c>
+      <c r="AJ12">
+        <f>IF(T12&lt;=0, 0, IF(T12&lt;=40,0, IF(T12-S12&lt;=0,0,IF(T12&gt;40, T12-40-SUM(AD12:AI12),0))))</f>
+        <v/>
+      </c>
+      <c r="AK12" t="inlineStr">
+        <is>
+          <t>YuniorOrtiz</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1005,6 +2020,90 @@
         <is>
           <t>-</t>
         </is>
+      </c>
+      <c r="N13">
+        <f>SUM(N3:N12)</f>
+        <v/>
+      </c>
+      <c r="O13">
+        <f>SUM(O3:O12)</f>
+        <v/>
+      </c>
+      <c r="P13">
+        <f>SUM(P3:P12)</f>
+        <v/>
+      </c>
+      <c r="Q13">
+        <f>SUM(Q3:Q12)</f>
+        <v/>
+      </c>
+      <c r="R13">
+        <f>SUM(R3:R12)</f>
+        <v/>
+      </c>
+      <c r="S13">
+        <f>SUM(S3:S12)</f>
+        <v/>
+      </c>
+      <c r="T13">
+        <f>SUM(T3:T12)</f>
+        <v/>
+      </c>
+      <c r="V13">
+        <f>SUM(V3:V12)</f>
+        <v/>
+      </c>
+      <c r="W13">
+        <f>SUM(W3:W12)</f>
+        <v/>
+      </c>
+      <c r="X13">
+        <f>SUM(X3:X12)</f>
+        <v/>
+      </c>
+      <c r="Y13">
+        <f>SUM(Y3:Y12)</f>
+        <v/>
+      </c>
+      <c r="Z13">
+        <f>SUM(Z3:Z12)</f>
+        <v/>
+      </c>
+      <c r="AA13">
+        <f>SUM(AA3:AA12)</f>
+        <v/>
+      </c>
+      <c r="AB13">
+        <f>SUM(AB3:AB12)</f>
+        <v/>
+      </c>
+      <c r="AD13">
+        <f>SUM(AD3:AD12)</f>
+        <v/>
+      </c>
+      <c r="AE13">
+        <f>SUM(AE3:AE12)</f>
+        <v/>
+      </c>
+      <c r="AF13">
+        <f>SUM(AF3:AF12)</f>
+        <v/>
+      </c>
+      <c r="AG13">
+        <f>SUM(AG3:AG12)</f>
+        <v/>
+      </c>
+      <c r="AH13">
+        <f>SUM(AH3:AH12)</f>
+        <v/>
+      </c>
+      <c r="AI13">
+        <f>SUM(AI3:AI12)</f>
+        <v/>
+      </c>
+      <c r="AJ13">
+        <f>SUM(AJ3:AJ12)</f>
+        <v/>
       </c>
     </row>
     <row r="14">
@@ -1714,31 +2813,31 @@
         </is>
       </c>
       <c r="B14">
-        <f>SUM(B3:B12)</f>
+        <f>B13-B15</f>
         <v/>
       </c>
       <c r="C14">
-        <f>SUM(C3:C12)</f>
+        <f>C13-C15</f>
         <v/>
       </c>
       <c r="D14">
-        <f>SUM(D3:D12)</f>
+        <f>D13-D15</f>
         <v/>
       </c>
       <c r="E14">
-        <f>SUM(E3:E12)</f>
+        <f>E13-E15</f>
         <v/>
       </c>
       <c r="F14">
-        <f>SUM(F3:F12)</f>
+        <f>F13-F15</f>
         <v/>
       </c>
       <c r="G14">
-        <f>SUM(G3:G12)</f>
+        <f>G13-G15</f>
         <v/>
       </c>
       <c r="H14">
-        <f>SUM(H3:H12)</f>
+        <f>H13-H15</f>
         <v/>
       </c>
       <c r="I14" t="inlineStr">
@@ -1763,31 +2862,31 @@
         </is>
       </c>
       <c r="B15">
-        <f>SUM(B3:B12)</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="C15">
-        <f>SUM(C3:C12)</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="D15">
-        <f>SUM(D3:D12)</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="E15">
-        <f>SUM(E3:E12)</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="F15">
-        <f>SUM(F3:F12)</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="G15">
-        <f>SUM(G3:G12)</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="H15">
-        <f>SUM(H3:H12)</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="I15" t="inlineStr">
@@ -2414,31 +3513,31 @@
         </is>
       </c>
       <c r="B14">
-        <f>SUM(B3:B12)</f>
+        <f>B13-B15</f>
         <v/>
       </c>
       <c r="C14">
-        <f>SUM(C3:C12)</f>
+        <f>C13-C15</f>
         <v/>
       </c>
       <c r="D14">
-        <f>SUM(D3:D12)</f>
+        <f>D13-D15</f>
         <v/>
       </c>
       <c r="E14">
-        <f>SUM(E3:E12)</f>
+        <f>E13-E15</f>
         <v/>
       </c>
       <c r="F14">
-        <f>SUM(F3:F12)</f>
+        <f>F13-F15</f>
         <v/>
       </c>
       <c r="G14">
-        <f>SUM(G3:G12)</f>
+        <f>G13-G15</f>
         <v/>
       </c>
       <c r="H14">
-        <f>SUM(H3:H12)</f>
+        <f>H13-H15</f>
         <v/>
       </c>
       <c r="I14" t="inlineStr">
@@ -2463,31 +3562,31 @@
         </is>
       </c>
       <c r="B15">
-        <f>SUM(B3:B12)</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="C15">
-        <f>SUM(C3:C12)</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="D15">
-        <f>SUM(D3:D12)</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="E15">
-        <f>SUM(E3:E12)</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="F15">
-        <f>SUM(F3:F12)</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="G15">
-        <f>SUM(G3:G12)</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="H15">
-        <f>SUM(H3:H12)</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="I15" t="inlineStr">

</xml_diff>

<commit_message>
Update version - 28/12/2023 ~ 4:00pm
</commit_message>
<xml_diff>
--- a/test_savedata.xlsx
+++ b/test_savedata.xlsx
@@ -2113,31 +2113,31 @@
         </is>
       </c>
       <c r="B14">
-        <f>SUM(B3:B12)</f>
+        <f>V13</f>
         <v/>
       </c>
       <c r="C14">
-        <f>SUM(C3:C12)</f>
+        <f>W13</f>
         <v/>
       </c>
       <c r="D14">
-        <f>SUM(D3:D12)</f>
+        <f>X13</f>
         <v/>
       </c>
       <c r="E14">
-        <f>SUM(E3:E12)</f>
+        <f>Y13</f>
         <v/>
       </c>
       <c r="F14">
-        <f>SUM(F3:F12)</f>
+        <f>Z13</f>
         <v/>
       </c>
       <c r="G14">
-        <f>SUM(G3:G12)</f>
+        <f>AA13</f>
         <v/>
       </c>
       <c r="H14">
-        <f>SUM(H3:H12)</f>
+        <f>AB13</f>
         <v/>
       </c>
       <c r="I14" t="inlineStr">
@@ -2162,31 +2162,31 @@
         </is>
       </c>
       <c r="B15">
-        <f>SUM(B3:B12)</f>
+        <f>AD13</f>
         <v/>
       </c>
       <c r="C15">
-        <f>SUM(C3:C12)</f>
+        <f>AE13</f>
         <v/>
       </c>
       <c r="D15">
-        <f>SUM(D3:D12)</f>
+        <f>AF13</f>
         <v/>
       </c>
       <c r="E15">
-        <f>SUM(E3:E12)</f>
+        <f>AG13</f>
         <v/>
       </c>
       <c r="F15">
-        <f>SUM(F3:F12)</f>
+        <f>AH13</f>
         <v/>
       </c>
       <c r="G15">
-        <f>SUM(G3:G12)</f>
+        <f>AI13</f>
         <v/>
       </c>
       <c r="H15">
-        <f>SUM(H3:H12)</f>
+        <f>AJ13</f>
         <v/>
       </c>
       <c r="I15" t="inlineStr">

</xml_diff>

<commit_message>
Update version - 28/12/2023 ~ 9:06 PM
</commit_message>
<xml_diff>
--- a/test_savedata.xlsx
+++ b/test_savedata.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,16 +27,81 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="24"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="13">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00666666"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ffd966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00b7b7b7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00b6d7a8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00f9cb9c"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00a4c2f4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ea9999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0093c47d"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00f6b26b"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="006d9eeb"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00b4a7d6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -44,12 +109,87 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,1789 +562,2010 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="23" customWidth="1" min="1" max="1"/>
+    <col width="11.86" customWidth="1" min="2" max="2"/>
+    <col width="11.86" customWidth="1" min="3" max="3"/>
+    <col width="11.86" customWidth="1" min="4" max="4"/>
+    <col width="11.86" customWidth="1" min="5" max="5"/>
+    <col width="11.86" customWidth="1" min="6" max="6"/>
+    <col width="11.86" customWidth="1" min="7" max="7"/>
+    <col width="11.86" customWidth="1" min="8" max="8"/>
+    <col width="11.86" customWidth="1" min="9" max="9"/>
+    <col width="11.86" customWidth="1" min="10" max="10"/>
+    <col width="11.86" customWidth="1" min="11" max="11"/>
+    <col width="11.86" customWidth="1" min="12" max="12"/>
+    <col width="11.86" customWidth="1" min="13" max="13"/>
+    <col width="11.86" customWidth="1" min="14" max="14"/>
+    <col width="11.86" customWidth="1" min="15" max="15"/>
+    <col width="11.86" customWidth="1" min="16" max="16"/>
+    <col width="11.86" customWidth="1" min="17" max="17"/>
+    <col width="11.86" customWidth="1" min="18" max="18"/>
+    <col width="11.86" customWidth="1" min="19" max="19"/>
+    <col width="11.86" customWidth="1" min="20" max="20"/>
+    <col width="11.86" customWidth="1" min="21" max="21"/>
+    <col width="11.86" customWidth="1" min="22" max="22"/>
+    <col width="11.86" customWidth="1" min="23" max="23"/>
+    <col width="11.86" customWidth="1" min="24" max="24"/>
+    <col width="11.86" customWidth="1" min="25" max="25"/>
+    <col width="11.86" customWidth="1" min="26" max="26"/>
+    <col width="11.86" customWidth="1" min="27" max="27"/>
+    <col width="11.86" customWidth="1" min="28" max="28"/>
+    <col width="11.86" customWidth="1" min="29" max="29"/>
+    <col width="11.86" customWidth="1" min="30" max="30"/>
+    <col width="11.86" customWidth="1" min="31" max="31"/>
+    <col width="11.86" customWidth="1" min="32" max="32"/>
+    <col width="11.86" customWidth="1" min="33" max="33"/>
+    <col width="11.86" customWidth="1" min="34" max="34"/>
+    <col width="11.86" customWidth="1" min="35" max="35"/>
+    <col width="11.86" customWidth="1" min="36" max="36"/>
+    <col width="23" customWidth="1" min="37" max="37"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Start day of week: Friday 5
- End day of week: Thursday 11</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
+    <row r="1" ht="56.25" customHeight="1">
+      <c r="A1" s="1" t="n"/>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>5th Nov to 11th Nov - Chicago</t>
+        </is>
+      </c>
+      <c r="C1" s="13" t="n"/>
+      <c r="D1" s="13" t="n"/>
+      <c r="E1" s="13" t="n"/>
+      <c r="F1" s="13" t="n"/>
+      <c r="G1" s="13" t="n"/>
+      <c r="H1" s="13" t="n"/>
+      <c r="I1" s="13" t="n"/>
+      <c r="J1" s="13" t="n"/>
+      <c r="K1" s="14" t="n"/>
+      <c r="L1" s="1" t="n"/>
+      <c r="M1" s="3" t="n"/>
+      <c r="N1" s="4" t="inlineStr">
         <is>
           <t>TOTAL HOURS (ACCUMULATED)</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="O1" s="13" t="n"/>
+      <c r="P1" s="13" t="n"/>
+      <c r="Q1" s="13" t="n"/>
+      <c r="R1" s="13" t="n"/>
+      <c r="S1" s="13" t="n"/>
+      <c r="T1" s="14" t="n"/>
+      <c r="U1" s="3" t="n"/>
+      <c r="V1" s="4" t="inlineStr">
         <is>
           <t>REGULAR HOURS</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="W1" s="13" t="n"/>
+      <c r="X1" s="13" t="n"/>
+      <c r="Y1" s="13" t="n"/>
+      <c r="Z1" s="13" t="n"/>
+      <c r="AA1" s="13" t="n"/>
+      <c r="AB1" s="14" t="n"/>
+      <c r="AC1" s="3" t="n"/>
+      <c r="AD1" s="4" t="inlineStr">
         <is>
           <t>OVERTIME HOURS (PER DAY)</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="AE1" s="13" t="n"/>
+      <c r="AF1" s="13" t="n"/>
+      <c r="AG1" s="13" t="n"/>
+      <c r="AH1" s="13" t="n"/>
+      <c r="AI1" s="13" t="n"/>
+      <c r="AJ1" s="14" t="n"/>
+      <c r="AK1" s="3" t="n"/>
+    </row>
+    <row r="2" ht="56.25" customHeight="1">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>NAMES</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr">
         <is>
           <t>Friday 5</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="4" t="inlineStr">
         <is>
           <t>Saturday 6</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="4" t="inlineStr">
         <is>
           <t>Sunday 7</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="4" t="inlineStr">
         <is>
           <t>Monday 8</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="4" t="inlineStr">
         <is>
           <t>Tuesday 9</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="4" t="inlineStr">
         <is>
           <t>Wednesday 10</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" s="4" t="inlineStr">
         <is>
           <t>Thursday 11</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" s="5" t="inlineStr">
         <is>
           <t>TOTAL HOURS - WEEKLY</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" s="6" t="inlineStr">
         <is>
           <t>TOTAL REGULAR HOURS - WEEKLY</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K2" s="7" t="inlineStr">
         <is>
           <t>TOTAL OVERTIME HOURS - WEEKLY</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="L2" s="8" t="inlineStr">
+        <is>
+          <t>PAGOS</t>
+        </is>
+      </c>
+      <c r="M2" s="3" t="n"/>
+      <c r="N2" s="4" t="inlineStr">
         <is>
           <t>Friday 5</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="O2" s="4" t="inlineStr">
         <is>
           <t>Saturday 6</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="P2" s="4" t="inlineStr">
         <is>
           <t>Sunday 7</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="Q2" s="4" t="inlineStr">
         <is>
           <t>Monday 8</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="R2" s="4" t="inlineStr">
         <is>
           <t>Tuesday 9</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="S2" s="4" t="inlineStr">
         <is>
           <t>Wednesday 10</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="T2" s="4" t="inlineStr">
         <is>
           <t>Thursday 11</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="U2" s="3" t="n"/>
+      <c r="V2" s="4" t="inlineStr">
         <is>
           <t>Friday 5</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
+      <c r="W2" s="4" t="inlineStr">
         <is>
           <t>Saturday 6</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr">
+      <c r="X2" s="4" t="inlineStr">
         <is>
           <t>Sunday 7</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
+      <c r="Y2" s="4" t="inlineStr">
         <is>
           <t>Monday 8</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
+      <c r="Z2" s="4" t="inlineStr">
         <is>
           <t>Tuesday 9</t>
         </is>
       </c>
-      <c r="AA2" t="inlineStr">
+      <c r="AA2" s="4" t="inlineStr">
         <is>
           <t>Wednesday 10</t>
         </is>
       </c>
-      <c r="AB2" t="inlineStr">
+      <c r="AB2" s="4" t="inlineStr">
         <is>
           <t>Thursday 11</t>
         </is>
       </c>
-      <c r="AD2" t="inlineStr">
+      <c r="AC2" s="3" t="n"/>
+      <c r="AD2" s="4" t="inlineStr">
         <is>
           <t>Friday 5</t>
         </is>
       </c>
-      <c r="AE2" t="inlineStr">
+      <c r="AE2" s="4" t="inlineStr">
         <is>
           <t>Saturday 6</t>
         </is>
       </c>
-      <c r="AF2" t="inlineStr">
+      <c r="AF2" s="4" t="inlineStr">
         <is>
           <t>Sunday 7</t>
         </is>
       </c>
-      <c r="AG2" t="inlineStr">
+      <c r="AG2" s="4" t="inlineStr">
         <is>
           <t>Monday 8</t>
         </is>
       </c>
-      <c r="AH2" t="inlineStr">
+      <c r="AH2" s="4" t="inlineStr">
         <is>
           <t>Tuesday 9</t>
         </is>
       </c>
-      <c r="AI2" t="inlineStr">
+      <c r="AI2" s="4" t="inlineStr">
         <is>
           <t>Wednesday 10</t>
         </is>
       </c>
-      <c r="AJ2" t="inlineStr">
+      <c r="AJ2" s="4" t="inlineStr">
         <is>
           <t>Thursday 11</t>
         </is>
       </c>
-      <c r="AK2" t="inlineStr">
+      <c r="AK2" s="4" t="inlineStr">
         <is>
           <t>NAMES</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="9" t="inlineStr">
         <is>
           <t>ClaudiaGil</t>
         </is>
       </c>
-      <c r="B3">
+      <c r="B3" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!B3)</f>
         <v/>
       </c>
-      <c r="C3">
+      <c r="C3" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!C3)</f>
         <v/>
       </c>
-      <c r="D3">
+      <c r="D3" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!D3)</f>
         <v/>
       </c>
-      <c r="E3">
+      <c r="E3" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!E3)</f>
         <v/>
       </c>
-      <c r="F3">
+      <c r="F3" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!F3)</f>
         <v/>
       </c>
-      <c r="G3">
+      <c r="G3" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!G3)</f>
         <v/>
       </c>
-      <c r="H3">
+      <c r="H3" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!H3)</f>
         <v/>
       </c>
-      <c r="I3">
+      <c r="I3" s="5">
         <f>SUM(B3:H3)</f>
         <v/>
       </c>
-      <c r="J3">
+      <c r="J3" s="6">
         <f>IF(I3&lt;=40,I3,40)</f>
         <v/>
       </c>
-      <c r="K3">
+      <c r="K3" s="7">
         <f>I3-J3</f>
         <v/>
       </c>
-      <c r="N3">
+      <c r="L3" s="8">
+        <f>I3*15</f>
+        <v/>
+      </c>
+      <c r="M3" s="3" t="n"/>
+      <c r="N3" s="5">
         <f>B3</f>
         <v/>
       </c>
-      <c r="O3">
+      <c r="O3" s="5">
         <f>C3+N3</f>
         <v/>
       </c>
-      <c r="P3">
+      <c r="P3" s="5">
         <f>D3+O3</f>
         <v/>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="5">
         <f>E3+P3</f>
         <v/>
       </c>
-      <c r="R3">
+      <c r="R3" s="5">
         <f>F3+Q3</f>
         <v/>
       </c>
-      <c r="S3">
+      <c r="S3" s="5">
         <f>G3+R3</f>
         <v/>
       </c>
-      <c r="T3">
+      <c r="T3" s="5">
         <f>H3+S3</f>
         <v/>
       </c>
-      <c r="V3">
+      <c r="U3" s="3" t="n"/>
+      <c r="V3" s="6">
         <f>N3</f>
         <v/>
       </c>
-      <c r="W3">
+      <c r="W3" s="6">
         <f>IF(O3&lt;=0, 0, IF(O3&lt;=40,O3-N3,IF(O3-N3&lt;=0, 0, ABS(O3-N3-AE3))))</f>
         <v/>
       </c>
-      <c r="X3">
+      <c r="X3" s="6">
         <f>IF(P3&lt;=0, 0, IF(P3&lt;=40,P3-O3,IF(P3-O3&lt;=0, 0, ABS(P3-O3-AF3))))</f>
         <v/>
       </c>
-      <c r="Y3">
+      <c r="Y3" s="6">
         <f>IF(Q3&lt;=0, 0, IF(Q3&lt;=40,Q3-P3,IF(Q3-P3&lt;=0, 0, ABS(Q3-P3-AG3))))</f>
         <v/>
       </c>
-      <c r="Z3">
+      <c r="Z3" s="6">
         <f>IF(R3&lt;=0, 0, IF(R3&lt;=40,R3-Q3,IF(R3-Q3&lt;=0, 0, ABS(R3-Q3-AH3))))</f>
         <v/>
       </c>
-      <c r="AA3">
+      <c r="AA3" s="6">
         <f>IF(S3&lt;=0, 0, IF(S3&lt;=40,S3-R3,IF(S3-R3&lt;=0, 0, ABS(S3-R3-AI3))))</f>
         <v/>
       </c>
-      <c r="AB3">
+      <c r="AB3" s="6">
         <f>IF(T3&lt;=0, 0, IF(T3&lt;=40,T3-S3,IF(T3-S3&lt;=0, 0, ABS(T3-S3-AJ3))))</f>
         <v/>
       </c>
-      <c r="AD3">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="AE3">
+      <c r="AC3" s="3" t="n"/>
+      <c r="AD3" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE3" s="7">
         <f>IF(O3&lt;=0, 0, IF(O3&lt;=40,0, IF(O3-N3&lt;=0,0,IF(O3&gt;40, O3-40-SUM(AD3:AD3),0))))</f>
         <v/>
       </c>
-      <c r="AF3">
+      <c r="AF3" s="7">
         <f>IF(P3&lt;=0, 0, IF(P3&lt;=40,0, IF(P3-O3&lt;=0,0,IF(P3&gt;40, P3-40-SUM(AD3:AE3),0))))</f>
         <v/>
       </c>
-      <c r="AG3">
+      <c r="AG3" s="7">
         <f>IF(Q3&lt;=0, 0, IF(Q3&lt;=40,0, IF(Q3-P3&lt;=0,0,IF(Q3&gt;40, Q3-40-SUM(AD3:AF3),0))))</f>
         <v/>
       </c>
-      <c r="AH3">
+      <c r="AH3" s="7">
         <f>IF(R3&lt;=0, 0, IF(R3&lt;=40,0, IF(R3-Q3&lt;=0,0,IF(R3&gt;40, R3-40-SUM(AD3:AG3),0))))</f>
         <v/>
       </c>
-      <c r="AI3">
+      <c r="AI3" s="7">
         <f>IF(S3&lt;=0, 0, IF(S3&lt;=40,0, IF(S3-R3&lt;=0,0,IF(S3&gt;40, S3-40-SUM(AD3:AH3),0))))</f>
         <v/>
       </c>
-      <c r="AJ3">
+      <c r="AJ3" s="7">
         <f>IF(T3&lt;=0, 0, IF(T3&lt;=40,0, IF(T3-S3&lt;=0,0,IF(T3&gt;40, T3-40-SUM(AD3:AI3),0))))</f>
         <v/>
       </c>
-      <c r="AK3" t="inlineStr">
+      <c r="AK3" s="9" t="inlineStr">
         <is>
           <t>ClaudiaGil</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="9" t="inlineStr">
         <is>
           <t>Darwinparedes</t>
         </is>
       </c>
-      <c r="B4">
+      <c r="B4" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!B4)</f>
         <v/>
       </c>
-      <c r="C4">
+      <c r="C4" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!C4)</f>
         <v/>
       </c>
-      <c r="D4">
+      <c r="D4" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!D4)</f>
         <v/>
       </c>
-      <c r="E4">
+      <c r="E4" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!E4)</f>
         <v/>
       </c>
-      <c r="F4">
+      <c r="F4" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!F4)</f>
         <v/>
       </c>
-      <c r="G4">
+      <c r="G4" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!G4)</f>
         <v/>
       </c>
-      <c r="H4">
+      <c r="H4" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!H4)</f>
         <v/>
       </c>
-      <c r="I4">
+      <c r="I4" s="5">
         <f>SUM(B4:H4)</f>
         <v/>
       </c>
-      <c r="J4">
+      <c r="J4" s="6">
         <f>IF(I4&lt;=40,I4,40)</f>
         <v/>
       </c>
-      <c r="K4">
+      <c r="K4" s="7">
         <f>I4-J4</f>
         <v/>
       </c>
-      <c r="N4">
+      <c r="L4" s="8">
+        <f>I4*15</f>
+        <v/>
+      </c>
+      <c r="M4" s="3" t="n"/>
+      <c r="N4" s="5">
         <f>B4</f>
         <v/>
       </c>
-      <c r="O4">
+      <c r="O4" s="5">
         <f>C4+N4</f>
         <v/>
       </c>
-      <c r="P4">
+      <c r="P4" s="5">
         <f>D4+O4</f>
         <v/>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="5">
         <f>E4+P4</f>
         <v/>
       </c>
-      <c r="R4">
+      <c r="R4" s="5">
         <f>F4+Q4</f>
         <v/>
       </c>
-      <c r="S4">
+      <c r="S4" s="5">
         <f>G4+R4</f>
         <v/>
       </c>
-      <c r="T4">
+      <c r="T4" s="5">
         <f>H4+S4</f>
         <v/>
       </c>
-      <c r="V4">
+      <c r="U4" s="3" t="n"/>
+      <c r="V4" s="6">
         <f>N4</f>
         <v/>
       </c>
-      <c r="W4">
+      <c r="W4" s="6">
         <f>IF(O4&lt;=0, 0, IF(O4&lt;=40,O4-N4,IF(O4-N4&lt;=0, 0, ABS(O4-N4-AE4))))</f>
         <v/>
       </c>
-      <c r="X4">
+      <c r="X4" s="6">
         <f>IF(P4&lt;=0, 0, IF(P4&lt;=40,P4-O4,IF(P4-O4&lt;=0, 0, ABS(P4-O4-AF4))))</f>
         <v/>
       </c>
-      <c r="Y4">
+      <c r="Y4" s="6">
         <f>IF(Q4&lt;=0, 0, IF(Q4&lt;=40,Q4-P4,IF(Q4-P4&lt;=0, 0, ABS(Q4-P4-AG4))))</f>
         <v/>
       </c>
-      <c r="Z4">
+      <c r="Z4" s="6">
         <f>IF(R4&lt;=0, 0, IF(R4&lt;=40,R4-Q4,IF(R4-Q4&lt;=0, 0, ABS(R4-Q4-AH4))))</f>
         <v/>
       </c>
-      <c r="AA4">
+      <c r="AA4" s="6">
         <f>IF(S4&lt;=0, 0, IF(S4&lt;=40,S4-R4,IF(S4-R4&lt;=0, 0, ABS(S4-R4-AI4))))</f>
         <v/>
       </c>
-      <c r="AB4">
+      <c r="AB4" s="6">
         <f>IF(T4&lt;=0, 0, IF(T4&lt;=40,T4-S4,IF(T4-S4&lt;=0, 0, ABS(T4-S4-AJ4))))</f>
         <v/>
       </c>
-      <c r="AD4">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="AE4">
+      <c r="AC4" s="3" t="n"/>
+      <c r="AD4" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE4" s="7">
         <f>IF(O4&lt;=0, 0, IF(O4&lt;=40,0, IF(O4-N4&lt;=0,0,IF(O4&gt;40, O4-40-SUM(AD4:AD4),0))))</f>
         <v/>
       </c>
-      <c r="AF4">
+      <c r="AF4" s="7">
         <f>IF(P4&lt;=0, 0, IF(P4&lt;=40,0, IF(P4-O4&lt;=0,0,IF(P4&gt;40, P4-40-SUM(AD4:AE4),0))))</f>
         <v/>
       </c>
-      <c r="AG4">
+      <c r="AG4" s="7">
         <f>IF(Q4&lt;=0, 0, IF(Q4&lt;=40,0, IF(Q4-P4&lt;=0,0,IF(Q4&gt;40, Q4-40-SUM(AD4:AF4),0))))</f>
         <v/>
       </c>
-      <c r="AH4">
+      <c r="AH4" s="7">
         <f>IF(R4&lt;=0, 0, IF(R4&lt;=40,0, IF(R4-Q4&lt;=0,0,IF(R4&gt;40, R4-40-SUM(AD4:AG4),0))))</f>
         <v/>
       </c>
-      <c r="AI4">
+      <c r="AI4" s="7">
         <f>IF(S4&lt;=0, 0, IF(S4&lt;=40,0, IF(S4-R4&lt;=0,0,IF(S4&gt;40, S4-40-SUM(AD4:AH4),0))))</f>
         <v/>
       </c>
-      <c r="AJ4">
+      <c r="AJ4" s="7">
         <f>IF(T4&lt;=0, 0, IF(T4&lt;=40,0, IF(T4-S4&lt;=0,0,IF(T4&gt;40, T4-40-SUM(AD4:AI4),0))))</f>
         <v/>
       </c>
-      <c r="AK4" t="inlineStr">
+      <c r="AK4" s="9" t="inlineStr">
         <is>
           <t>Darwinparedes</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="9" t="inlineStr">
         <is>
           <t>EdgarCamacho</t>
         </is>
       </c>
-      <c r="B5">
+      <c r="B5" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!B5)</f>
         <v/>
       </c>
-      <c r="C5">
+      <c r="C5" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!C5)</f>
         <v/>
       </c>
-      <c r="D5">
+      <c r="D5" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!D5)</f>
         <v/>
       </c>
-      <c r="E5">
+      <c r="E5" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!E5)</f>
         <v/>
       </c>
-      <c r="F5">
+      <c r="F5" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!F5)</f>
         <v/>
       </c>
-      <c r="G5">
+      <c r="G5" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!G5)</f>
         <v/>
       </c>
-      <c r="H5">
+      <c r="H5" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!H5)</f>
         <v/>
       </c>
-      <c r="I5">
+      <c r="I5" s="5">
         <f>SUM(B5:H5)</f>
         <v/>
       </c>
-      <c r="J5">
+      <c r="J5" s="6">
         <f>IF(I5&lt;=40,I5,40)</f>
         <v/>
       </c>
-      <c r="K5">
+      <c r="K5" s="7">
         <f>I5-J5</f>
         <v/>
       </c>
-      <c r="N5">
+      <c r="L5" s="8">
+        <f>I5*15</f>
+        <v/>
+      </c>
+      <c r="M5" s="3" t="n"/>
+      <c r="N5" s="5">
         <f>B5</f>
         <v/>
       </c>
-      <c r="O5">
+      <c r="O5" s="5">
         <f>C5+N5</f>
         <v/>
       </c>
-      <c r="P5">
+      <c r="P5" s="5">
         <f>D5+O5</f>
         <v/>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="5">
         <f>E5+P5</f>
         <v/>
       </c>
-      <c r="R5">
+      <c r="R5" s="5">
         <f>F5+Q5</f>
         <v/>
       </c>
-      <c r="S5">
+      <c r="S5" s="5">
         <f>G5+R5</f>
         <v/>
       </c>
-      <c r="T5">
+      <c r="T5" s="5">
         <f>H5+S5</f>
         <v/>
       </c>
-      <c r="V5">
+      <c r="U5" s="3" t="n"/>
+      <c r="V5" s="6">
         <f>N5</f>
         <v/>
       </c>
-      <c r="W5">
+      <c r="W5" s="6">
         <f>IF(O5&lt;=0, 0, IF(O5&lt;=40,O5-N5,IF(O5-N5&lt;=0, 0, ABS(O5-N5-AE5))))</f>
         <v/>
       </c>
-      <c r="X5">
+      <c r="X5" s="6">
         <f>IF(P5&lt;=0, 0, IF(P5&lt;=40,P5-O5,IF(P5-O5&lt;=0, 0, ABS(P5-O5-AF5))))</f>
         <v/>
       </c>
-      <c r="Y5">
+      <c r="Y5" s="6">
         <f>IF(Q5&lt;=0, 0, IF(Q5&lt;=40,Q5-P5,IF(Q5-P5&lt;=0, 0, ABS(Q5-P5-AG5))))</f>
         <v/>
       </c>
-      <c r="Z5">
+      <c r="Z5" s="6">
         <f>IF(R5&lt;=0, 0, IF(R5&lt;=40,R5-Q5,IF(R5-Q5&lt;=0, 0, ABS(R5-Q5-AH5))))</f>
         <v/>
       </c>
-      <c r="AA5">
+      <c r="AA5" s="6">
         <f>IF(S5&lt;=0, 0, IF(S5&lt;=40,S5-R5,IF(S5-R5&lt;=0, 0, ABS(S5-R5-AI5))))</f>
         <v/>
       </c>
-      <c r="AB5">
+      <c r="AB5" s="6">
         <f>IF(T5&lt;=0, 0, IF(T5&lt;=40,T5-S5,IF(T5-S5&lt;=0, 0, ABS(T5-S5-AJ5))))</f>
         <v/>
       </c>
-      <c r="AD5">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="AE5">
+      <c r="AC5" s="3" t="n"/>
+      <c r="AD5" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE5" s="7">
         <f>IF(O5&lt;=0, 0, IF(O5&lt;=40,0, IF(O5-N5&lt;=0,0,IF(O5&gt;40, O5-40-SUM(AD5:AD5),0))))</f>
         <v/>
       </c>
-      <c r="AF5">
+      <c r="AF5" s="7">
         <f>IF(P5&lt;=0, 0, IF(P5&lt;=40,0, IF(P5-O5&lt;=0,0,IF(P5&gt;40, P5-40-SUM(AD5:AE5),0))))</f>
         <v/>
       </c>
-      <c r="AG5">
+      <c r="AG5" s="7">
         <f>IF(Q5&lt;=0, 0, IF(Q5&lt;=40,0, IF(Q5-P5&lt;=0,0,IF(Q5&gt;40, Q5-40-SUM(AD5:AF5),0))))</f>
         <v/>
       </c>
-      <c r="AH5">
+      <c r="AH5" s="7">
         <f>IF(R5&lt;=0, 0, IF(R5&lt;=40,0, IF(R5-Q5&lt;=0,0,IF(R5&gt;40, R5-40-SUM(AD5:AG5),0))))</f>
         <v/>
       </c>
-      <c r="AI5">
+      <c r="AI5" s="7">
         <f>IF(S5&lt;=0, 0, IF(S5&lt;=40,0, IF(S5-R5&lt;=0,0,IF(S5&gt;40, S5-40-SUM(AD5:AH5),0))))</f>
         <v/>
       </c>
-      <c r="AJ5">
+      <c r="AJ5" s="7">
         <f>IF(T5&lt;=0, 0, IF(T5&lt;=40,0, IF(T5-S5&lt;=0,0,IF(T5&gt;40, T5-40-SUM(AD5:AI5),0))))</f>
         <v/>
       </c>
-      <c r="AK5" t="inlineStr">
+      <c r="AK5" s="9" t="inlineStr">
         <is>
           <t>EdgarCamacho</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="9" t="inlineStr">
         <is>
           <t>EduardodeSouza</t>
         </is>
       </c>
-      <c r="B6">
+      <c r="B6" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!B6)</f>
         <v/>
       </c>
-      <c r="C6">
+      <c r="C6" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!C6)</f>
         <v/>
       </c>
-      <c r="D6">
+      <c r="D6" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!D6)</f>
         <v/>
       </c>
-      <c r="E6">
+      <c r="E6" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!E6)</f>
         <v/>
       </c>
-      <c r="F6">
+      <c r="F6" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!F6)</f>
         <v/>
       </c>
-      <c r="G6">
+      <c r="G6" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!G6)</f>
         <v/>
       </c>
-      <c r="H6">
+      <c r="H6" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!H6)</f>
         <v/>
       </c>
-      <c r="I6">
+      <c r="I6" s="5">
         <f>SUM(B6:H6)</f>
         <v/>
       </c>
-      <c r="J6">
+      <c r="J6" s="6">
         <f>IF(I6&lt;=40,I6,40)</f>
         <v/>
       </c>
-      <c r="K6">
+      <c r="K6" s="7">
         <f>I6-J6</f>
         <v/>
       </c>
-      <c r="N6">
+      <c r="L6" s="8">
+        <f>I6*15</f>
+        <v/>
+      </c>
+      <c r="M6" s="3" t="n"/>
+      <c r="N6" s="5">
         <f>B6</f>
         <v/>
       </c>
-      <c r="O6">
+      <c r="O6" s="5">
         <f>C6+N6</f>
         <v/>
       </c>
-      <c r="P6">
+      <c r="P6" s="5">
         <f>D6+O6</f>
         <v/>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="5">
         <f>E6+P6</f>
         <v/>
       </c>
-      <c r="R6">
+      <c r="R6" s="5">
         <f>F6+Q6</f>
         <v/>
       </c>
-      <c r="S6">
+      <c r="S6" s="5">
         <f>G6+R6</f>
         <v/>
       </c>
-      <c r="T6">
+      <c r="T6" s="5">
         <f>H6+S6</f>
         <v/>
       </c>
-      <c r="V6">
+      <c r="U6" s="3" t="n"/>
+      <c r="V6" s="6">
         <f>N6</f>
         <v/>
       </c>
-      <c r="W6">
+      <c r="W6" s="6">
         <f>IF(O6&lt;=0, 0, IF(O6&lt;=40,O6-N6,IF(O6-N6&lt;=0, 0, ABS(O6-N6-AE6))))</f>
         <v/>
       </c>
-      <c r="X6">
+      <c r="X6" s="6">
         <f>IF(P6&lt;=0, 0, IF(P6&lt;=40,P6-O6,IF(P6-O6&lt;=0, 0, ABS(P6-O6-AF6))))</f>
         <v/>
       </c>
-      <c r="Y6">
+      <c r="Y6" s="6">
         <f>IF(Q6&lt;=0, 0, IF(Q6&lt;=40,Q6-P6,IF(Q6-P6&lt;=0, 0, ABS(Q6-P6-AG6))))</f>
         <v/>
       </c>
-      <c r="Z6">
+      <c r="Z6" s="6">
         <f>IF(R6&lt;=0, 0, IF(R6&lt;=40,R6-Q6,IF(R6-Q6&lt;=0, 0, ABS(R6-Q6-AH6))))</f>
         <v/>
       </c>
-      <c r="AA6">
+      <c r="AA6" s="6">
         <f>IF(S6&lt;=0, 0, IF(S6&lt;=40,S6-R6,IF(S6-R6&lt;=0, 0, ABS(S6-R6-AI6))))</f>
         <v/>
       </c>
-      <c r="AB6">
+      <c r="AB6" s="6">
         <f>IF(T6&lt;=0, 0, IF(T6&lt;=40,T6-S6,IF(T6-S6&lt;=0, 0, ABS(T6-S6-AJ6))))</f>
         <v/>
       </c>
-      <c r="AD6">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="AE6">
+      <c r="AC6" s="3" t="n"/>
+      <c r="AD6" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE6" s="7">
         <f>IF(O6&lt;=0, 0, IF(O6&lt;=40,0, IF(O6-N6&lt;=0,0,IF(O6&gt;40, O6-40-SUM(AD6:AD6),0))))</f>
         <v/>
       </c>
-      <c r="AF6">
+      <c r="AF6" s="7">
         <f>IF(P6&lt;=0, 0, IF(P6&lt;=40,0, IF(P6-O6&lt;=0,0,IF(P6&gt;40, P6-40-SUM(AD6:AE6),0))))</f>
         <v/>
       </c>
-      <c r="AG6">
+      <c r="AG6" s="7">
         <f>IF(Q6&lt;=0, 0, IF(Q6&lt;=40,0, IF(Q6-P6&lt;=0,0,IF(Q6&gt;40, Q6-40-SUM(AD6:AF6),0))))</f>
         <v/>
       </c>
-      <c r="AH6">
+      <c r="AH6" s="7">
         <f>IF(R6&lt;=0, 0, IF(R6&lt;=40,0, IF(R6-Q6&lt;=0,0,IF(R6&gt;40, R6-40-SUM(AD6:AG6),0))))</f>
         <v/>
       </c>
-      <c r="AI6">
+      <c r="AI6" s="7">
         <f>IF(S6&lt;=0, 0, IF(S6&lt;=40,0, IF(S6-R6&lt;=0,0,IF(S6&gt;40, S6-40-SUM(AD6:AH6),0))))</f>
         <v/>
       </c>
-      <c r="AJ6">
+      <c r="AJ6" s="7">
         <f>IF(T6&lt;=0, 0, IF(T6&lt;=40,0, IF(T6-S6&lt;=0,0,IF(T6&gt;40, T6-40-SUM(AD6:AI6),0))))</f>
         <v/>
       </c>
-      <c r="AK6" t="inlineStr">
+      <c r="AK6" s="9" t="inlineStr">
         <is>
           <t>EduardodeSouza</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="9" t="inlineStr">
         <is>
           <t>Eliasalbornoz</t>
         </is>
       </c>
-      <c r="B7">
+      <c r="B7" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!B7)</f>
         <v/>
       </c>
-      <c r="C7">
+      <c r="C7" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!C7)</f>
         <v/>
       </c>
-      <c r="D7">
+      <c r="D7" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!D7)</f>
         <v/>
       </c>
-      <c r="E7">
+      <c r="E7" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!E7)</f>
         <v/>
       </c>
-      <c r="F7">
+      <c r="F7" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!F7)</f>
         <v/>
       </c>
-      <c r="G7">
+      <c r="G7" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!G7)</f>
         <v/>
       </c>
-      <c r="H7">
+      <c r="H7" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!H7)</f>
         <v/>
       </c>
-      <c r="I7">
+      <c r="I7" s="5">
         <f>SUM(B7:H7)</f>
         <v/>
       </c>
-      <c r="J7">
+      <c r="J7" s="6">
         <f>IF(I7&lt;=40,I7,40)</f>
         <v/>
       </c>
-      <c r="K7">
+      <c r="K7" s="7">
         <f>I7-J7</f>
         <v/>
       </c>
-      <c r="N7">
+      <c r="L7" s="8">
+        <f>I7*15</f>
+        <v/>
+      </c>
+      <c r="M7" s="3" t="n"/>
+      <c r="N7" s="5">
         <f>B7</f>
         <v/>
       </c>
-      <c r="O7">
+      <c r="O7" s="5">
         <f>C7+N7</f>
         <v/>
       </c>
-      <c r="P7">
+      <c r="P7" s="5">
         <f>D7+O7</f>
         <v/>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="5">
         <f>E7+P7</f>
         <v/>
       </c>
-      <c r="R7">
+      <c r="R7" s="5">
         <f>F7+Q7</f>
         <v/>
       </c>
-      <c r="S7">
+      <c r="S7" s="5">
         <f>G7+R7</f>
         <v/>
       </c>
-      <c r="T7">
+      <c r="T7" s="5">
         <f>H7+S7</f>
         <v/>
       </c>
-      <c r="V7">
+      <c r="U7" s="3" t="n"/>
+      <c r="V7" s="6">
         <f>N7</f>
         <v/>
       </c>
-      <c r="W7">
+      <c r="W7" s="6">
         <f>IF(O7&lt;=0, 0, IF(O7&lt;=40,O7-N7,IF(O7-N7&lt;=0, 0, ABS(O7-N7-AE7))))</f>
         <v/>
       </c>
-      <c r="X7">
+      <c r="X7" s="6">
         <f>IF(P7&lt;=0, 0, IF(P7&lt;=40,P7-O7,IF(P7-O7&lt;=0, 0, ABS(P7-O7-AF7))))</f>
         <v/>
       </c>
-      <c r="Y7">
+      <c r="Y7" s="6">
         <f>IF(Q7&lt;=0, 0, IF(Q7&lt;=40,Q7-P7,IF(Q7-P7&lt;=0, 0, ABS(Q7-P7-AG7))))</f>
         <v/>
       </c>
-      <c r="Z7">
+      <c r="Z7" s="6">
         <f>IF(R7&lt;=0, 0, IF(R7&lt;=40,R7-Q7,IF(R7-Q7&lt;=0, 0, ABS(R7-Q7-AH7))))</f>
         <v/>
       </c>
-      <c r="AA7">
+      <c r="AA7" s="6">
         <f>IF(S7&lt;=0, 0, IF(S7&lt;=40,S7-R7,IF(S7-R7&lt;=0, 0, ABS(S7-R7-AI7))))</f>
         <v/>
       </c>
-      <c r="AB7">
+      <c r="AB7" s="6">
         <f>IF(T7&lt;=0, 0, IF(T7&lt;=40,T7-S7,IF(T7-S7&lt;=0, 0, ABS(T7-S7-AJ7))))</f>
         <v/>
       </c>
-      <c r="AD7">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="AE7">
+      <c r="AC7" s="3" t="n"/>
+      <c r="AD7" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE7" s="7">
         <f>IF(O7&lt;=0, 0, IF(O7&lt;=40,0, IF(O7-N7&lt;=0,0,IF(O7&gt;40, O7-40-SUM(AD7:AD7),0))))</f>
         <v/>
       </c>
-      <c r="AF7">
+      <c r="AF7" s="7">
         <f>IF(P7&lt;=0, 0, IF(P7&lt;=40,0, IF(P7-O7&lt;=0,0,IF(P7&gt;40, P7-40-SUM(AD7:AE7),0))))</f>
         <v/>
       </c>
-      <c r="AG7">
+      <c r="AG7" s="7">
         <f>IF(Q7&lt;=0, 0, IF(Q7&lt;=40,0, IF(Q7-P7&lt;=0,0,IF(Q7&gt;40, Q7-40-SUM(AD7:AF7),0))))</f>
         <v/>
       </c>
-      <c r="AH7">
+      <c r="AH7" s="7">
         <f>IF(R7&lt;=0, 0, IF(R7&lt;=40,0, IF(R7-Q7&lt;=0,0,IF(R7&gt;40, R7-40-SUM(AD7:AG7),0))))</f>
         <v/>
       </c>
-      <c r="AI7">
+      <c r="AI7" s="7">
         <f>IF(S7&lt;=0, 0, IF(S7&lt;=40,0, IF(S7-R7&lt;=0,0,IF(S7&gt;40, S7-40-SUM(AD7:AH7),0))))</f>
         <v/>
       </c>
-      <c r="AJ7">
+      <c r="AJ7" s="7">
         <f>IF(T7&lt;=0, 0, IF(T7&lt;=40,0, IF(T7-S7&lt;=0,0,IF(T7&gt;40, T7-40-SUM(AD7:AI7),0))))</f>
         <v/>
       </c>
-      <c r="AK7" t="inlineStr">
+      <c r="AK7" s="9" t="inlineStr">
         <is>
           <t>Eliasalbornoz</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="9" t="inlineStr">
         <is>
           <t>GermanCastro</t>
         </is>
       </c>
-      <c r="B8">
+      <c r="B8" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!B8)</f>
         <v/>
       </c>
-      <c r="C8">
+      <c r="C8" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!C8)</f>
         <v/>
       </c>
-      <c r="D8">
+      <c r="D8" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!D8)</f>
         <v/>
       </c>
-      <c r="E8">
+      <c r="E8" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!E8)</f>
         <v/>
       </c>
-      <c r="F8">
+      <c r="F8" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!F8)</f>
         <v/>
       </c>
-      <c r="G8">
+      <c r="G8" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!G8)</f>
         <v/>
       </c>
-      <c r="H8">
+      <c r="H8" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!H8)</f>
         <v/>
       </c>
-      <c r="I8">
+      <c r="I8" s="5">
         <f>SUM(B8:H8)</f>
         <v/>
       </c>
-      <c r="J8">
+      <c r="J8" s="6">
         <f>IF(I8&lt;=40,I8,40)</f>
         <v/>
       </c>
-      <c r="K8">
+      <c r="K8" s="7">
         <f>I8-J8</f>
         <v/>
       </c>
-      <c r="N8">
+      <c r="L8" s="8">
+        <f>I8*15</f>
+        <v/>
+      </c>
+      <c r="M8" s="3" t="n"/>
+      <c r="N8" s="5">
         <f>B8</f>
         <v/>
       </c>
-      <c r="O8">
+      <c r="O8" s="5">
         <f>C8+N8</f>
         <v/>
       </c>
-      <c r="P8">
+      <c r="P8" s="5">
         <f>D8+O8</f>
         <v/>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="5">
         <f>E8+P8</f>
         <v/>
       </c>
-      <c r="R8">
+      <c r="R8" s="5">
         <f>F8+Q8</f>
         <v/>
       </c>
-      <c r="S8">
+      <c r="S8" s="5">
         <f>G8+R8</f>
         <v/>
       </c>
-      <c r="T8">
+      <c r="T8" s="5">
         <f>H8+S8</f>
         <v/>
       </c>
-      <c r="V8">
+      <c r="U8" s="3" t="n"/>
+      <c r="V8" s="6">
         <f>N8</f>
         <v/>
       </c>
-      <c r="W8">
+      <c r="W8" s="6">
         <f>IF(O8&lt;=0, 0, IF(O8&lt;=40,O8-N8,IF(O8-N8&lt;=0, 0, ABS(O8-N8-AE8))))</f>
         <v/>
       </c>
-      <c r="X8">
+      <c r="X8" s="6">
         <f>IF(P8&lt;=0, 0, IF(P8&lt;=40,P8-O8,IF(P8-O8&lt;=0, 0, ABS(P8-O8-AF8))))</f>
         <v/>
       </c>
-      <c r="Y8">
+      <c r="Y8" s="6">
         <f>IF(Q8&lt;=0, 0, IF(Q8&lt;=40,Q8-P8,IF(Q8-P8&lt;=0, 0, ABS(Q8-P8-AG8))))</f>
         <v/>
       </c>
-      <c r="Z8">
+      <c r="Z8" s="6">
         <f>IF(R8&lt;=0, 0, IF(R8&lt;=40,R8-Q8,IF(R8-Q8&lt;=0, 0, ABS(R8-Q8-AH8))))</f>
         <v/>
       </c>
-      <c r="AA8">
+      <c r="AA8" s="6">
         <f>IF(S8&lt;=0, 0, IF(S8&lt;=40,S8-R8,IF(S8-R8&lt;=0, 0, ABS(S8-R8-AI8))))</f>
         <v/>
       </c>
-      <c r="AB8">
+      <c r="AB8" s="6">
         <f>IF(T8&lt;=0, 0, IF(T8&lt;=40,T8-S8,IF(T8-S8&lt;=0, 0, ABS(T8-S8-AJ8))))</f>
         <v/>
       </c>
-      <c r="AD8">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="AE8">
+      <c r="AC8" s="3" t="n"/>
+      <c r="AD8" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE8" s="7">
         <f>IF(O8&lt;=0, 0, IF(O8&lt;=40,0, IF(O8-N8&lt;=0,0,IF(O8&gt;40, O8-40-SUM(AD8:AD8),0))))</f>
         <v/>
       </c>
-      <c r="AF8">
+      <c r="AF8" s="7">
         <f>IF(P8&lt;=0, 0, IF(P8&lt;=40,0, IF(P8-O8&lt;=0,0,IF(P8&gt;40, P8-40-SUM(AD8:AE8),0))))</f>
         <v/>
       </c>
-      <c r="AG8">
+      <c r="AG8" s="7">
         <f>IF(Q8&lt;=0, 0, IF(Q8&lt;=40,0, IF(Q8-P8&lt;=0,0,IF(Q8&gt;40, Q8-40-SUM(AD8:AF8),0))))</f>
         <v/>
       </c>
-      <c r="AH8">
+      <c r="AH8" s="7">
         <f>IF(R8&lt;=0, 0, IF(R8&lt;=40,0, IF(R8-Q8&lt;=0,0,IF(R8&gt;40, R8-40-SUM(AD8:AG8),0))))</f>
         <v/>
       </c>
-      <c r="AI8">
+      <c r="AI8" s="7">
         <f>IF(S8&lt;=0, 0, IF(S8&lt;=40,0, IF(S8-R8&lt;=0,0,IF(S8&gt;40, S8-40-SUM(AD8:AH8),0))))</f>
         <v/>
       </c>
-      <c r="AJ8">
+      <c r="AJ8" s="7">
         <f>IF(T8&lt;=0, 0, IF(T8&lt;=40,0, IF(T8-S8&lt;=0,0,IF(T8&gt;40, T8-40-SUM(AD8:AI8),0))))</f>
         <v/>
       </c>
-      <c r="AK8" t="inlineStr">
+      <c r="AK8" s="9" t="inlineStr">
         <is>
           <t>GermanCastro</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="9" t="inlineStr">
         <is>
           <t>LuisJimenez</t>
         </is>
       </c>
-      <c r="B9">
+      <c r="B9" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!B9)</f>
         <v/>
       </c>
-      <c r="C9">
+      <c r="C9" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!C9)</f>
         <v/>
       </c>
-      <c r="D9">
+      <c r="D9" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!D9)</f>
         <v/>
       </c>
-      <c r="E9">
+      <c r="E9" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!E9)</f>
         <v/>
       </c>
-      <c r="F9">
+      <c r="F9" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!F9)</f>
         <v/>
       </c>
-      <c r="G9">
+      <c r="G9" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!G9)</f>
         <v/>
       </c>
-      <c r="H9">
+      <c r="H9" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!H9)</f>
         <v/>
       </c>
-      <c r="I9">
+      <c r="I9" s="5">
         <f>SUM(B9:H9)</f>
         <v/>
       </c>
-      <c r="J9">
+      <c r="J9" s="6">
         <f>IF(I9&lt;=40,I9,40)</f>
         <v/>
       </c>
-      <c r="K9">
+      <c r="K9" s="7">
         <f>I9-J9</f>
         <v/>
       </c>
-      <c r="N9">
+      <c r="L9" s="8">
+        <f>I9*15</f>
+        <v/>
+      </c>
+      <c r="M9" s="3" t="n"/>
+      <c r="N9" s="5">
         <f>B9</f>
         <v/>
       </c>
-      <c r="O9">
+      <c r="O9" s="5">
         <f>C9+N9</f>
         <v/>
       </c>
-      <c r="P9">
+      <c r="P9" s="5">
         <f>D9+O9</f>
         <v/>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="5">
         <f>E9+P9</f>
         <v/>
       </c>
-      <c r="R9">
+      <c r="R9" s="5">
         <f>F9+Q9</f>
         <v/>
       </c>
-      <c r="S9">
+      <c r="S9" s="5">
         <f>G9+R9</f>
         <v/>
       </c>
-      <c r="T9">
+      <c r="T9" s="5">
         <f>H9+S9</f>
         <v/>
       </c>
-      <c r="V9">
+      <c r="U9" s="3" t="n"/>
+      <c r="V9" s="6">
         <f>N9</f>
         <v/>
       </c>
-      <c r="W9">
+      <c r="W9" s="6">
         <f>IF(O9&lt;=0, 0, IF(O9&lt;=40,O9-N9,IF(O9-N9&lt;=0, 0, ABS(O9-N9-AE9))))</f>
         <v/>
       </c>
-      <c r="X9">
+      <c r="X9" s="6">
         <f>IF(P9&lt;=0, 0, IF(P9&lt;=40,P9-O9,IF(P9-O9&lt;=0, 0, ABS(P9-O9-AF9))))</f>
         <v/>
       </c>
-      <c r="Y9">
+      <c r="Y9" s="6">
         <f>IF(Q9&lt;=0, 0, IF(Q9&lt;=40,Q9-P9,IF(Q9-P9&lt;=0, 0, ABS(Q9-P9-AG9))))</f>
         <v/>
       </c>
-      <c r="Z9">
+      <c r="Z9" s="6">
         <f>IF(R9&lt;=0, 0, IF(R9&lt;=40,R9-Q9,IF(R9-Q9&lt;=0, 0, ABS(R9-Q9-AH9))))</f>
         <v/>
       </c>
-      <c r="AA9">
+      <c r="AA9" s="6">
         <f>IF(S9&lt;=0, 0, IF(S9&lt;=40,S9-R9,IF(S9-R9&lt;=0, 0, ABS(S9-R9-AI9))))</f>
         <v/>
       </c>
-      <c r="AB9">
+      <c r="AB9" s="6">
         <f>IF(T9&lt;=0, 0, IF(T9&lt;=40,T9-S9,IF(T9-S9&lt;=0, 0, ABS(T9-S9-AJ9))))</f>
         <v/>
       </c>
-      <c r="AD9">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="AE9">
+      <c r="AC9" s="3" t="n"/>
+      <c r="AD9" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE9" s="7">
         <f>IF(O9&lt;=0, 0, IF(O9&lt;=40,0, IF(O9-N9&lt;=0,0,IF(O9&gt;40, O9-40-SUM(AD9:AD9),0))))</f>
         <v/>
       </c>
-      <c r="AF9">
+      <c r="AF9" s="7">
         <f>IF(P9&lt;=0, 0, IF(P9&lt;=40,0, IF(P9-O9&lt;=0,0,IF(P9&gt;40, P9-40-SUM(AD9:AE9),0))))</f>
         <v/>
       </c>
-      <c r="AG9">
+      <c r="AG9" s="7">
         <f>IF(Q9&lt;=0, 0, IF(Q9&lt;=40,0, IF(Q9-P9&lt;=0,0,IF(Q9&gt;40, Q9-40-SUM(AD9:AF9),0))))</f>
         <v/>
       </c>
-      <c r="AH9">
+      <c r="AH9" s="7">
         <f>IF(R9&lt;=0, 0, IF(R9&lt;=40,0, IF(R9-Q9&lt;=0,0,IF(R9&gt;40, R9-40-SUM(AD9:AG9),0))))</f>
         <v/>
       </c>
-      <c r="AI9">
+      <c r="AI9" s="7">
         <f>IF(S9&lt;=0, 0, IF(S9&lt;=40,0, IF(S9-R9&lt;=0,0,IF(S9&gt;40, S9-40-SUM(AD9:AH9),0))))</f>
         <v/>
       </c>
-      <c r="AJ9">
+      <c r="AJ9" s="7">
         <f>IF(T9&lt;=0, 0, IF(T9&lt;=40,0, IF(T9-S9&lt;=0,0,IF(T9&gt;40, T9-40-SUM(AD9:AI9),0))))</f>
         <v/>
       </c>
-      <c r="AK9" t="inlineStr">
+      <c r="AK9" s="9" t="inlineStr">
         <is>
           <t>LuisJimenez</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="9" t="inlineStr">
         <is>
           <t>ManuelLopez</t>
         </is>
       </c>
-      <c r="B10">
+      <c r="B10" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!B10)</f>
         <v/>
       </c>
-      <c r="C10">
+      <c r="C10" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!C10)</f>
         <v/>
       </c>
-      <c r="D10">
+      <c r="D10" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!D10)</f>
         <v/>
       </c>
-      <c r="E10">
+      <c r="E10" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!E10)</f>
         <v/>
       </c>
-      <c r="F10">
+      <c r="F10" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!F10)</f>
         <v/>
       </c>
-      <c r="G10">
+      <c r="G10" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!G10)</f>
         <v/>
       </c>
-      <c r="H10">
+      <c r="H10" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!H10)</f>
         <v/>
       </c>
-      <c r="I10">
+      <c r="I10" s="5">
         <f>SUM(B10:H10)</f>
         <v/>
       </c>
-      <c r="J10">
+      <c r="J10" s="6">
         <f>IF(I10&lt;=40,I10,40)</f>
         <v/>
       </c>
-      <c r="K10">
+      <c r="K10" s="7">
         <f>I10-J10</f>
         <v/>
       </c>
-      <c r="N10">
+      <c r="L10" s="8">
+        <f>I10*15</f>
+        <v/>
+      </c>
+      <c r="M10" s="3" t="n"/>
+      <c r="N10" s="5">
         <f>B10</f>
         <v/>
       </c>
-      <c r="O10">
+      <c r="O10" s="5">
         <f>C10+N10</f>
         <v/>
       </c>
-      <c r="P10">
+      <c r="P10" s="5">
         <f>D10+O10</f>
         <v/>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="5">
         <f>E10+P10</f>
         <v/>
       </c>
-      <c r="R10">
+      <c r="R10" s="5">
         <f>F10+Q10</f>
         <v/>
       </c>
-      <c r="S10">
+      <c r="S10" s="5">
         <f>G10+R10</f>
         <v/>
       </c>
-      <c r="T10">
+      <c r="T10" s="5">
         <f>H10+S10</f>
         <v/>
       </c>
-      <c r="V10">
+      <c r="U10" s="3" t="n"/>
+      <c r="V10" s="6">
         <f>N10</f>
         <v/>
       </c>
-      <c r="W10">
+      <c r="W10" s="6">
         <f>IF(O10&lt;=0, 0, IF(O10&lt;=40,O10-N10,IF(O10-N10&lt;=0, 0, ABS(O10-N10-AE10))))</f>
         <v/>
       </c>
-      <c r="X10">
+      <c r="X10" s="6">
         <f>IF(P10&lt;=0, 0, IF(P10&lt;=40,P10-O10,IF(P10-O10&lt;=0, 0, ABS(P10-O10-AF10))))</f>
         <v/>
       </c>
-      <c r="Y10">
+      <c r="Y10" s="6">
         <f>IF(Q10&lt;=0, 0, IF(Q10&lt;=40,Q10-P10,IF(Q10-P10&lt;=0, 0, ABS(Q10-P10-AG10))))</f>
         <v/>
       </c>
-      <c r="Z10">
+      <c r="Z10" s="6">
         <f>IF(R10&lt;=0, 0, IF(R10&lt;=40,R10-Q10,IF(R10-Q10&lt;=0, 0, ABS(R10-Q10-AH10))))</f>
         <v/>
       </c>
-      <c r="AA10">
+      <c r="AA10" s="6">
         <f>IF(S10&lt;=0, 0, IF(S10&lt;=40,S10-R10,IF(S10-R10&lt;=0, 0, ABS(S10-R10-AI10))))</f>
         <v/>
       </c>
-      <c r="AB10">
+      <c r="AB10" s="6">
         <f>IF(T10&lt;=0, 0, IF(T10&lt;=40,T10-S10,IF(T10-S10&lt;=0, 0, ABS(T10-S10-AJ10))))</f>
         <v/>
       </c>
-      <c r="AD10">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="AE10">
+      <c r="AC10" s="3" t="n"/>
+      <c r="AD10" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE10" s="7">
         <f>IF(O10&lt;=0, 0, IF(O10&lt;=40,0, IF(O10-N10&lt;=0,0,IF(O10&gt;40, O10-40-SUM(AD10:AD10),0))))</f>
         <v/>
       </c>
-      <c r="AF10">
+      <c r="AF10" s="7">
         <f>IF(P10&lt;=0, 0, IF(P10&lt;=40,0, IF(P10-O10&lt;=0,0,IF(P10&gt;40, P10-40-SUM(AD10:AE10),0))))</f>
         <v/>
       </c>
-      <c r="AG10">
+      <c r="AG10" s="7">
         <f>IF(Q10&lt;=0, 0, IF(Q10&lt;=40,0, IF(Q10-P10&lt;=0,0,IF(Q10&gt;40, Q10-40-SUM(AD10:AF10),0))))</f>
         <v/>
       </c>
-      <c r="AH10">
+      <c r="AH10" s="7">
         <f>IF(R10&lt;=0, 0, IF(R10&lt;=40,0, IF(R10-Q10&lt;=0,0,IF(R10&gt;40, R10-40-SUM(AD10:AG10),0))))</f>
         <v/>
       </c>
-      <c r="AI10">
+      <c r="AI10" s="7">
         <f>IF(S10&lt;=0, 0, IF(S10&lt;=40,0, IF(S10-R10&lt;=0,0,IF(S10&gt;40, S10-40-SUM(AD10:AH10),0))))</f>
         <v/>
       </c>
-      <c r="AJ10">
+      <c r="AJ10" s="7">
         <f>IF(T10&lt;=0, 0, IF(T10&lt;=40,0, IF(T10-S10&lt;=0,0,IF(T10&gt;40, T10-40-SUM(AD10:AI10),0))))</f>
         <v/>
       </c>
-      <c r="AK10" t="inlineStr">
+      <c r="AK10" s="9" t="inlineStr">
         <is>
           <t>ManuelLopez</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="9" t="inlineStr">
         <is>
           <t>SaraOrtiz</t>
         </is>
       </c>
-      <c r="B11">
+      <c r="B11" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!B11)</f>
         <v/>
       </c>
-      <c r="C11">
+      <c r="C11" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!C11)</f>
         <v/>
       </c>
-      <c r="D11">
+      <c r="D11" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!D11)</f>
         <v/>
       </c>
-      <c r="E11">
+      <c r="E11" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!E11)</f>
         <v/>
       </c>
-      <c r="F11">
+      <c r="F11" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!F11)</f>
         <v/>
       </c>
-      <c r="G11">
+      <c r="G11" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!G11)</f>
         <v/>
       </c>
-      <c r="H11">
+      <c r="H11" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!H11)</f>
         <v/>
       </c>
-      <c r="I11">
+      <c r="I11" s="5">
         <f>SUM(B11:H11)</f>
         <v/>
       </c>
-      <c r="J11">
+      <c r="J11" s="6">
         <f>IF(I11&lt;=40,I11,40)</f>
         <v/>
       </c>
-      <c r="K11">
+      <c r="K11" s="7">
         <f>I11-J11</f>
         <v/>
       </c>
-      <c r="N11">
+      <c r="L11" s="8">
+        <f>I11*15</f>
+        <v/>
+      </c>
+      <c r="M11" s="3" t="n"/>
+      <c r="N11" s="5">
         <f>B11</f>
         <v/>
       </c>
-      <c r="O11">
+      <c r="O11" s="5">
         <f>C11+N11</f>
         <v/>
       </c>
-      <c r="P11">
+      <c r="P11" s="5">
         <f>D11+O11</f>
         <v/>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="5">
         <f>E11+P11</f>
         <v/>
       </c>
-      <c r="R11">
+      <c r="R11" s="5">
         <f>F11+Q11</f>
         <v/>
       </c>
-      <c r="S11">
+      <c r="S11" s="5">
         <f>G11+R11</f>
         <v/>
       </c>
-      <c r="T11">
+      <c r="T11" s="5">
         <f>H11+S11</f>
         <v/>
       </c>
-      <c r="V11">
+      <c r="U11" s="3" t="n"/>
+      <c r="V11" s="6">
         <f>N11</f>
         <v/>
       </c>
-      <c r="W11">
+      <c r="W11" s="6">
         <f>IF(O11&lt;=0, 0, IF(O11&lt;=40,O11-N11,IF(O11-N11&lt;=0, 0, ABS(O11-N11-AE11))))</f>
         <v/>
       </c>
-      <c r="X11">
+      <c r="X11" s="6">
         <f>IF(P11&lt;=0, 0, IF(P11&lt;=40,P11-O11,IF(P11-O11&lt;=0, 0, ABS(P11-O11-AF11))))</f>
         <v/>
       </c>
-      <c r="Y11">
+      <c r="Y11" s="6">
         <f>IF(Q11&lt;=0, 0, IF(Q11&lt;=40,Q11-P11,IF(Q11-P11&lt;=0, 0, ABS(Q11-P11-AG11))))</f>
         <v/>
       </c>
-      <c r="Z11">
+      <c r="Z11" s="6">
         <f>IF(R11&lt;=0, 0, IF(R11&lt;=40,R11-Q11,IF(R11-Q11&lt;=0, 0, ABS(R11-Q11-AH11))))</f>
         <v/>
       </c>
-      <c r="AA11">
+      <c r="AA11" s="6">
         <f>IF(S11&lt;=0, 0, IF(S11&lt;=40,S11-R11,IF(S11-R11&lt;=0, 0, ABS(S11-R11-AI11))))</f>
         <v/>
       </c>
-      <c r="AB11">
+      <c r="AB11" s="6">
         <f>IF(T11&lt;=0, 0, IF(T11&lt;=40,T11-S11,IF(T11-S11&lt;=0, 0, ABS(T11-S11-AJ11))))</f>
         <v/>
       </c>
-      <c r="AD11">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="AE11">
+      <c r="AC11" s="3" t="n"/>
+      <c r="AD11" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE11" s="7">
         <f>IF(O11&lt;=0, 0, IF(O11&lt;=40,0, IF(O11-N11&lt;=0,0,IF(O11&gt;40, O11-40-SUM(AD11:AD11),0))))</f>
         <v/>
       </c>
-      <c r="AF11">
+      <c r="AF11" s="7">
         <f>IF(P11&lt;=0, 0, IF(P11&lt;=40,0, IF(P11-O11&lt;=0,0,IF(P11&gt;40, P11-40-SUM(AD11:AE11),0))))</f>
         <v/>
       </c>
-      <c r="AG11">
+      <c r="AG11" s="7">
         <f>IF(Q11&lt;=0, 0, IF(Q11&lt;=40,0, IF(Q11-P11&lt;=0,0,IF(Q11&gt;40, Q11-40-SUM(AD11:AF11),0))))</f>
         <v/>
       </c>
-      <c r="AH11">
+      <c r="AH11" s="7">
         <f>IF(R11&lt;=0, 0, IF(R11&lt;=40,0, IF(R11-Q11&lt;=0,0,IF(R11&gt;40, R11-40-SUM(AD11:AG11),0))))</f>
         <v/>
       </c>
-      <c r="AI11">
+      <c r="AI11" s="7">
         <f>IF(S11&lt;=0, 0, IF(S11&lt;=40,0, IF(S11-R11&lt;=0,0,IF(S11&gt;40, S11-40-SUM(AD11:AH11),0))))</f>
         <v/>
       </c>
-      <c r="AJ11">
+      <c r="AJ11" s="7">
         <f>IF(T11&lt;=0, 0, IF(T11&lt;=40,0, IF(T11-S11&lt;=0,0,IF(T11&gt;40, T11-40-SUM(AD11:AI11),0))))</f>
         <v/>
       </c>
-      <c r="AK11" t="inlineStr">
+      <c r="AK11" s="9" t="inlineStr">
         <is>
           <t>SaraOrtiz</t>
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="9" t="inlineStr">
         <is>
           <t>YuniorOrtiz</t>
         </is>
       </c>
-      <c r="B12">
+      <c r="B12" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!B12)</f>
         <v/>
       </c>
-      <c r="C12">
+      <c r="C12" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!C12)</f>
         <v/>
       </c>
-      <c r="D12">
+      <c r="D12" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!D12)</f>
         <v/>
       </c>
-      <c r="E12">
+      <c r="E12" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!E12)</f>
         <v/>
       </c>
-      <c r="F12">
+      <c r="F12" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!F12)</f>
         <v/>
       </c>
-      <c r="G12">
+      <c r="G12" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!G12)</f>
         <v/>
       </c>
-      <c r="H12">
+      <c r="H12" s="15">
         <f>SUM('CWAthleticoNapervilleRTE59:WindwoodCondo'!H12)</f>
         <v/>
       </c>
-      <c r="I12">
+      <c r="I12" s="5">
         <f>SUM(B12:H12)</f>
         <v/>
       </c>
-      <c r="J12">
+      <c r="J12" s="6">
         <f>IF(I12&lt;=40,I12,40)</f>
         <v/>
       </c>
-      <c r="K12">
+      <c r="K12" s="7">
         <f>I12-J12</f>
         <v/>
       </c>
-      <c r="N12">
+      <c r="L12" s="8">
+        <f>I12*15</f>
+        <v/>
+      </c>
+      <c r="M12" s="3" t="n"/>
+      <c r="N12" s="5">
         <f>B12</f>
         <v/>
       </c>
-      <c r="O12">
+      <c r="O12" s="5">
         <f>C12+N12</f>
         <v/>
       </c>
-      <c r="P12">
+      <c r="P12" s="5">
         <f>D12+O12</f>
         <v/>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="5">
         <f>E12+P12</f>
         <v/>
       </c>
-      <c r="R12">
+      <c r="R12" s="5">
         <f>F12+Q12</f>
         <v/>
       </c>
-      <c r="S12">
+      <c r="S12" s="5">
         <f>G12+R12</f>
         <v/>
       </c>
-      <c r="T12">
+      <c r="T12" s="5">
         <f>H12+S12</f>
         <v/>
       </c>
-      <c r="V12">
+      <c r="U12" s="3" t="n"/>
+      <c r="V12" s="6">
         <f>N12</f>
         <v/>
       </c>
-      <c r="W12">
+      <c r="W12" s="6">
         <f>IF(O12&lt;=0, 0, IF(O12&lt;=40,O12-N12,IF(O12-N12&lt;=0, 0, ABS(O12-N12-AE12))))</f>
         <v/>
       </c>
-      <c r="X12">
+      <c r="X12" s="6">
         <f>IF(P12&lt;=0, 0, IF(P12&lt;=40,P12-O12,IF(P12-O12&lt;=0, 0, ABS(P12-O12-AF12))))</f>
         <v/>
       </c>
-      <c r="Y12">
+      <c r="Y12" s="6">
         <f>IF(Q12&lt;=0, 0, IF(Q12&lt;=40,Q12-P12,IF(Q12-P12&lt;=0, 0, ABS(Q12-P12-AG12))))</f>
         <v/>
       </c>
-      <c r="Z12">
+      <c r="Z12" s="6">
         <f>IF(R12&lt;=0, 0, IF(R12&lt;=40,R12-Q12,IF(R12-Q12&lt;=0, 0, ABS(R12-Q12-AH12))))</f>
         <v/>
       </c>
-      <c r="AA12">
+      <c r="AA12" s="6">
         <f>IF(S12&lt;=0, 0, IF(S12&lt;=40,S12-R12,IF(S12-R12&lt;=0, 0, ABS(S12-R12-AI12))))</f>
         <v/>
       </c>
-      <c r="AB12">
+      <c r="AB12" s="6">
         <f>IF(T12&lt;=0, 0, IF(T12&lt;=40,T12-S12,IF(T12-S12&lt;=0, 0, ABS(T12-S12-AJ12))))</f>
         <v/>
       </c>
-      <c r="AD12">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="AE12">
+      <c r="AC12" s="3" t="n"/>
+      <c r="AD12" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="AE12" s="7">
         <f>IF(O12&lt;=0, 0, IF(O12&lt;=40,0, IF(O12-N12&lt;=0,0,IF(O12&gt;40, O12-40-SUM(AD12:AD12),0))))</f>
         <v/>
       </c>
-      <c r="AF12">
+      <c r="AF12" s="7">
         <f>IF(P12&lt;=0, 0, IF(P12&lt;=40,0, IF(P12-O12&lt;=0,0,IF(P12&gt;40, P12-40-SUM(AD12:AE12),0))))</f>
         <v/>
       </c>
-      <c r="AG12">
+      <c r="AG12" s="7">
         <f>IF(Q12&lt;=0, 0, IF(Q12&lt;=40,0, IF(Q12-P12&lt;=0,0,IF(Q12&gt;40, Q12-40-SUM(AD12:AF12),0))))</f>
         <v/>
       </c>
-      <c r="AH12">
+      <c r="AH12" s="7">
         <f>IF(R12&lt;=0, 0, IF(R12&lt;=40,0, IF(R12-Q12&lt;=0,0,IF(R12&gt;40, R12-40-SUM(AD12:AG12),0))))</f>
         <v/>
       </c>
-      <c r="AI12">
+      <c r="AI12" s="7">
         <f>IF(S12&lt;=0, 0, IF(S12&lt;=40,0, IF(S12-R12&lt;=0,0,IF(S12&gt;40, S12-40-SUM(AD12:AH12),0))))</f>
         <v/>
       </c>
-      <c r="AJ12">
+      <c r="AJ12" s="7">
         <f>IF(T12&lt;=0, 0, IF(T12&lt;=40,0, IF(T12-S12&lt;=0,0,IF(T12&gt;40, T12-40-SUM(AD12:AI12),0))))</f>
         <v/>
       </c>
-      <c r="AK12" t="inlineStr">
+      <c r="AK12" s="9" t="inlineStr">
         <is>
           <t>YuniorOrtiz</t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="13" ht="33" customHeight="1">
+      <c r="A13" s="5" t="inlineStr">
         <is>
           <t>TOTAL HOURS DAY - DAILY</t>
         </is>
       </c>
-      <c r="B13">
+      <c r="B13" s="5">
         <f>SUM(B3:B12)</f>
         <v/>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <f>SUM(C3:C12)</f>
         <v/>
       </c>
-      <c r="D13">
+      <c r="D13" s="5">
         <f>SUM(D3:D12)</f>
         <v/>
       </c>
-      <c r="E13">
+      <c r="E13" s="5">
         <f>SUM(E3:E12)</f>
         <v/>
       </c>
-      <c r="F13">
+      <c r="F13" s="5">
         <f>SUM(F3:F12)</f>
         <v/>
       </c>
-      <c r="G13">
+      <c r="G13" s="5">
         <f>SUM(G3:G12)</f>
         <v/>
       </c>
-      <c r="H13">
+      <c r="H13" s="5">
         <f>SUM(H3:H12)</f>
         <v/>
       </c>
-      <c r="I13">
+      <c r="I13" s="10">
         <f>SUM(I3:I12)</f>
         <v/>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="J13" s="6" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="K13" s="7" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="N13">
+      <c r="L13" s="8">
+        <f>I13*15</f>
+        <v/>
+      </c>
+      <c r="M13" s="3" t="n"/>
+      <c r="N13" s="10">
         <f>SUM(N3:N12)</f>
         <v/>
       </c>
-      <c r="O13">
+      <c r="O13" s="10">
         <f>SUM(O3:O12)</f>
         <v/>
       </c>
-      <c r="P13">
+      <c r="P13" s="10">
         <f>SUM(P3:P12)</f>
         <v/>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="10">
         <f>SUM(Q3:Q12)</f>
         <v/>
       </c>
-      <c r="R13">
+      <c r="R13" s="10">
         <f>SUM(R3:R12)</f>
         <v/>
       </c>
-      <c r="S13">
+      <c r="S13" s="10">
         <f>SUM(S3:S12)</f>
         <v/>
       </c>
-      <c r="T13">
+      <c r="T13" s="10">
         <f>SUM(T3:T12)</f>
         <v/>
       </c>
-      <c r="V13">
+      <c r="U13" s="3" t="n"/>
+      <c r="V13" s="11">
         <f>SUM(V3:V12)</f>
         <v/>
       </c>
-      <c r="W13">
+      <c r="W13" s="11">
         <f>SUM(W3:W12)</f>
         <v/>
       </c>
-      <c r="X13">
+      <c r="X13" s="11">
         <f>SUM(X3:X12)</f>
         <v/>
       </c>
-      <c r="Y13">
+      <c r="Y13" s="11">
         <f>SUM(Y3:Y12)</f>
         <v/>
       </c>
-      <c r="Z13">
+      <c r="Z13" s="11">
         <f>SUM(Z3:Z12)</f>
         <v/>
       </c>
-      <c r="AA13">
+      <c r="AA13" s="11">
         <f>SUM(AA3:AA12)</f>
         <v/>
       </c>
-      <c r="AB13">
+      <c r="AB13" s="11">
         <f>SUM(AB3:AB12)</f>
         <v/>
       </c>
-      <c r="AD13">
+      <c r="AC13" s="3" t="n"/>
+      <c r="AD13" s="12">
         <f>SUM(AD3:AD12)</f>
         <v/>
       </c>
-      <c r="AE13">
+      <c r="AE13" s="12">
         <f>SUM(AE3:AE12)</f>
         <v/>
       </c>
-      <c r="AF13">
+      <c r="AF13" s="12">
         <f>SUM(AF3:AF12)</f>
         <v/>
       </c>
-      <c r="AG13">
+      <c r="AG13" s="12">
         <f>SUM(AG3:AG12)</f>
         <v/>
       </c>
-      <c r="AH13">
+      <c r="AH13" s="12">
         <f>SUM(AH3:AH12)</f>
         <v/>
       </c>
-      <c r="AI13">
+      <c r="AI13" s="12">
         <f>SUM(AI3:AI12)</f>
         <v/>
       </c>
-      <c r="AJ13">
+      <c r="AJ13" s="12">
         <f>SUM(AJ3:AJ12)</f>
         <v/>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="AK13" s="3" t="n"/>
+    </row>
+    <row r="14" ht="33" customHeight="1">
+      <c r="A14" s="6" t="inlineStr">
         <is>
           <t>TOTAL REGULAR HOURS - DAILY</t>
         </is>
       </c>
-      <c r="B14">
+      <c r="B14" s="6">
         <f>V13</f>
         <v/>
       </c>
-      <c r="C14">
+      <c r="C14" s="6">
         <f>W13</f>
         <v/>
       </c>
-      <c r="D14">
+      <c r="D14" s="6">
         <f>X13</f>
         <v/>
       </c>
-      <c r="E14">
+      <c r="E14" s="6">
         <f>Y13</f>
         <v/>
       </c>
-      <c r="F14">
+      <c r="F14" s="6">
         <f>Z13</f>
         <v/>
       </c>
-      <c r="G14">
+      <c r="G14" s="6">
         <f>AA13</f>
         <v/>
       </c>
-      <c r="H14">
+      <c r="H14" s="6">
         <f>AB13</f>
         <v/>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="I14" s="6" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="J14">
+      <c r="J14" s="11">
         <f>SUM(J3:J12)</f>
         <v/>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="K14" s="7" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="L14" s="8">
+        <f>J14*15</f>
+        <v/>
+      </c>
+      <c r="M14" s="3" t="n"/>
+      <c r="N14" s="3" t="n"/>
+      <c r="O14" s="3" t="n"/>
+      <c r="P14" s="3" t="n"/>
+      <c r="Q14" s="3" t="n"/>
+      <c r="R14" s="3" t="n"/>
+      <c r="S14" s="3" t="n"/>
+      <c r="T14" s="3" t="n"/>
+      <c r="U14" s="3" t="n"/>
+      <c r="V14" s="3" t="n"/>
+      <c r="W14" s="3" t="n"/>
+      <c r="X14" s="3" t="n"/>
+      <c r="Y14" s="3" t="n"/>
+      <c r="Z14" s="3" t="n"/>
+      <c r="AA14" s="3" t="n"/>
+      <c r="AB14" s="3" t="n"/>
+      <c r="AC14" s="3" t="n"/>
+      <c r="AD14" s="3" t="n"/>
+      <c r="AE14" s="3" t="n"/>
+      <c r="AF14" s="3" t="n"/>
+      <c r="AG14" s="3" t="n"/>
+      <c r="AH14" s="3" t="n"/>
+      <c r="AI14" s="3" t="n"/>
+      <c r="AJ14" s="3" t="n"/>
+      <c r="AK14" s="3" t="n"/>
+    </row>
+    <row r="15" ht="33" customHeight="1">
+      <c r="A15" s="7" t="inlineStr">
         <is>
           <t>TOTAL OVERTIME HOURS - DAILY</t>
         </is>
       </c>
-      <c r="B15">
+      <c r="B15" s="7">
         <f>AD13</f>
         <v/>
       </c>
-      <c r="C15">
+      <c r="C15" s="7">
         <f>AE13</f>
         <v/>
       </c>
-      <c r="D15">
+      <c r="D15" s="7">
         <f>AF13</f>
         <v/>
       </c>
-      <c r="E15">
+      <c r="E15" s="7">
         <f>AG13</f>
         <v/>
       </c>
-      <c r="F15">
+      <c r="F15" s="7">
         <f>AH13</f>
         <v/>
       </c>
-      <c r="G15">
+      <c r="G15" s="7">
         <f>AI13</f>
         <v/>
       </c>
-      <c r="H15">
+      <c r="H15" s="7">
         <f>AJ13</f>
         <v/>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="I15" s="7" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="J15" s="7" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="K15">
+      <c r="K15" s="12">
         <f>SUM(K3:K12)</f>
         <v/>
       </c>
+      <c r="L15" s="8">
+        <f>K15*15</f>
+        <v/>
+      </c>
+      <c r="M15" s="3" t="n"/>
+      <c r="N15" s="3" t="n"/>
+      <c r="O15" s="3" t="n"/>
+      <c r="P15" s="3" t="n"/>
+      <c r="Q15" s="3" t="n"/>
+      <c r="R15" s="3" t="n"/>
+      <c r="S15" s="3" t="n"/>
+      <c r="T15" s="3" t="n"/>
+      <c r="U15" s="3" t="n"/>
+      <c r="V15" s="3" t="n"/>
+      <c r="W15" s="3" t="n"/>
+      <c r="X15" s="3" t="n"/>
+      <c r="Y15" s="3" t="n"/>
+      <c r="Z15" s="3" t="n"/>
+      <c r="AA15" s="3" t="n"/>
+      <c r="AB15" s="3" t="n"/>
+      <c r="AC15" s="3" t="n"/>
+      <c r="AD15" s="3" t="n"/>
+      <c r="AE15" s="3" t="n"/>
+      <c r="AF15" s="3" t="n"/>
+      <c r="AG15" s="3" t="n"/>
+      <c r="AH15" s="3" t="n"/>
+      <c r="AI15" s="3" t="n"/>
+      <c r="AJ15" s="3" t="n"/>
+      <c r="AK15" s="3" t="n"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="AD1:AJ1"/>
+    <mergeCell ref="N1:T1"/>
+    <mergeCell ref="V1:AB1"/>
+    <mergeCell ref="B1:K1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2222,689 +2583,717 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="23" customWidth="1" min="1" max="1"/>
+    <col width="11.86" customWidth="1" min="2" max="2"/>
+    <col width="11.86" customWidth="1" min="3" max="3"/>
+    <col width="11.86" customWidth="1" min="4" max="4"/>
+    <col width="11.86" customWidth="1" min="5" max="5"/>
+    <col width="11.86" customWidth="1" min="6" max="6"/>
+    <col width="11.86" customWidth="1" min="7" max="7"/>
+    <col width="11.86" customWidth="1" min="8" max="8"/>
+    <col width="11.86" customWidth="1" min="9" max="9"/>
+    <col width="11.86" customWidth="1" min="10" max="10"/>
+    <col width="11.86" customWidth="1" min="11" max="11"/>
+    <col width="11.86" customWidth="1" min="12" max="12"/>
+    <col width="11.86" customWidth="1" min="13" max="13"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="56.25" customHeight="1">
+      <c r="A1" s="1" t="n"/>
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>CWAthleticoNapervilleRTE59-101107527</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="C1" s="13" t="n"/>
+      <c r="D1" s="13" t="n"/>
+      <c r="E1" s="13" t="n"/>
+      <c r="F1" s="13" t="n"/>
+      <c r="G1" s="13" t="n"/>
+      <c r="H1" s="13" t="n"/>
+      <c r="I1" s="13" t="n"/>
+      <c r="J1" s="13" t="n"/>
+      <c r="K1" s="14" t="n"/>
+    </row>
+    <row r="2" ht="56.25" customHeight="1">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Names</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr">
         <is>
           <t>Friday 5</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="4" t="inlineStr">
         <is>
           <t>Saturday 6</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="4" t="inlineStr">
         <is>
           <t>Sunday 7</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="4" t="inlineStr">
         <is>
           <t>Monday 8</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="4" t="inlineStr">
         <is>
           <t>Tuesday 9</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="4" t="inlineStr">
         <is>
           <t>Wednesday 10</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" s="4" t="inlineStr">
         <is>
           <t>Thursday 11</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" s="5" t="inlineStr">
         <is>
           <t>TOTAL HOURS - WEEKLY</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" s="6" t="inlineStr">
         <is>
           <t>TOTAL REGULAR HOURS - WEEKLY</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K2" s="7" t="inlineStr">
         <is>
           <t>TOTAL OVERTIME HOURS - WEEKLY</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="9" t="inlineStr">
         <is>
           <t>ClaudiaGil</t>
         </is>
       </c>
-      <c r="B3">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C3">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D3">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E3">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F3">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G3">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H3">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I3">
+      <c r="B3" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C3" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D3" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E3" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F3" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G3" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H3" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I3" s="5">
         <f>SUM(B3:H3)</f>
         <v/>
       </c>
-      <c r="J3">
+      <c r="J3" s="6">
         <f>I3-K3</f>
         <v/>
       </c>
-      <c r="K3">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="K3" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="9" t="inlineStr">
         <is>
           <t>Darwinparedes</t>
         </is>
       </c>
-      <c r="B4">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C4">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D4">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E4">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F4">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G4">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H4">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I4">
+      <c r="B4" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C4" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D4" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E4" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F4" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G4" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H4" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I4" s="5">
         <f>SUM(B4:H4)</f>
         <v/>
       </c>
-      <c r="J4">
+      <c r="J4" s="6">
         <f>I4-K4</f>
         <v/>
       </c>
-      <c r="K4">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="K4" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="9" t="inlineStr">
         <is>
           <t>EdgarCamacho</t>
         </is>
       </c>
-      <c r="B5">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C5">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D5">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E5">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F5">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G5">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H5">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I5">
+      <c r="B5" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C5" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D5" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E5" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F5" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G5" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H5" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I5" s="5">
         <f>SUM(B5:H5)</f>
         <v/>
       </c>
-      <c r="J5">
+      <c r="J5" s="6">
         <f>I5-K5</f>
         <v/>
       </c>
-      <c r="K5">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="K5" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="9" t="inlineStr">
         <is>
           <t>EduardodeSouza</t>
         </is>
       </c>
-      <c r="B6">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C6">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D6">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E6">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F6">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G6">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H6">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I6">
+      <c r="B6" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C6" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D6" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E6" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F6" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G6" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H6" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I6" s="5">
         <f>SUM(B6:H6)</f>
         <v/>
       </c>
-      <c r="J6">
+      <c r="J6" s="6">
         <f>I6-K6</f>
         <v/>
       </c>
-      <c r="K6">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="K6" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="9" t="inlineStr">
         <is>
           <t>Eliasalbornoz</t>
         </is>
       </c>
-      <c r="B7">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C7">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D7">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E7">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F7">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G7">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H7">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I7">
+      <c r="B7" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C7" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D7" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E7" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F7" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G7" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H7" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I7" s="5">
         <f>SUM(B7:H7)</f>
         <v/>
       </c>
-      <c r="J7">
+      <c r="J7" s="6">
         <f>I7-K7</f>
         <v/>
       </c>
-      <c r="K7">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="K7" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="9" t="inlineStr">
         <is>
           <t>GermanCastro</t>
         </is>
       </c>
-      <c r="B8">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C8">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D8">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E8">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F8">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G8">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H8">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I8">
+      <c r="B8" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C8" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D8" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E8" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F8" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G8" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H8" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I8" s="5">
         <f>SUM(B8:H8)</f>
         <v/>
       </c>
-      <c r="J8">
+      <c r="J8" s="6">
         <f>I8-K8</f>
         <v/>
       </c>
-      <c r="K8">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="K8" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="9" t="inlineStr">
         <is>
           <t>LuisJimenez</t>
         </is>
       </c>
-      <c r="B9">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C9">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D9">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E9">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F9">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G9">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H9">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I9">
+      <c r="B9" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C9" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D9" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E9" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F9" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G9" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H9" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I9" s="5">
         <f>SUM(B9:H9)</f>
         <v/>
       </c>
-      <c r="J9">
+      <c r="J9" s="6">
         <f>I9-K9</f>
         <v/>
       </c>
-      <c r="K9">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="K9" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="9" t="inlineStr">
         <is>
           <t>ManuelLopez</t>
         </is>
       </c>
-      <c r="B10">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C10">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D10">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E10">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F10">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G10">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H10">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I10">
+      <c r="B10" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C10" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D10" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E10" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F10" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G10" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H10" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I10" s="5">
         <f>SUM(B10:H10)</f>
         <v/>
       </c>
-      <c r="J10">
+      <c r="J10" s="6">
         <f>I10-K10</f>
         <v/>
       </c>
-      <c r="K10">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="K10" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="9" t="inlineStr">
         <is>
           <t>SaraOrtiz</t>
         </is>
       </c>
-      <c r="B11">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C11">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D11">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E11">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F11">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G11">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H11">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I11">
+      <c r="B11" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C11" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D11" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E11" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F11" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G11" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H11" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I11" s="5">
         <f>SUM(B11:H11)</f>
         <v/>
       </c>
-      <c r="J11">
+      <c r="J11" s="6">
         <f>I11-K11</f>
         <v/>
       </c>
-      <c r="K11">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="K11" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="9" t="inlineStr">
         <is>
           <t>YuniorOrtiz</t>
         </is>
       </c>
-      <c r="B12">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C12">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D12">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E12">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F12">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G12">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H12">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I12">
+      <c r="B12" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C12" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D12" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E12" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F12" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G12" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H12" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I12" s="5">
         <f>SUM(B12:H12)</f>
         <v/>
       </c>
-      <c r="J12">
+      <c r="J12" s="6">
         <f>I12-K12</f>
         <v/>
       </c>
-      <c r="K12">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="K12" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" ht="33" customHeight="1">
+      <c r="A13" s="5" t="inlineStr">
         <is>
           <t>TOTAL HOURS DAY - DAILY</t>
         </is>
       </c>
-      <c r="B13">
+      <c r="B13" s="5">
         <f>SUM(B3:B12)</f>
         <v/>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <f>SUM(C3:C12)</f>
         <v/>
       </c>
-      <c r="D13">
+      <c r="D13" s="5">
         <f>SUM(D3:D12)</f>
         <v/>
       </c>
-      <c r="E13">
+      <c r="E13" s="5">
         <f>SUM(E3:E12)</f>
         <v/>
       </c>
-      <c r="F13">
+      <c r="F13" s="5">
         <f>SUM(F3:F12)</f>
         <v/>
       </c>
-      <c r="G13">
+      <c r="G13" s="5">
         <f>SUM(G3:G12)</f>
         <v/>
       </c>
-      <c r="H13">
+      <c r="H13" s="5">
         <f>SUM(H3:H12)</f>
         <v/>
       </c>
-      <c r="I13">
+      <c r="I13" s="10">
         <f>SUM(I3:I12)</f>
         <v/>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="J13" s="6" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="K13" s="7" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+    <row r="14" ht="33" customHeight="1">
+      <c r="A14" s="6" t="inlineStr">
         <is>
           <t>TOTAL REGULAR HOURS - DAILY</t>
         </is>
       </c>
-      <c r="B14">
+      <c r="B14" s="6">
         <f>B13-B15</f>
         <v/>
       </c>
-      <c r="C14">
+      <c r="C14" s="6">
         <f>C13-C15</f>
         <v/>
       </c>
-      <c r="D14">
+      <c r="D14" s="6">
         <f>D13-D15</f>
         <v/>
       </c>
-      <c r="E14">
+      <c r="E14" s="6">
         <f>E13-E15</f>
         <v/>
       </c>
-      <c r="F14">
+      <c r="F14" s="6">
         <f>F13-F15</f>
         <v/>
       </c>
-      <c r="G14">
+      <c r="G14" s="6">
         <f>G13-G15</f>
         <v/>
       </c>
-      <c r="H14">
+      <c r="H14" s="6">
         <f>H13-H15</f>
         <v/>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="I14" s="6" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="J14">
+      <c r="J14" s="11">
         <f>SUM(J3:J12)</f>
         <v/>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="K14" s="7" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+    <row r="15" ht="33" customHeight="1">
+      <c r="A15" s="7" t="inlineStr">
         <is>
           <t>TOTAL OVERTIME HOURS - DAILY</t>
         </is>
       </c>
-      <c r="B15">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C15">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D15">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E15">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F15">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G15">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H15">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I15" t="inlineStr">
+      <c r="B15" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C15" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D15" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E15" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F15" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G15" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H15" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I15" s="7" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="J15" s="7" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="K15">
+      <c r="K15" s="12">
         <f>SUM(K3:K12)</f>
         <v/>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:K1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2922,689 +3311,717 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="23" customWidth="1" min="1" max="1"/>
+    <col width="11.86" customWidth="1" min="2" max="2"/>
+    <col width="11.86" customWidth="1" min="3" max="3"/>
+    <col width="11.86" customWidth="1" min="4" max="4"/>
+    <col width="11.86" customWidth="1" min="5" max="5"/>
+    <col width="11.86" customWidth="1" min="6" max="6"/>
+    <col width="11.86" customWidth="1" min="7" max="7"/>
+    <col width="11.86" customWidth="1" min="8" max="8"/>
+    <col width="11.86" customWidth="1" min="9" max="9"/>
+    <col width="11.86" customWidth="1" min="10" max="10"/>
+    <col width="11.86" customWidth="1" min="11" max="11"/>
+    <col width="11.86" customWidth="1" min="12" max="12"/>
+    <col width="11.86" customWidth="1" min="13" max="13"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="56.25" customHeight="1">
+      <c r="A1" s="1" t="n"/>
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>WindwoodCondo-101107012</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="C1" s="13" t="n"/>
+      <c r="D1" s="13" t="n"/>
+      <c r="E1" s="13" t="n"/>
+      <c r="F1" s="13" t="n"/>
+      <c r="G1" s="13" t="n"/>
+      <c r="H1" s="13" t="n"/>
+      <c r="I1" s="13" t="n"/>
+      <c r="J1" s="13" t="n"/>
+      <c r="K1" s="14" t="n"/>
+    </row>
+    <row r="2" ht="56.25" customHeight="1">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Names</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr">
         <is>
           <t>Friday 5</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="4" t="inlineStr">
         <is>
           <t>Saturday 6</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="4" t="inlineStr">
         <is>
           <t>Sunday 7</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="4" t="inlineStr">
         <is>
           <t>Monday 8</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="4" t="inlineStr">
         <is>
           <t>Tuesday 9</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="4" t="inlineStr">
         <is>
           <t>Wednesday 10</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" s="4" t="inlineStr">
         <is>
           <t>Thursday 11</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" s="5" t="inlineStr">
         <is>
           <t>TOTAL HOURS - WEEKLY</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" s="6" t="inlineStr">
         <is>
           <t>TOTAL REGULAR HOURS - WEEKLY</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K2" s="7" t="inlineStr">
         <is>
           <t>TOTAL OVERTIME HOURS - WEEKLY</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="9" t="inlineStr">
         <is>
           <t>ClaudiaGil</t>
         </is>
       </c>
-      <c r="B3">
+      <c r="B3" s="15">
         <f>8.50</f>
         <v/>
       </c>
-      <c r="C3">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D3">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E3">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F3">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G3">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H3">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I3">
+      <c r="C3" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D3" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E3" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F3" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G3" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H3" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I3" s="5">
         <f>SUM(B3:H3)</f>
         <v/>
       </c>
-      <c r="J3">
+      <c r="J3" s="6">
         <f>I3-K3</f>
         <v/>
       </c>
-      <c r="K3">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="K3" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="9" t="inlineStr">
         <is>
           <t>Darwinparedes</t>
         </is>
       </c>
-      <c r="B4">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C4">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D4">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E4">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F4">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G4">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H4">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I4">
+      <c r="B4" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C4" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D4" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E4" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F4" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G4" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H4" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I4" s="5">
         <f>SUM(B4:H4)</f>
         <v/>
       </c>
-      <c r="J4">
+      <c r="J4" s="6">
         <f>I4-K4</f>
         <v/>
       </c>
-      <c r="K4">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="K4" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="9" t="inlineStr">
         <is>
           <t>EdgarCamacho</t>
         </is>
       </c>
-      <c r="B5">
+      <c r="B5" s="15">
         <f>8.50</f>
         <v/>
       </c>
-      <c r="C5">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D5">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E5">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F5">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G5">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H5">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I5">
+      <c r="C5" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D5" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E5" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F5" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G5" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H5" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I5" s="5">
         <f>SUM(B5:H5)</f>
         <v/>
       </c>
-      <c r="J5">
+      <c r="J5" s="6">
         <f>I5-K5</f>
         <v/>
       </c>
-      <c r="K5">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="K5" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="9" t="inlineStr">
         <is>
           <t>EduardodeSouza</t>
         </is>
       </c>
-      <c r="B6">
+      <c r="B6" s="15">
         <f>8.50</f>
         <v/>
       </c>
-      <c r="C6">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D6">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E6">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F6">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G6">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H6">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I6">
+      <c r="C6" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D6" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E6" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F6" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G6" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H6" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I6" s="5">
         <f>SUM(B6:H6)</f>
         <v/>
       </c>
-      <c r="J6">
+      <c r="J6" s="6">
         <f>I6-K6</f>
         <v/>
       </c>
-      <c r="K6">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="K6" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="9" t="inlineStr">
         <is>
           <t>Eliasalbornoz</t>
         </is>
       </c>
-      <c r="B7">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C7">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D7">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E7">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F7">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G7">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H7">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I7">
+      <c r="B7" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C7" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D7" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E7" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F7" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G7" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H7" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I7" s="5">
         <f>SUM(B7:H7)</f>
         <v/>
       </c>
-      <c r="J7">
+      <c r="J7" s="6">
         <f>I7-K7</f>
         <v/>
       </c>
-      <c r="K7">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="K7" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="9" t="inlineStr">
         <is>
           <t>GermanCastro</t>
         </is>
       </c>
-      <c r="B8">
+      <c r="B8" s="15">
         <f>8.50</f>
         <v/>
       </c>
-      <c r="C8">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D8">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E8">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F8">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G8">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H8">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I8">
+      <c r="C8" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D8" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E8" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F8" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G8" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H8" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I8" s="5">
         <f>SUM(B8:H8)</f>
         <v/>
       </c>
-      <c r="J8">
+      <c r="J8" s="6">
         <f>I8-K8</f>
         <v/>
       </c>
-      <c r="K8">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="K8" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="9" t="inlineStr">
         <is>
           <t>LuisJimenez</t>
         </is>
       </c>
-      <c r="B9">
+      <c r="B9" s="15">
         <f>8.50</f>
         <v/>
       </c>
-      <c r="C9">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D9">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E9">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F9">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G9">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H9">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I9">
+      <c r="C9" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D9" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E9" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F9" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G9" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H9" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I9" s="5">
         <f>SUM(B9:H9)</f>
         <v/>
       </c>
-      <c r="J9">
+      <c r="J9" s="6">
         <f>I9-K9</f>
         <v/>
       </c>
-      <c r="K9">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="K9" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="9" t="inlineStr">
         <is>
           <t>ManuelLopez</t>
         </is>
       </c>
-      <c r="B10">
+      <c r="B10" s="15">
         <f>8.50</f>
         <v/>
       </c>
-      <c r="C10">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D10">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E10">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F10">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G10">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H10">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I10">
+      <c r="C10" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D10" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E10" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F10" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G10" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H10" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I10" s="5">
         <f>SUM(B10:H10)</f>
         <v/>
       </c>
-      <c r="J10">
+      <c r="J10" s="6">
         <f>I10-K10</f>
         <v/>
       </c>
-      <c r="K10">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="K10" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="9" t="inlineStr">
         <is>
           <t>SaraOrtiz</t>
         </is>
       </c>
-      <c r="B11">
+      <c r="B11" s="15">
         <f>8.50</f>
         <v/>
       </c>
-      <c r="C11">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D11">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E11">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F11">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G11">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H11">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I11">
+      <c r="C11" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D11" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E11" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F11" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G11" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H11" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I11" s="5">
         <f>SUM(B11:H11)</f>
         <v/>
       </c>
-      <c r="J11">
+      <c r="J11" s="6">
         <f>I11-K11</f>
         <v/>
       </c>
-      <c r="K11">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="K11" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="9" t="inlineStr">
         <is>
           <t>YuniorOrtiz</t>
         </is>
       </c>
-      <c r="B12">
+      <c r="B12" s="15">
         <f>8.50</f>
         <v/>
       </c>
-      <c r="C12">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D12">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E12">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F12">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G12">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H12">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I12">
+      <c r="C12" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D12" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E12" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F12" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G12" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H12" s="15">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I12" s="5">
         <f>SUM(B12:H12)</f>
         <v/>
       </c>
-      <c r="J12">
+      <c r="J12" s="6">
         <f>I12-K12</f>
         <v/>
       </c>
-      <c r="K12">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="K12" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" ht="33" customHeight="1">
+      <c r="A13" s="5" t="inlineStr">
         <is>
           <t>TOTAL HOURS DAY - DAILY</t>
         </is>
       </c>
-      <c r="B13">
+      <c r="B13" s="5">
         <f>SUM(B3:B12)</f>
         <v/>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <f>SUM(C3:C12)</f>
         <v/>
       </c>
-      <c r="D13">
+      <c r="D13" s="5">
         <f>SUM(D3:D12)</f>
         <v/>
       </c>
-      <c r="E13">
+      <c r="E13" s="5">
         <f>SUM(E3:E12)</f>
         <v/>
       </c>
-      <c r="F13">
+      <c r="F13" s="5">
         <f>SUM(F3:F12)</f>
         <v/>
       </c>
-      <c r="G13">
+      <c r="G13" s="5">
         <f>SUM(G3:G12)</f>
         <v/>
       </c>
-      <c r="H13">
+      <c r="H13" s="5">
         <f>SUM(H3:H12)</f>
         <v/>
       </c>
-      <c r="I13">
+      <c r="I13" s="10">
         <f>SUM(I3:I12)</f>
         <v/>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="J13" s="6" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="K13" s="7" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+    <row r="14" ht="33" customHeight="1">
+      <c r="A14" s="6" t="inlineStr">
         <is>
           <t>TOTAL REGULAR HOURS - DAILY</t>
         </is>
       </c>
-      <c r="B14">
+      <c r="B14" s="6">
         <f>B13-B15</f>
         <v/>
       </c>
-      <c r="C14">
+      <c r="C14" s="6">
         <f>C13-C15</f>
         <v/>
       </c>
-      <c r="D14">
+      <c r="D14" s="6">
         <f>D13-D15</f>
         <v/>
       </c>
-      <c r="E14">
+      <c r="E14" s="6">
         <f>E13-E15</f>
         <v/>
       </c>
-      <c r="F14">
+      <c r="F14" s="6">
         <f>F13-F15</f>
         <v/>
       </c>
-      <c r="G14">
+      <c r="G14" s="6">
         <f>G13-G15</f>
         <v/>
       </c>
-      <c r="H14">
+      <c r="H14" s="6">
         <f>H13-H15</f>
         <v/>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="I14" s="6" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="J14">
+      <c r="J14" s="11">
         <f>SUM(J3:J12)</f>
         <v/>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="K14" s="7" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+    <row r="15" ht="33" customHeight="1">
+      <c r="A15" s="7" t="inlineStr">
         <is>
           <t>TOTAL OVERTIME HOURS - DAILY</t>
         </is>
       </c>
-      <c r="B15">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C15">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D15">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E15">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F15">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G15">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H15">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I15" t="inlineStr">
+      <c r="B15" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C15" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D15" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E15" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F15" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G15" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H15" s="7">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I15" s="7" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="J15" s="7" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="K15">
+      <c r="K15" s="12">
         <f>SUM(K3:K12)</f>
         <v/>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:K1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update version - 30/12/2023 ~ Interface integrated
</commit_message>
<xml_diff>
--- a/test_savedata.xlsx
+++ b/test_savedata.xlsx
@@ -8,12 +8,10 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="General" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="COorMtElandEstatesJBNA" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CortlandEstates" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ParkAstorCondo" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="POARMKASTORCONDOSJBNAE" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpringsAtWeber" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WindwoodCondo" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CortlandEstates" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ParkAstorCondo" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpringsAtWeber" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WindwoodCondo" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -864,31 +862,31 @@
         </is>
       </c>
       <c r="B3" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B3)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!B3)</f>
         <v/>
       </c>
       <c r="C3" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C3)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!C3)</f>
         <v/>
       </c>
       <c r="D3" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D3)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!D3)</f>
         <v/>
       </c>
       <c r="E3" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E3)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!E3)</f>
         <v/>
       </c>
       <c r="F3" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F3)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!F3)</f>
         <v/>
       </c>
       <c r="G3" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G3)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!G3)</f>
         <v/>
       </c>
       <c r="H3" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H3)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!H3)</f>
         <v/>
       </c>
       <c r="I3" s="11">
@@ -1007,31 +1005,31 @@
         </is>
       </c>
       <c r="B4" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B4)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!B4)</f>
         <v/>
       </c>
       <c r="C4" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C4)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!C4)</f>
         <v/>
       </c>
       <c r="D4" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D4)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!D4)</f>
         <v/>
       </c>
       <c r="E4" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E4)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!E4)</f>
         <v/>
       </c>
       <c r="F4" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F4)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!F4)</f>
         <v/>
       </c>
       <c r="G4" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G4)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!G4)</f>
         <v/>
       </c>
       <c r="H4" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H4)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!H4)</f>
         <v/>
       </c>
       <c r="I4" s="11">
@@ -1150,31 +1148,31 @@
         </is>
       </c>
       <c r="B5" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B5)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!B5)</f>
         <v/>
       </c>
       <c r="C5" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C5)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!C5)</f>
         <v/>
       </c>
       <c r="D5" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D5)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!D5)</f>
         <v/>
       </c>
       <c r="E5" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E5)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!E5)</f>
         <v/>
       </c>
       <c r="F5" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F5)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!F5)</f>
         <v/>
       </c>
       <c r="G5" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G5)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!G5)</f>
         <v/>
       </c>
       <c r="H5" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H5)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!H5)</f>
         <v/>
       </c>
       <c r="I5" s="11">
@@ -1293,31 +1291,31 @@
         </is>
       </c>
       <c r="B6" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B6)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!B6)</f>
         <v/>
       </c>
       <c r="C6" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C6)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!C6)</f>
         <v/>
       </c>
       <c r="D6" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D6)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!D6)</f>
         <v/>
       </c>
       <c r="E6" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E6)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!E6)</f>
         <v/>
       </c>
       <c r="F6" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F6)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!F6)</f>
         <v/>
       </c>
       <c r="G6" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G6)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!G6)</f>
         <v/>
       </c>
       <c r="H6" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H6)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!H6)</f>
         <v/>
       </c>
       <c r="I6" s="11">
@@ -1436,31 +1434,31 @@
         </is>
       </c>
       <c r="B7" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B7)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!B7)</f>
         <v/>
       </c>
       <c r="C7" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C7)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!C7)</f>
         <v/>
       </c>
       <c r="D7" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D7)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!D7)</f>
         <v/>
       </c>
       <c r="E7" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E7)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!E7)</f>
         <v/>
       </c>
       <c r="F7" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F7)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!F7)</f>
         <v/>
       </c>
       <c r="G7" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G7)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!G7)</f>
         <v/>
       </c>
       <c r="H7" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H7)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!H7)</f>
         <v/>
       </c>
       <c r="I7" s="11">
@@ -1579,31 +1577,31 @@
         </is>
       </c>
       <c r="B8" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B8)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!B8)</f>
         <v/>
       </c>
       <c r="C8" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C8)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!C8)</f>
         <v/>
       </c>
       <c r="D8" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D8)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!D8)</f>
         <v/>
       </c>
       <c r="E8" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E8)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!E8)</f>
         <v/>
       </c>
       <c r="F8" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F8)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!F8)</f>
         <v/>
       </c>
       <c r="G8" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G8)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!G8)</f>
         <v/>
       </c>
       <c r="H8" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H8)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!H8)</f>
         <v/>
       </c>
       <c r="I8" s="11">
@@ -1722,31 +1720,31 @@
         </is>
       </c>
       <c r="B9" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B9)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!B9)</f>
         <v/>
       </c>
       <c r="C9" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C9)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!C9)</f>
         <v/>
       </c>
       <c r="D9" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D9)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!D9)</f>
         <v/>
       </c>
       <c r="E9" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E9)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!E9)</f>
         <v/>
       </c>
       <c r="F9" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F9)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!F9)</f>
         <v/>
       </c>
       <c r="G9" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G9)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!G9)</f>
         <v/>
       </c>
       <c r="H9" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H9)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!H9)</f>
         <v/>
       </c>
       <c r="I9" s="11">
@@ -1865,31 +1863,31 @@
         </is>
       </c>
       <c r="B10" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B10)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!B10)</f>
         <v/>
       </c>
       <c r="C10" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C10)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!C10)</f>
         <v/>
       </c>
       <c r="D10" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D10)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!D10)</f>
         <v/>
       </c>
       <c r="E10" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E10)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!E10)</f>
         <v/>
       </c>
       <c r="F10" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F10)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!F10)</f>
         <v/>
       </c>
       <c r="G10" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G10)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!G10)</f>
         <v/>
       </c>
       <c r="H10" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H10)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!H10)</f>
         <v/>
       </c>
       <c r="I10" s="11">
@@ -2008,31 +2006,31 @@
         </is>
       </c>
       <c r="B11" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B11)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!B11)</f>
         <v/>
       </c>
       <c r="C11" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C11)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!C11)</f>
         <v/>
       </c>
       <c r="D11" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D11)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!D11)</f>
         <v/>
       </c>
       <c r="E11" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E11)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!E11)</f>
         <v/>
       </c>
       <c r="F11" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F11)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!F11)</f>
         <v/>
       </c>
       <c r="G11" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G11)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!G11)</f>
         <v/>
       </c>
       <c r="H11" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H11)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!H11)</f>
         <v/>
       </c>
       <c r="I11" s="11">
@@ -2151,31 +2149,31 @@
         </is>
       </c>
       <c r="B12" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B12)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!B12)</f>
         <v/>
       </c>
       <c r="C12" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C12)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!C12)</f>
         <v/>
       </c>
       <c r="D12" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D12)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!D12)</f>
         <v/>
       </c>
       <c r="E12" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E12)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!E12)</f>
         <v/>
       </c>
       <c r="F12" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F12)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!F12)</f>
         <v/>
       </c>
       <c r="G12" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G12)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!G12)</f>
         <v/>
       </c>
       <c r="H12" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H12)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!H12)</f>
         <v/>
       </c>
       <c r="I12" s="11">
@@ -2294,31 +2292,31 @@
         </is>
       </c>
       <c r="B13" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B13)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!B13)</f>
         <v/>
       </c>
       <c r="C13" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C13)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!C13)</f>
         <v/>
       </c>
       <c r="D13" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D13)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!D13)</f>
         <v/>
       </c>
       <c r="E13" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E13)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!E13)</f>
         <v/>
       </c>
       <c r="F13" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F13)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!F13)</f>
         <v/>
       </c>
       <c r="G13" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G13)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!G13)</f>
         <v/>
       </c>
       <c r="H13" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H13)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!H13)</f>
         <v/>
       </c>
       <c r="I13" s="11">
@@ -2437,31 +2435,31 @@
         </is>
       </c>
       <c r="B14" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B14)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!B14)</f>
         <v/>
       </c>
       <c r="C14" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C14)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!C14)</f>
         <v/>
       </c>
       <c r="D14" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D14)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!D14)</f>
         <v/>
       </c>
       <c r="E14" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E14)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!E14)</f>
         <v/>
       </c>
       <c r="F14" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F14)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!F14)</f>
         <v/>
       </c>
       <c r="G14" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G14)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!G14)</f>
         <v/>
       </c>
       <c r="H14" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H14)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!H14)</f>
         <v/>
       </c>
       <c r="I14" s="11">
@@ -2580,31 +2578,31 @@
         </is>
       </c>
       <c r="B15" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B15)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!B15)</f>
         <v/>
       </c>
       <c r="C15" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C15)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!C15)</f>
         <v/>
       </c>
       <c r="D15" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D15)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!D15)</f>
         <v/>
       </c>
       <c r="E15" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E15)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!E15)</f>
         <v/>
       </c>
       <c r="F15" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F15)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!F15)</f>
         <v/>
       </c>
       <c r="G15" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G15)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!G15)</f>
         <v/>
       </c>
       <c r="H15" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H15)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!H15)</f>
         <v/>
       </c>
       <c r="I15" s="11">
@@ -2723,31 +2721,31 @@
         </is>
       </c>
       <c r="B16" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B16)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!B16)</f>
         <v/>
       </c>
       <c r="C16" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C16)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!C16)</f>
         <v/>
       </c>
       <c r="D16" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D16)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!D16)</f>
         <v/>
       </c>
       <c r="E16" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E16)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!E16)</f>
         <v/>
       </c>
       <c r="F16" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F16)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!F16)</f>
         <v/>
       </c>
       <c r="G16" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G16)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!G16)</f>
         <v/>
       </c>
       <c r="H16" s="20">
-        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H16)</f>
+        <f>SUM('CortlandEstates:WindwoodCondo'!H16)</f>
         <v/>
       </c>
       <c r="I16" s="11">
@@ -3200,7 +3198,7 @@
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>COorMtElandEstatesJBNA-101107056</t>
+          <t>CortlandEstates-101107057</t>
         </is>
       </c>
       <c r="C1" s="18" t="n"/>
@@ -3806,7 +3804,7 @@
         <v/>
       </c>
       <c r="E14" s="20">
-        <f>1.00</f>
+        <f>1.00+8.50</f>
         <v/>
       </c>
       <c r="F14" s="20">
@@ -4116,7 +4114,7 @@
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>CortlandEstates-101107057</t>
+          <t>ParkAstorCondo-101107060</t>
         </is>
       </c>
       <c r="C1" s="18" t="n"/>
@@ -4248,7 +4246,7 @@
         <v/>
       </c>
       <c r="D4" s="20">
-        <f>0</f>
+        <f>0+4.50</f>
         <v/>
       </c>
       <c r="E4" s="20">
@@ -4346,7 +4344,7 @@
         <v/>
       </c>
       <c r="E6" s="20">
-        <f>0</f>
+        <f>9.00</f>
         <v/>
       </c>
       <c r="F6" s="20">
@@ -4440,7 +4438,7 @@
         <v/>
       </c>
       <c r="E8" s="20">
-        <f>0</f>
+        <f>9.00</f>
         <v/>
       </c>
       <c r="F8" s="20">
@@ -4487,7 +4485,7 @@
         <v/>
       </c>
       <c r="E9" s="20">
-        <f>0</f>
+        <f>9.00</f>
         <v/>
       </c>
       <c r="F9" s="20">
@@ -4577,7 +4575,7 @@
         <v/>
       </c>
       <c r="D11" s="20">
-        <f>0</f>
+        <f>0+4.50</f>
         <v/>
       </c>
       <c r="E11" s="20">
@@ -4624,7 +4622,7 @@
         <v/>
       </c>
       <c r="D12" s="20">
-        <f>0</f>
+        <f>0+4.50</f>
         <v/>
       </c>
       <c r="E12" s="20">
@@ -4675,7 +4673,7 @@
         <v/>
       </c>
       <c r="E13" s="20">
-        <f>0</f>
+        <f>9.00</f>
         <v/>
       </c>
       <c r="F13" s="20">
@@ -4718,11 +4716,11 @@
         <v/>
       </c>
       <c r="D14" s="20">
-        <f>0</f>
+        <f>0+4.50</f>
         <v/>
       </c>
       <c r="E14" s="20">
-        <f>8.50</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="F14" s="20">
@@ -5032,7 +5030,7 @@
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>ParkAstorCondo-101107060</t>
+          <t>SpringsAtWeber-101107046</t>
         </is>
       </c>
       <c r="C1" s="18" t="n"/>
@@ -5262,7 +5260,7 @@
         <v/>
       </c>
       <c r="E6" s="20">
-        <f>9.00</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="F6" s="20">
@@ -5356,7 +5354,7 @@
         <v/>
       </c>
       <c r="E8" s="20">
-        <f>9.00</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="F8" s="20">
@@ -5403,7 +5401,7 @@
         <v/>
       </c>
       <c r="E9" s="20">
-        <f>9.00</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="F9" s="20">
@@ -5591,7 +5589,7 @@
         <v/>
       </c>
       <c r="E13" s="20">
-        <f>9.00</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="F13" s="20">
@@ -5638,7 +5636,7 @@
         <v/>
       </c>
       <c r="E14" s="20">
-        <f>0</f>
+        <f>2.50</f>
         <v/>
       </c>
       <c r="F14" s="20">
@@ -5948,7 +5946,7 @@
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>POARMKASTORCONDOSJBNAE-101107060</t>
+          <t>WindwoodCondo-101107012</t>
         </is>
       </c>
       <c r="C1" s="18" t="n"/>
@@ -6025,1838 +6023,6 @@
         </is>
       </c>
       <c r="B3" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C3" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D3" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E3" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F3" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G3" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H3" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I3" s="11">
-        <f>SUM(B3:H3)</f>
-        <v/>
-      </c>
-      <c r="J3" s="12">
-        <f>I3-K3</f>
-        <v/>
-      </c>
-      <c r="K3" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="9" t="inlineStr">
-        <is>
-          <t>EdgarCamacho</t>
-        </is>
-      </c>
-      <c r="B4" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C4" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D4" s="20">
-        <f>4.50</f>
-        <v/>
-      </c>
-      <c r="E4" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F4" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G4" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H4" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I4" s="11">
-        <f>SUM(B4:H4)</f>
-        <v/>
-      </c>
-      <c r="J4" s="12">
-        <f>I4-K4</f>
-        <v/>
-      </c>
-      <c r="K4" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="9" t="inlineStr">
-        <is>
-          <t>EduardodeSouza</t>
-        </is>
-      </c>
-      <c r="B5" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C5" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D5" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E5" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F5" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G5" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H5" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I5" s="11">
-        <f>SUM(B5:H5)</f>
-        <v/>
-      </c>
-      <c r="J5" s="12">
-        <f>I5-K5</f>
-        <v/>
-      </c>
-      <c r="K5" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="9" t="inlineStr">
-        <is>
-          <t>EdwardoSauca</t>
-        </is>
-      </c>
-      <c r="B6" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C6" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D6" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E6" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F6" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G6" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H6" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I6" s="11">
-        <f>SUM(B6:H6)</f>
-        <v/>
-      </c>
-      <c r="J6" s="12">
-        <f>I6-K6</f>
-        <v/>
-      </c>
-      <c r="K6" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="9" t="inlineStr">
-        <is>
-          <t>GermanCastro</t>
-        </is>
-      </c>
-      <c r="B7" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C7" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D7" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E7" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F7" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G7" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H7" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I7" s="11">
-        <f>SUM(B7:H7)</f>
-        <v/>
-      </c>
-      <c r="J7" s="12">
-        <f>I7-K7</f>
-        <v/>
-      </c>
-      <c r="K7" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="9" t="inlineStr">
-        <is>
-          <t>IsabelaArturo</t>
-        </is>
-      </c>
-      <c r="B8" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C8" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D8" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E8" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F8" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G8" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H8" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I8" s="11">
-        <f>SUM(B8:H8)</f>
-        <v/>
-      </c>
-      <c r="J8" s="12">
-        <f>I8-K8</f>
-        <v/>
-      </c>
-      <c r="K8" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="9" t="inlineStr">
-        <is>
-          <t>Liz</t>
-        </is>
-      </c>
-      <c r="B9" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C9" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D9" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E9" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F9" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G9" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H9" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I9" s="11">
-        <f>SUM(B9:H9)</f>
-        <v/>
-      </c>
-      <c r="J9" s="12">
-        <f>I9-K9</f>
-        <v/>
-      </c>
-      <c r="K9" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="9" t="inlineStr">
-        <is>
-          <t>LuisJimenez</t>
-        </is>
-      </c>
-      <c r="B10" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C10" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D10" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E10" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F10" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G10" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H10" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I10" s="11">
-        <f>SUM(B10:H10)</f>
-        <v/>
-      </c>
-      <c r="J10" s="12">
-        <f>I10-K10</f>
-        <v/>
-      </c>
-      <c r="K10" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="9" t="inlineStr">
-        <is>
-          <t>ManuelLopez</t>
-        </is>
-      </c>
-      <c r="B11" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C11" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D11" s="20">
-        <f>4.50</f>
-        <v/>
-      </c>
-      <c r="E11" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F11" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G11" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H11" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I11" s="11">
-        <f>SUM(B11:H11)</f>
-        <v/>
-      </c>
-      <c r="J11" s="12">
-        <f>I11-K11</f>
-        <v/>
-      </c>
-      <c r="K11" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="9" t="inlineStr">
-        <is>
-          <t>MateoLaverde</t>
-        </is>
-      </c>
-      <c r="B12" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C12" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D12" s="20">
-        <f>4.50</f>
-        <v/>
-      </c>
-      <c r="E12" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F12" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G12" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H12" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I12" s="11">
-        <f>SUM(B12:H12)</f>
-        <v/>
-      </c>
-      <c r="J12" s="12">
-        <f>I12-K12</f>
-        <v/>
-      </c>
-      <c r="K12" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="9" t="inlineStr">
-        <is>
-          <t>MateoMarverde</t>
-        </is>
-      </c>
-      <c r="B13" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C13" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D13" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E13" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F13" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G13" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H13" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I13" s="11">
-        <f>SUM(B13:H13)</f>
-        <v/>
-      </c>
-      <c r="J13" s="12">
-        <f>I13-K13</f>
-        <v/>
-      </c>
-      <c r="K13" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="9" t="inlineStr">
-        <is>
-          <t>PedroForrero</t>
-        </is>
-      </c>
-      <c r="B14" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C14" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D14" s="20">
-        <f>4.50</f>
-        <v/>
-      </c>
-      <c r="E14" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F14" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G14" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H14" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I14" s="11">
-        <f>SUM(B14:H14)</f>
-        <v/>
-      </c>
-      <c r="J14" s="12">
-        <f>I14-K14</f>
-        <v/>
-      </c>
-      <c r="K14" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="9" t="inlineStr">
-        <is>
-          <t>SaraOrtiz</t>
-        </is>
-      </c>
-      <c r="B15" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C15" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D15" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E15" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F15" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G15" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H15" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I15" s="11">
-        <f>SUM(B15:H15)</f>
-        <v/>
-      </c>
-      <c r="J15" s="12">
-        <f>I15-K15</f>
-        <v/>
-      </c>
-      <c r="K15" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="9" t="inlineStr">
-        <is>
-          <t>YuniorOrtiz</t>
-        </is>
-      </c>
-      <c r="B16" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C16" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D16" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E16" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F16" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G16" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H16" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I16" s="11">
-        <f>SUM(B16:H16)</f>
-        <v/>
-      </c>
-      <c r="J16" s="12">
-        <f>I16-K16</f>
-        <v/>
-      </c>
-      <c r="K16" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" ht="33" customHeight="1">
-      <c r="A17" s="5" t="inlineStr">
-        <is>
-          <t>TOTAL HOURS DAY - DAILY</t>
-        </is>
-      </c>
-      <c r="B17" s="11">
-        <f>SUM(B3:B16)</f>
-        <v/>
-      </c>
-      <c r="C17" s="11">
-        <f>SUM(C3:C16)</f>
-        <v/>
-      </c>
-      <c r="D17" s="11">
-        <f>SUM(D3:D16)</f>
-        <v/>
-      </c>
-      <c r="E17" s="11">
-        <f>SUM(E3:E16)</f>
-        <v/>
-      </c>
-      <c r="F17" s="11">
-        <f>SUM(F3:F16)</f>
-        <v/>
-      </c>
-      <c r="G17" s="11">
-        <f>SUM(G3:G16)</f>
-        <v/>
-      </c>
-      <c r="H17" s="11">
-        <f>SUM(H3:H16)</f>
-        <v/>
-      </c>
-      <c r="I17" s="15">
-        <f>SUM(I3:I16)</f>
-        <v/>
-      </c>
-      <c r="J17" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K17" s="13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="18" ht="33" customHeight="1">
-      <c r="A18" s="6" t="inlineStr">
-        <is>
-          <t>TOTAL REGULAR HOURS - DAILY</t>
-        </is>
-      </c>
-      <c r="B18" s="12">
-        <f>B17-B19</f>
-        <v/>
-      </c>
-      <c r="C18" s="12">
-        <f>C17-C19</f>
-        <v/>
-      </c>
-      <c r="D18" s="12">
-        <f>D17-D19</f>
-        <v/>
-      </c>
-      <c r="E18" s="12">
-        <f>E17-E19</f>
-        <v/>
-      </c>
-      <c r="F18" s="12">
-        <f>F17-F19</f>
-        <v/>
-      </c>
-      <c r="G18" s="12">
-        <f>G17-G19</f>
-        <v/>
-      </c>
-      <c r="H18" s="12">
-        <f>H17-H19</f>
-        <v/>
-      </c>
-      <c r="I18" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J18" s="16">
-        <f>SUM(J3:J16)</f>
-        <v/>
-      </c>
-      <c r="K18" s="13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="19" ht="33" customHeight="1">
-      <c r="A19" s="7" t="inlineStr">
-        <is>
-          <t>TOTAL OVERTIME HOURS - DAILY</t>
-        </is>
-      </c>
-      <c r="B19" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C19" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D19" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E19" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F19" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G19" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H19" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I19" s="13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J19" s="13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K19" s="17">
-        <f>SUM(K3:K16)</f>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:K1"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="23" customWidth="1" min="1" max="1"/>
-    <col width="11.86" customWidth="1" min="2" max="2"/>
-    <col width="11.86" customWidth="1" min="3" max="3"/>
-    <col width="11.86" customWidth="1" min="4" max="4"/>
-    <col width="11.86" customWidth="1" min="5" max="5"/>
-    <col width="11.86" customWidth="1" min="6" max="6"/>
-    <col width="11.86" customWidth="1" min="7" max="7"/>
-    <col width="11.86" customWidth="1" min="8" max="8"/>
-    <col width="11.86" customWidth="1" min="9" max="9"/>
-    <col width="11.86" customWidth="1" min="10" max="10"/>
-    <col width="11.86" customWidth="1" min="11" max="11"/>
-    <col width="11.86" customWidth="1" min="12" max="12"/>
-    <col width="11.86" customWidth="1" min="13" max="13"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="56.25" customHeight="1">
-      <c r="A1" s="1" t="n"/>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>SpringsAtWeber-101107046</t>
-        </is>
-      </c>
-      <c r="C1" s="18" t="n"/>
-      <c r="D1" s="18" t="n"/>
-      <c r="E1" s="18" t="n"/>
-      <c r="F1" s="18" t="n"/>
-      <c r="G1" s="18" t="n"/>
-      <c r="H1" s="18" t="n"/>
-      <c r="I1" s="18" t="n"/>
-      <c r="J1" s="18" t="n"/>
-      <c r="K1" s="19" t="n"/>
-    </row>
-    <row r="2" ht="56.25" customHeight="1">
-      <c r="A2" s="4" t="inlineStr">
-        <is>
-          <t>Names</t>
-        </is>
-      </c>
-      <c r="B2" s="4" t="inlineStr">
-        <is>
-          <t>Friday 5</t>
-        </is>
-      </c>
-      <c r="C2" s="4" t="inlineStr">
-        <is>
-          <t>Saturday 6</t>
-        </is>
-      </c>
-      <c r="D2" s="4" t="inlineStr">
-        <is>
-          <t>Sunday 7</t>
-        </is>
-      </c>
-      <c r="E2" s="4" t="inlineStr">
-        <is>
-          <t>Monday 8</t>
-        </is>
-      </c>
-      <c r="F2" s="4" t="inlineStr">
-        <is>
-          <t>Tuesday 9</t>
-        </is>
-      </c>
-      <c r="G2" s="4" t="inlineStr">
-        <is>
-          <t>Wednesday 10</t>
-        </is>
-      </c>
-      <c r="H2" s="4" t="inlineStr">
-        <is>
-          <t>Thursday 11</t>
-        </is>
-      </c>
-      <c r="I2" s="5" t="inlineStr">
-        <is>
-          <t>TOTAL HOURS - WEEKLY</t>
-        </is>
-      </c>
-      <c r="J2" s="6" t="inlineStr">
-        <is>
-          <t>TOTAL REGULAR HOURS - WEEKLY</t>
-        </is>
-      </c>
-      <c r="K2" s="7" t="inlineStr">
-        <is>
-          <t>TOTAL OVERTIME HOURS - WEEKLY</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="9" t="inlineStr">
-        <is>
-          <t>ClaudiaGil</t>
-        </is>
-      </c>
-      <c r="B3" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C3" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D3" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E3" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F3" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G3" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H3" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I3" s="11">
-        <f>SUM(B3:H3)</f>
-        <v/>
-      </c>
-      <c r="J3" s="12">
-        <f>I3-K3</f>
-        <v/>
-      </c>
-      <c r="K3" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="9" t="inlineStr">
-        <is>
-          <t>EdgarCamacho</t>
-        </is>
-      </c>
-      <c r="B4" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C4" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D4" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E4" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F4" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G4" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H4" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I4" s="11">
-        <f>SUM(B4:H4)</f>
-        <v/>
-      </c>
-      <c r="J4" s="12">
-        <f>I4-K4</f>
-        <v/>
-      </c>
-      <c r="K4" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="9" t="inlineStr">
-        <is>
-          <t>EduardodeSouza</t>
-        </is>
-      </c>
-      <c r="B5" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C5" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D5" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E5" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F5" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G5" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H5" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I5" s="11">
-        <f>SUM(B5:H5)</f>
-        <v/>
-      </c>
-      <c r="J5" s="12">
-        <f>I5-K5</f>
-        <v/>
-      </c>
-      <c r="K5" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="9" t="inlineStr">
-        <is>
-          <t>EdwardoSauca</t>
-        </is>
-      </c>
-      <c r="B6" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C6" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D6" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E6" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F6" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G6" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H6" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I6" s="11">
-        <f>SUM(B6:H6)</f>
-        <v/>
-      </c>
-      <c r="J6" s="12">
-        <f>I6-K6</f>
-        <v/>
-      </c>
-      <c r="K6" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="9" t="inlineStr">
-        <is>
-          <t>GermanCastro</t>
-        </is>
-      </c>
-      <c r="B7" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C7" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D7" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E7" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F7" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G7" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H7" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I7" s="11">
-        <f>SUM(B7:H7)</f>
-        <v/>
-      </c>
-      <c r="J7" s="12">
-        <f>I7-K7</f>
-        <v/>
-      </c>
-      <c r="K7" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="9" t="inlineStr">
-        <is>
-          <t>IsabelaArturo</t>
-        </is>
-      </c>
-      <c r="B8" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C8" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D8" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E8" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F8" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G8" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H8" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I8" s="11">
-        <f>SUM(B8:H8)</f>
-        <v/>
-      </c>
-      <c r="J8" s="12">
-        <f>I8-K8</f>
-        <v/>
-      </c>
-      <c r="K8" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="9" t="inlineStr">
-        <is>
-          <t>Liz</t>
-        </is>
-      </c>
-      <c r="B9" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C9" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D9" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E9" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F9" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G9" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H9" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I9" s="11">
-        <f>SUM(B9:H9)</f>
-        <v/>
-      </c>
-      <c r="J9" s="12">
-        <f>I9-K9</f>
-        <v/>
-      </c>
-      <c r="K9" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="9" t="inlineStr">
-        <is>
-          <t>LuisJimenez</t>
-        </is>
-      </c>
-      <c r="B10" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C10" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D10" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E10" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F10" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G10" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H10" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I10" s="11">
-        <f>SUM(B10:H10)</f>
-        <v/>
-      </c>
-      <c r="J10" s="12">
-        <f>I10-K10</f>
-        <v/>
-      </c>
-      <c r="K10" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="9" t="inlineStr">
-        <is>
-          <t>ManuelLopez</t>
-        </is>
-      </c>
-      <c r="B11" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C11" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D11" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E11" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F11" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G11" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H11" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I11" s="11">
-        <f>SUM(B11:H11)</f>
-        <v/>
-      </c>
-      <c r="J11" s="12">
-        <f>I11-K11</f>
-        <v/>
-      </c>
-      <c r="K11" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="9" t="inlineStr">
-        <is>
-          <t>MateoLaverde</t>
-        </is>
-      </c>
-      <c r="B12" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C12" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D12" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E12" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F12" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G12" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H12" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I12" s="11">
-        <f>SUM(B12:H12)</f>
-        <v/>
-      </c>
-      <c r="J12" s="12">
-        <f>I12-K12</f>
-        <v/>
-      </c>
-      <c r="K12" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="9" t="inlineStr">
-        <is>
-          <t>MateoMarverde</t>
-        </is>
-      </c>
-      <c r="B13" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C13" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D13" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E13" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F13" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G13" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H13" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I13" s="11">
-        <f>SUM(B13:H13)</f>
-        <v/>
-      </c>
-      <c r="J13" s="12">
-        <f>I13-K13</f>
-        <v/>
-      </c>
-      <c r="K13" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="9" t="inlineStr">
-        <is>
-          <t>PedroForrero</t>
-        </is>
-      </c>
-      <c r="B14" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C14" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D14" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E14" s="20">
-        <f>2.50</f>
-        <v/>
-      </c>
-      <c r="F14" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G14" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H14" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I14" s="11">
-        <f>SUM(B14:H14)</f>
-        <v/>
-      </c>
-      <c r="J14" s="12">
-        <f>I14-K14</f>
-        <v/>
-      </c>
-      <c r="K14" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="9" t="inlineStr">
-        <is>
-          <t>SaraOrtiz</t>
-        </is>
-      </c>
-      <c r="B15" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C15" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D15" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E15" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F15" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G15" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H15" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I15" s="11">
-        <f>SUM(B15:H15)</f>
-        <v/>
-      </c>
-      <c r="J15" s="12">
-        <f>I15-K15</f>
-        <v/>
-      </c>
-      <c r="K15" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="9" t="inlineStr">
-        <is>
-          <t>YuniorOrtiz</t>
-        </is>
-      </c>
-      <c r="B16" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C16" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D16" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E16" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F16" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G16" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H16" s="20">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I16" s="11">
-        <f>SUM(B16:H16)</f>
-        <v/>
-      </c>
-      <c r="J16" s="12">
-        <f>I16-K16</f>
-        <v/>
-      </c>
-      <c r="K16" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" ht="33" customHeight="1">
-      <c r="A17" s="5" t="inlineStr">
-        <is>
-          <t>TOTAL HOURS DAY - DAILY</t>
-        </is>
-      </c>
-      <c r="B17" s="11">
-        <f>SUM(B3:B16)</f>
-        <v/>
-      </c>
-      <c r="C17" s="11">
-        <f>SUM(C3:C16)</f>
-        <v/>
-      </c>
-      <c r="D17" s="11">
-        <f>SUM(D3:D16)</f>
-        <v/>
-      </c>
-      <c r="E17" s="11">
-        <f>SUM(E3:E16)</f>
-        <v/>
-      </c>
-      <c r="F17" s="11">
-        <f>SUM(F3:F16)</f>
-        <v/>
-      </c>
-      <c r="G17" s="11">
-        <f>SUM(G3:G16)</f>
-        <v/>
-      </c>
-      <c r="H17" s="11">
-        <f>SUM(H3:H16)</f>
-        <v/>
-      </c>
-      <c r="I17" s="15">
-        <f>SUM(I3:I16)</f>
-        <v/>
-      </c>
-      <c r="J17" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K17" s="13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="18" ht="33" customHeight="1">
-      <c r="A18" s="6" t="inlineStr">
-        <is>
-          <t>TOTAL REGULAR HOURS - DAILY</t>
-        </is>
-      </c>
-      <c r="B18" s="12">
-        <f>B17-B19</f>
-        <v/>
-      </c>
-      <c r="C18" s="12">
-        <f>C17-C19</f>
-        <v/>
-      </c>
-      <c r="D18" s="12">
-        <f>D17-D19</f>
-        <v/>
-      </c>
-      <c r="E18" s="12">
-        <f>E17-E19</f>
-        <v/>
-      </c>
-      <c r="F18" s="12">
-        <f>F17-F19</f>
-        <v/>
-      </c>
-      <c r="G18" s="12">
-        <f>G17-G19</f>
-        <v/>
-      </c>
-      <c r="H18" s="12">
-        <f>H17-H19</f>
-        <v/>
-      </c>
-      <c r="I18" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J18" s="16">
-        <f>SUM(J3:J16)</f>
-        <v/>
-      </c>
-      <c r="K18" s="13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="19" ht="33" customHeight="1">
-      <c r="A19" s="7" t="inlineStr">
-        <is>
-          <t>TOTAL OVERTIME HOURS - DAILY</t>
-        </is>
-      </c>
-      <c r="B19" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C19" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="D19" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E19" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="F19" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G19" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="H19" s="13">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="I19" s="13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J19" s="13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K19" s="17">
-        <f>SUM(K3:K16)</f>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:K1"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="23" customWidth="1" min="1" max="1"/>
-    <col width="11.86" customWidth="1" min="2" max="2"/>
-    <col width="11.86" customWidth="1" min="3" max="3"/>
-    <col width="11.86" customWidth="1" min="4" max="4"/>
-    <col width="11.86" customWidth="1" min="5" max="5"/>
-    <col width="11.86" customWidth="1" min="6" max="6"/>
-    <col width="11.86" customWidth="1" min="7" max="7"/>
-    <col width="11.86" customWidth="1" min="8" max="8"/>
-    <col width="11.86" customWidth="1" min="9" max="9"/>
-    <col width="11.86" customWidth="1" min="10" max="10"/>
-    <col width="11.86" customWidth="1" min="11" max="11"/>
-    <col width="11.86" customWidth="1" min="12" max="12"/>
-    <col width="11.86" customWidth="1" min="13" max="13"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="56.25" customHeight="1">
-      <c r="A1" s="1" t="n"/>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>WindwoodCondo-101107012</t>
-        </is>
-      </c>
-      <c r="C1" s="18" t="n"/>
-      <c r="D1" s="18" t="n"/>
-      <c r="E1" s="18" t="n"/>
-      <c r="F1" s="18" t="n"/>
-      <c r="G1" s="18" t="n"/>
-      <c r="H1" s="18" t="n"/>
-      <c r="I1" s="18" t="n"/>
-      <c r="J1" s="18" t="n"/>
-      <c r="K1" s="19" t="n"/>
-    </row>
-    <row r="2" ht="56.25" customHeight="1">
-      <c r="A2" s="4" t="inlineStr">
-        <is>
-          <t>Names</t>
-        </is>
-      </c>
-      <c r="B2" s="4" t="inlineStr">
-        <is>
-          <t>Friday 5</t>
-        </is>
-      </c>
-      <c r="C2" s="4" t="inlineStr">
-        <is>
-          <t>Saturday 6</t>
-        </is>
-      </c>
-      <c r="D2" s="4" t="inlineStr">
-        <is>
-          <t>Sunday 7</t>
-        </is>
-      </c>
-      <c r="E2" s="4" t="inlineStr">
-        <is>
-          <t>Monday 8</t>
-        </is>
-      </c>
-      <c r="F2" s="4" t="inlineStr">
-        <is>
-          <t>Tuesday 9</t>
-        </is>
-      </c>
-      <c r="G2" s="4" t="inlineStr">
-        <is>
-          <t>Wednesday 10</t>
-        </is>
-      </c>
-      <c r="H2" s="4" t="inlineStr">
-        <is>
-          <t>Thursday 11</t>
-        </is>
-      </c>
-      <c r="I2" s="5" t="inlineStr">
-        <is>
-          <t>TOTAL HOURS - WEEKLY</t>
-        </is>
-      </c>
-      <c r="J2" s="6" t="inlineStr">
-        <is>
-          <t>TOTAL REGULAR HOURS - WEEKLY</t>
-        </is>
-      </c>
-      <c r="K2" s="7" t="inlineStr">
-        <is>
-          <t>TOTAL OVERTIME HOURS - WEEKLY</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="9" t="inlineStr">
-        <is>
-          <t>ClaudiaGil</t>
-        </is>
-      </c>
-      <c r="B3" s="20">
         <f>8.50</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
Update version - 31/12/2023 ~ First funcional version
</commit_message>
<xml_diff>
--- a/test_savedata.xlsx
+++ b/test_savedata.xlsx
@@ -8,10 +8,11 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="General" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CortlandEstates" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ParkAstorCondo" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpringsAtWeber" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WindwoodCondo" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CortlandEstates1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CortlandEstates" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ParkAstorCondo" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpringsAtWeber" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WindwoodCondo" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -858,35 +859,35 @@
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>ClaudiaGil</t>
+          <t>Claudia Gil</t>
         </is>
       </c>
       <c r="B3" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!B3)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!B3)</f>
         <v/>
       </c>
       <c r="C3" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!C3)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!C3)</f>
         <v/>
       </c>
       <c r="D3" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!D3)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!D3)</f>
         <v/>
       </c>
       <c r="E3" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!E3)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!E3)</f>
         <v/>
       </c>
       <c r="F3" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!F3)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!F3)</f>
         <v/>
       </c>
       <c r="G3" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!G3)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!G3)</f>
         <v/>
       </c>
       <c r="H3" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!H3)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!H3)</f>
         <v/>
       </c>
       <c r="I3" s="11">
@@ -994,42 +995,42 @@
       </c>
       <c r="AK3" s="9" t="inlineStr">
         <is>
-          <t>ClaudiaGil</t>
+          <t>Claudia Gil</t>
         </is>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>EdgarCamacho</t>
+          <t>Edgar Camacho</t>
         </is>
       </c>
       <c r="B4" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!B4)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!B4)</f>
         <v/>
       </c>
       <c r="C4" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!C4)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!C4)</f>
         <v/>
       </c>
       <c r="D4" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!D4)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!D4)</f>
         <v/>
       </c>
       <c r="E4" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!E4)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!E4)</f>
         <v/>
       </c>
       <c r="F4" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!F4)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!F4)</f>
         <v/>
       </c>
       <c r="G4" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!G4)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!G4)</f>
         <v/>
       </c>
       <c r="H4" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!H4)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!H4)</f>
         <v/>
       </c>
       <c r="I4" s="11">
@@ -1137,7 +1138,7 @@
       </c>
       <c r="AK4" s="9" t="inlineStr">
         <is>
-          <t>EdgarCamacho</t>
+          <t>Edgar Camacho</t>
         </is>
       </c>
     </row>
@@ -1148,31 +1149,31 @@
         </is>
       </c>
       <c r="B5" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!B5)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!B5)</f>
         <v/>
       </c>
       <c r="C5" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!C5)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!C5)</f>
         <v/>
       </c>
       <c r="D5" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!D5)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!D5)</f>
         <v/>
       </c>
       <c r="E5" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!E5)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!E5)</f>
         <v/>
       </c>
       <c r="F5" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!F5)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!F5)</f>
         <v/>
       </c>
       <c r="G5" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!G5)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!G5)</f>
         <v/>
       </c>
       <c r="H5" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!H5)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!H5)</f>
         <v/>
       </c>
       <c r="I5" s="11">
@@ -1291,31 +1292,31 @@
         </is>
       </c>
       <c r="B6" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!B6)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!B6)</f>
         <v/>
       </c>
       <c r="C6" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!C6)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!C6)</f>
         <v/>
       </c>
       <c r="D6" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!D6)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!D6)</f>
         <v/>
       </c>
       <c r="E6" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!E6)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!E6)</f>
         <v/>
       </c>
       <c r="F6" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!F6)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!F6)</f>
         <v/>
       </c>
       <c r="G6" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!G6)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!G6)</f>
         <v/>
       </c>
       <c r="H6" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!H6)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!H6)</f>
         <v/>
       </c>
       <c r="I6" s="11">
@@ -1434,31 +1435,31 @@
         </is>
       </c>
       <c r="B7" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!B7)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!B7)</f>
         <v/>
       </c>
       <c r="C7" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!C7)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!C7)</f>
         <v/>
       </c>
       <c r="D7" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!D7)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!D7)</f>
         <v/>
       </c>
       <c r="E7" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!E7)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!E7)</f>
         <v/>
       </c>
       <c r="F7" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!F7)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!F7)</f>
         <v/>
       </c>
       <c r="G7" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!G7)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!G7)</f>
         <v/>
       </c>
       <c r="H7" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!H7)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!H7)</f>
         <v/>
       </c>
       <c r="I7" s="11">
@@ -1577,31 +1578,31 @@
         </is>
       </c>
       <c r="B8" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!B8)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!B8)</f>
         <v/>
       </c>
       <c r="C8" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!C8)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!C8)</f>
         <v/>
       </c>
       <c r="D8" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!D8)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!D8)</f>
         <v/>
       </c>
       <c r="E8" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!E8)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!E8)</f>
         <v/>
       </c>
       <c r="F8" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!F8)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!F8)</f>
         <v/>
       </c>
       <c r="G8" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!G8)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!G8)</f>
         <v/>
       </c>
       <c r="H8" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!H8)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!H8)</f>
         <v/>
       </c>
       <c r="I8" s="11">
@@ -1716,35 +1717,35 @@
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>Liz</t>
+          <t>Tigre Toño</t>
         </is>
       </c>
       <c r="B9" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!B9)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!B9)</f>
         <v/>
       </c>
       <c r="C9" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!C9)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!C9)</f>
         <v/>
       </c>
       <c r="D9" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!D9)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!D9)</f>
         <v/>
       </c>
       <c r="E9" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!E9)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!E9)</f>
         <v/>
       </c>
       <c r="F9" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!F9)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!F9)</f>
         <v/>
       </c>
       <c r="G9" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!G9)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!G9)</f>
         <v/>
       </c>
       <c r="H9" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!H9)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!H9)</f>
         <v/>
       </c>
       <c r="I9" s="11">
@@ -1852,7 +1853,7 @@
       </c>
       <c r="AK9" s="9" t="inlineStr">
         <is>
-          <t>Liz</t>
+          <t>Tigre Toño</t>
         </is>
       </c>
     </row>
@@ -1863,31 +1864,31 @@
         </is>
       </c>
       <c r="B10" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!B10)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!B10)</f>
         <v/>
       </c>
       <c r="C10" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!C10)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!C10)</f>
         <v/>
       </c>
       <c r="D10" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!D10)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!D10)</f>
         <v/>
       </c>
       <c r="E10" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!E10)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!E10)</f>
         <v/>
       </c>
       <c r="F10" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!F10)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!F10)</f>
         <v/>
       </c>
       <c r="G10" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!G10)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!G10)</f>
         <v/>
       </c>
       <c r="H10" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!H10)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!H10)</f>
         <v/>
       </c>
       <c r="I10" s="11">
@@ -2006,31 +2007,31 @@
         </is>
       </c>
       <c r="B11" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!B11)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!B11)</f>
         <v/>
       </c>
       <c r="C11" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!C11)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!C11)</f>
         <v/>
       </c>
       <c r="D11" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!D11)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!D11)</f>
         <v/>
       </c>
       <c r="E11" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!E11)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!E11)</f>
         <v/>
       </c>
       <c r="F11" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!F11)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!F11)</f>
         <v/>
       </c>
       <c r="G11" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!G11)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!G11)</f>
         <v/>
       </c>
       <c r="H11" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!H11)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!H11)</f>
         <v/>
       </c>
       <c r="I11" s="11">
@@ -2149,31 +2150,31 @@
         </is>
       </c>
       <c r="B12" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!B12)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!B12)</f>
         <v/>
       </c>
       <c r="C12" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!C12)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!C12)</f>
         <v/>
       </c>
       <c r="D12" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!D12)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!D12)</f>
         <v/>
       </c>
       <c r="E12" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!E12)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!E12)</f>
         <v/>
       </c>
       <c r="F12" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!F12)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!F12)</f>
         <v/>
       </c>
       <c r="G12" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!G12)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!G12)</f>
         <v/>
       </c>
       <c r="H12" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!H12)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!H12)</f>
         <v/>
       </c>
       <c r="I12" s="11">
@@ -2292,31 +2293,31 @@
         </is>
       </c>
       <c r="B13" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!B13)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!B13)</f>
         <v/>
       </c>
       <c r="C13" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!C13)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!C13)</f>
         <v/>
       </c>
       <c r="D13" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!D13)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!D13)</f>
         <v/>
       </c>
       <c r="E13" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!E13)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!E13)</f>
         <v/>
       </c>
       <c r="F13" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!F13)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!F13)</f>
         <v/>
       </c>
       <c r="G13" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!G13)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!G13)</f>
         <v/>
       </c>
       <c r="H13" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!H13)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!H13)</f>
         <v/>
       </c>
       <c r="I13" s="11">
@@ -2435,31 +2436,31 @@
         </is>
       </c>
       <c r="B14" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!B14)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!B14)</f>
         <v/>
       </c>
       <c r="C14" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!C14)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!C14)</f>
         <v/>
       </c>
       <c r="D14" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!D14)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!D14)</f>
         <v/>
       </c>
       <c r="E14" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!E14)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!E14)</f>
         <v/>
       </c>
       <c r="F14" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!F14)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!F14)</f>
         <v/>
       </c>
       <c r="G14" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!G14)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!G14)</f>
         <v/>
       </c>
       <c r="H14" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!H14)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!H14)</f>
         <v/>
       </c>
       <c r="I14" s="11">
@@ -2578,31 +2579,31 @@
         </is>
       </c>
       <c r="B15" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!B15)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!B15)</f>
         <v/>
       </c>
       <c r="C15" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!C15)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!C15)</f>
         <v/>
       </c>
       <c r="D15" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!D15)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!D15)</f>
         <v/>
       </c>
       <c r="E15" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!E15)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!E15)</f>
         <v/>
       </c>
       <c r="F15" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!F15)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!F15)</f>
         <v/>
       </c>
       <c r="G15" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!G15)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!G15)</f>
         <v/>
       </c>
       <c r="H15" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!H15)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!H15)</f>
         <v/>
       </c>
       <c r="I15" s="11">
@@ -2721,31 +2722,31 @@
         </is>
       </c>
       <c r="B16" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!B16)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!B16)</f>
         <v/>
       </c>
       <c r="C16" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!C16)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!C16)</f>
         <v/>
       </c>
       <c r="D16" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!D16)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!D16)</f>
         <v/>
       </c>
       <c r="E16" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!E16)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!E16)</f>
         <v/>
       </c>
       <c r="F16" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!F16)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!F16)</f>
         <v/>
       </c>
       <c r="G16" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!G16)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!G16)</f>
         <v/>
       </c>
       <c r="H16" s="20">
-        <f>SUM('CortlandEstates:WindwoodCondo'!H16)</f>
+        <f>SUM('CortlandEstates1:WindwoodCondo'!H16)</f>
         <v/>
       </c>
       <c r="I16" s="11">
@@ -3198,7 +3199,7 @@
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>CortlandEstates-101107057</t>
+          <t>CortlandEstates1-101107056</t>
         </is>
       </c>
       <c r="C1" s="18" t="n"/>
@@ -3271,7 +3272,7 @@
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>ClaudiaGil</t>
+          <t>Claudia Gil</t>
         </is>
       </c>
       <c r="B3" s="20">
@@ -3318,7 +3319,7 @@
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>EdgarCamacho</t>
+          <t>Edgar Camacho</t>
         </is>
       </c>
       <c r="B4" s="20">
@@ -3553,7 +3554,7 @@
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>Liz</t>
+          <t>Tigre Toño</t>
         </is>
       </c>
       <c r="B9" s="20">
@@ -3804,7 +3805,7 @@
         <v/>
       </c>
       <c r="E14" s="20">
-        <f>1.00+8.50</f>
+        <f>1.00</f>
         <v/>
       </c>
       <c r="F14" s="20">
@@ -4114,7 +4115,7 @@
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>ParkAstorCondo-101107060</t>
+          <t>CortlandEstates-101107057</t>
         </is>
       </c>
       <c r="C1" s="18" t="n"/>
@@ -4187,7 +4188,7 @@
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>ClaudiaGil</t>
+          <t>Claudia Gil</t>
         </is>
       </c>
       <c r="B3" s="20">
@@ -4234,7 +4235,7 @@
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>EdgarCamacho</t>
+          <t>Edgar Camacho</t>
         </is>
       </c>
       <c r="B4" s="20">
@@ -4246,7 +4247,7 @@
         <v/>
       </c>
       <c r="D4" s="20">
-        <f>0+4.50</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="E4" s="20">
@@ -4344,7 +4345,7 @@
         <v/>
       </c>
       <c r="E6" s="20">
-        <f>9.00</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="F6" s="20">
@@ -4438,7 +4439,7 @@
         <v/>
       </c>
       <c r="E8" s="20">
-        <f>9.00</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="F8" s="20">
@@ -4469,7 +4470,7 @@
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>Liz</t>
+          <t>Tigre Toño</t>
         </is>
       </c>
       <c r="B9" s="20">
@@ -4485,7 +4486,7 @@
         <v/>
       </c>
       <c r="E9" s="20">
-        <f>9.00</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="F9" s="20">
@@ -4575,7 +4576,7 @@
         <v/>
       </c>
       <c r="D11" s="20">
-        <f>0+4.50</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="E11" s="20">
@@ -4622,7 +4623,7 @@
         <v/>
       </c>
       <c r="D12" s="20">
-        <f>0+4.50</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="E12" s="20">
@@ -4673,7 +4674,7 @@
         <v/>
       </c>
       <c r="E13" s="20">
-        <f>9.00</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="F13" s="20">
@@ -4716,11 +4717,11 @@
         <v/>
       </c>
       <c r="D14" s="20">
-        <f>0+4.50</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="E14" s="20">
-        <f>0</f>
+        <f>8.50</f>
         <v/>
       </c>
       <c r="F14" s="20">
@@ -5030,7 +5031,7 @@
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>SpringsAtWeber-101107046</t>
+          <t>ParkAstorCondo-101107060</t>
         </is>
       </c>
       <c r="C1" s="18" t="n"/>
@@ -5103,7 +5104,7 @@
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>ClaudiaGil</t>
+          <t>Claudia Gil</t>
         </is>
       </c>
       <c r="B3" s="20">
@@ -5150,7 +5151,7 @@
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>EdgarCamacho</t>
+          <t>Edgar Camacho</t>
         </is>
       </c>
       <c r="B4" s="20">
@@ -5162,7 +5163,7 @@
         <v/>
       </c>
       <c r="D4" s="20">
-        <f>0</f>
+        <f>0+4.50</f>
         <v/>
       </c>
       <c r="E4" s="20">
@@ -5260,7 +5261,7 @@
         <v/>
       </c>
       <c r="E6" s="20">
-        <f>0</f>
+        <f>9.00</f>
         <v/>
       </c>
       <c r="F6" s="20">
@@ -5354,7 +5355,7 @@
         <v/>
       </c>
       <c r="E8" s="20">
-        <f>0</f>
+        <f>9.00</f>
         <v/>
       </c>
       <c r="F8" s="20">
@@ -5385,7 +5386,7 @@
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>Liz</t>
+          <t>Tigre Toño</t>
         </is>
       </c>
       <c r="B9" s="20">
@@ -5401,7 +5402,7 @@
         <v/>
       </c>
       <c r="E9" s="20">
-        <f>0</f>
+        <f>9.00</f>
         <v/>
       </c>
       <c r="F9" s="20">
@@ -5491,7 +5492,7 @@
         <v/>
       </c>
       <c r="D11" s="20">
-        <f>0</f>
+        <f>0+4.50</f>
         <v/>
       </c>
       <c r="E11" s="20">
@@ -5538,7 +5539,7 @@
         <v/>
       </c>
       <c r="D12" s="20">
-        <f>0</f>
+        <f>0+4.50</f>
         <v/>
       </c>
       <c r="E12" s="20">
@@ -5589,7 +5590,7 @@
         <v/>
       </c>
       <c r="E13" s="20">
-        <f>0</f>
+        <f>9.00</f>
         <v/>
       </c>
       <c r="F13" s="20">
@@ -5632,11 +5633,11 @@
         <v/>
       </c>
       <c r="D14" s="20">
-        <f>0</f>
+        <f>0+4.50</f>
         <v/>
       </c>
       <c r="E14" s="20">
-        <f>2.50</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="F14" s="20">
@@ -5946,7 +5947,7 @@
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>WindwoodCondo-101107012</t>
+          <t>SpringsAtWeber-101107046</t>
         </is>
       </c>
       <c r="C1" s="18" t="n"/>
@@ -6019,7 +6020,923 @@
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>ClaudiaGil</t>
+          <t>Claudia Gil</t>
+        </is>
+      </c>
+      <c r="B3" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C3" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D3" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E3" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F3" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G3" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H3" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I3" s="11">
+        <f>SUM(B3:H3)</f>
+        <v/>
+      </c>
+      <c r="J3" s="12">
+        <f>I3-K3</f>
+        <v/>
+      </c>
+      <c r="K3" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="9" t="inlineStr">
+        <is>
+          <t>Edgar Camacho</t>
+        </is>
+      </c>
+      <c r="B4" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C4" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D4" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E4" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F4" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G4" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H4" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I4" s="11">
+        <f>SUM(B4:H4)</f>
+        <v/>
+      </c>
+      <c r="J4" s="12">
+        <f>I4-K4</f>
+        <v/>
+      </c>
+      <c r="K4" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="9" t="inlineStr">
+        <is>
+          <t>EduardodeSouza</t>
+        </is>
+      </c>
+      <c r="B5" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C5" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D5" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E5" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F5" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G5" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H5" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I5" s="11">
+        <f>SUM(B5:H5)</f>
+        <v/>
+      </c>
+      <c r="J5" s="12">
+        <f>I5-K5</f>
+        <v/>
+      </c>
+      <c r="K5" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="9" t="inlineStr">
+        <is>
+          <t>EdwardoSauca</t>
+        </is>
+      </c>
+      <c r="B6" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C6" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D6" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E6" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F6" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G6" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H6" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I6" s="11">
+        <f>SUM(B6:H6)</f>
+        <v/>
+      </c>
+      <c r="J6" s="12">
+        <f>I6-K6</f>
+        <v/>
+      </c>
+      <c r="K6" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="9" t="inlineStr">
+        <is>
+          <t>GermanCastro</t>
+        </is>
+      </c>
+      <c r="B7" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C7" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D7" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E7" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F7" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G7" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H7" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I7" s="11">
+        <f>SUM(B7:H7)</f>
+        <v/>
+      </c>
+      <c r="J7" s="12">
+        <f>I7-K7</f>
+        <v/>
+      </c>
+      <c r="K7" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="9" t="inlineStr">
+        <is>
+          <t>IsabelaArturo</t>
+        </is>
+      </c>
+      <c r="B8" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C8" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D8" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E8" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F8" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G8" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H8" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I8" s="11">
+        <f>SUM(B8:H8)</f>
+        <v/>
+      </c>
+      <c r="J8" s="12">
+        <f>I8-K8</f>
+        <v/>
+      </c>
+      <c r="K8" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="9" t="inlineStr">
+        <is>
+          <t>Tigre Toño</t>
+        </is>
+      </c>
+      <c r="B9" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C9" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D9" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E9" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F9" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G9" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H9" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I9" s="11">
+        <f>SUM(B9:H9)</f>
+        <v/>
+      </c>
+      <c r="J9" s="12">
+        <f>I9-K9</f>
+        <v/>
+      </c>
+      <c r="K9" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="9" t="inlineStr">
+        <is>
+          <t>LuisJimenez</t>
+        </is>
+      </c>
+      <c r="B10" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C10" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D10" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E10" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F10" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G10" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H10" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I10" s="11">
+        <f>SUM(B10:H10)</f>
+        <v/>
+      </c>
+      <c r="J10" s="12">
+        <f>I10-K10</f>
+        <v/>
+      </c>
+      <c r="K10" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="9" t="inlineStr">
+        <is>
+          <t>ManuelLopez</t>
+        </is>
+      </c>
+      <c r="B11" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C11" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D11" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E11" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F11" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G11" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H11" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I11" s="11">
+        <f>SUM(B11:H11)</f>
+        <v/>
+      </c>
+      <c r="J11" s="12">
+        <f>I11-K11</f>
+        <v/>
+      </c>
+      <c r="K11" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="9" t="inlineStr">
+        <is>
+          <t>MateoLaverde</t>
+        </is>
+      </c>
+      <c r="B12" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C12" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D12" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E12" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F12" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G12" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H12" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I12" s="11">
+        <f>SUM(B12:H12)</f>
+        <v/>
+      </c>
+      <c r="J12" s="12">
+        <f>I12-K12</f>
+        <v/>
+      </c>
+      <c r="K12" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="9" t="inlineStr">
+        <is>
+          <t>MateoMarverde</t>
+        </is>
+      </c>
+      <c r="B13" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C13" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D13" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E13" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F13" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G13" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H13" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I13" s="11">
+        <f>SUM(B13:H13)</f>
+        <v/>
+      </c>
+      <c r="J13" s="12">
+        <f>I13-K13</f>
+        <v/>
+      </c>
+      <c r="K13" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="9" t="inlineStr">
+        <is>
+          <t>PedroForrero</t>
+        </is>
+      </c>
+      <c r="B14" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C14" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D14" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E14" s="20">
+        <f>2.50</f>
+        <v/>
+      </c>
+      <c r="F14" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G14" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H14" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I14" s="11">
+        <f>SUM(B14:H14)</f>
+        <v/>
+      </c>
+      <c r="J14" s="12">
+        <f>I14-K14</f>
+        <v/>
+      </c>
+      <c r="K14" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="9" t="inlineStr">
+        <is>
+          <t>SaraOrtiz</t>
+        </is>
+      </c>
+      <c r="B15" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C15" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D15" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E15" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F15" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G15" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H15" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I15" s="11">
+        <f>SUM(B15:H15)</f>
+        <v/>
+      </c>
+      <c r="J15" s="12">
+        <f>I15-K15</f>
+        <v/>
+      </c>
+      <c r="K15" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="9" t="inlineStr">
+        <is>
+          <t>YuniorOrtiz</t>
+        </is>
+      </c>
+      <c r="B16" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C16" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D16" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E16" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F16" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G16" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H16" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I16" s="11">
+        <f>SUM(B16:H16)</f>
+        <v/>
+      </c>
+      <c r="J16" s="12">
+        <f>I16-K16</f>
+        <v/>
+      </c>
+      <c r="K16" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" ht="33" customHeight="1">
+      <c r="A17" s="5" t="inlineStr">
+        <is>
+          <t>TOTAL HOURS DAY - DAILY</t>
+        </is>
+      </c>
+      <c r="B17" s="11">
+        <f>SUM(B3:B16)</f>
+        <v/>
+      </c>
+      <c r="C17" s="11">
+        <f>SUM(C3:C16)</f>
+        <v/>
+      </c>
+      <c r="D17" s="11">
+        <f>SUM(D3:D16)</f>
+        <v/>
+      </c>
+      <c r="E17" s="11">
+        <f>SUM(E3:E16)</f>
+        <v/>
+      </c>
+      <c r="F17" s="11">
+        <f>SUM(F3:F16)</f>
+        <v/>
+      </c>
+      <c r="G17" s="11">
+        <f>SUM(G3:G16)</f>
+        <v/>
+      </c>
+      <c r="H17" s="11">
+        <f>SUM(H3:H16)</f>
+        <v/>
+      </c>
+      <c r="I17" s="15">
+        <f>SUM(I3:I16)</f>
+        <v/>
+      </c>
+      <c r="J17" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K17" s="13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="33" customHeight="1">
+      <c r="A18" s="6" t="inlineStr">
+        <is>
+          <t>TOTAL REGULAR HOURS - DAILY</t>
+        </is>
+      </c>
+      <c r="B18" s="12">
+        <f>B17-B19</f>
+        <v/>
+      </c>
+      <c r="C18" s="12">
+        <f>C17-C19</f>
+        <v/>
+      </c>
+      <c r="D18" s="12">
+        <f>D17-D19</f>
+        <v/>
+      </c>
+      <c r="E18" s="12">
+        <f>E17-E19</f>
+        <v/>
+      </c>
+      <c r="F18" s="12">
+        <f>F17-F19</f>
+        <v/>
+      </c>
+      <c r="G18" s="12">
+        <f>G17-G19</f>
+        <v/>
+      </c>
+      <c r="H18" s="12">
+        <f>H17-H19</f>
+        <v/>
+      </c>
+      <c r="I18" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J18" s="16">
+        <f>SUM(J3:J16)</f>
+        <v/>
+      </c>
+      <c r="K18" s="13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="33" customHeight="1">
+      <c r="A19" s="7" t="inlineStr">
+        <is>
+          <t>TOTAL OVERTIME HOURS - DAILY</t>
+        </is>
+      </c>
+      <c r="B19" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C19" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D19" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E19" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F19" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G19" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H19" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I19" s="13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J19" s="13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K19" s="17">
+        <f>SUM(K3:K16)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="23" customWidth="1" min="1" max="1"/>
+    <col width="11.86" customWidth="1" min="2" max="2"/>
+    <col width="11.86" customWidth="1" min="3" max="3"/>
+    <col width="11.86" customWidth="1" min="4" max="4"/>
+    <col width="11.86" customWidth="1" min="5" max="5"/>
+    <col width="11.86" customWidth="1" min="6" max="6"/>
+    <col width="11.86" customWidth="1" min="7" max="7"/>
+    <col width="11.86" customWidth="1" min="8" max="8"/>
+    <col width="11.86" customWidth="1" min="9" max="9"/>
+    <col width="11.86" customWidth="1" min="10" max="10"/>
+    <col width="11.86" customWidth="1" min="11" max="11"/>
+    <col width="11.86" customWidth="1" min="12" max="12"/>
+    <col width="11.86" customWidth="1" min="13" max="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="56.25" customHeight="1">
+      <c r="A1" s="1" t="n"/>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>WindwoodCondo-101107012</t>
+        </is>
+      </c>
+      <c r="C1" s="18" t="n"/>
+      <c r="D1" s="18" t="n"/>
+      <c r="E1" s="18" t="n"/>
+      <c r="F1" s="18" t="n"/>
+      <c r="G1" s="18" t="n"/>
+      <c r="H1" s="18" t="n"/>
+      <c r="I1" s="18" t="n"/>
+      <c r="J1" s="18" t="n"/>
+      <c r="K1" s="19" t="n"/>
+    </row>
+    <row r="2" ht="56.25" customHeight="1">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>Names</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>Friday 5</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>Saturday 6</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>Sunday 7</t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>Monday 8</t>
+        </is>
+      </c>
+      <c r="F2" s="4" t="inlineStr">
+        <is>
+          <t>Tuesday 9</t>
+        </is>
+      </c>
+      <c r="G2" s="4" t="inlineStr">
+        <is>
+          <t>Wednesday 10</t>
+        </is>
+      </c>
+      <c r="H2" s="4" t="inlineStr">
+        <is>
+          <t>Thursday 11</t>
+        </is>
+      </c>
+      <c r="I2" s="5" t="inlineStr">
+        <is>
+          <t>TOTAL HOURS - WEEKLY</t>
+        </is>
+      </c>
+      <c r="J2" s="6" t="inlineStr">
+        <is>
+          <t>TOTAL REGULAR HOURS - WEEKLY</t>
+        </is>
+      </c>
+      <c r="K2" s="7" t="inlineStr">
+        <is>
+          <t>TOTAL OVERTIME HOURS - WEEKLY</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="9" t="inlineStr">
+        <is>
+          <t>Claudia Gil</t>
         </is>
       </c>
       <c r="B3" s="20">
@@ -6066,7 +6983,7 @@
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>EdgarCamacho</t>
+          <t>Edgar Camacho</t>
         </is>
       </c>
       <c r="B4" s="20">
@@ -6301,7 +7218,7 @@
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>Liz</t>
+          <t>Tigre Toño</t>
         </is>
       </c>
       <c r="B9" s="20">

</xml_diff>

<commit_message>
Update version - 01/01/2024 ~ First of the year
</commit_message>
<xml_diff>
--- a/test_savedata.xlsx
+++ b/test_savedata.xlsx
@@ -8,11 +8,12 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="General" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CortlandEstates1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="COorMtElandEstatesJBNA" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CortlandEstates" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ParkAstorCondo" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpringsAtWeber" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WindwoodCondo" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="POARMKASTORCONDOSJBNAE" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpringsAtWeber" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WindwoodCondo" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -41,7 +42,7 @@
       <sz val="24"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="21">
     <fill>
       <patternFill/>
     </fill>
@@ -103,6 +104,46 @@
         <fgColor rgb="00b4a7d6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CC66FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000B050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="008ED7DD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000B0F0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FABF8F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0066FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -150,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -212,6 +253,51 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="15" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="17" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="13" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="16" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="18" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="19" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="20" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -579,7 +665,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK19"/>
+  <dimension ref="A1:AK30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -859,35 +945,35 @@
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>Claudia Gil</t>
+          <t>ClaudiaGil</t>
         </is>
       </c>
       <c r="B3" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!B3)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B3)</f>
         <v/>
       </c>
       <c r="C3" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!C3)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C3)</f>
         <v/>
       </c>
       <c r="D3" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!D3)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D3)</f>
         <v/>
       </c>
       <c r="E3" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!E3)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E3)</f>
         <v/>
       </c>
       <c r="F3" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!F3)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F3)</f>
         <v/>
       </c>
       <c r="G3" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!G3)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G3)</f>
         <v/>
       </c>
       <c r="H3" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!H3)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H3)</f>
         <v/>
       </c>
       <c r="I3" s="11">
@@ -995,42 +1081,42 @@
       </c>
       <c r="AK3" s="9" t="inlineStr">
         <is>
-          <t>Claudia Gil</t>
+          <t>ClaudiaGil</t>
         </is>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>Edgar Camacho</t>
+          <t>EdgarCamacho</t>
         </is>
       </c>
       <c r="B4" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!B4)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B4)</f>
         <v/>
       </c>
       <c r="C4" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!C4)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C4)</f>
         <v/>
       </c>
       <c r="D4" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!D4)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D4)</f>
         <v/>
       </c>
       <c r="E4" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!E4)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E4)</f>
         <v/>
       </c>
       <c r="F4" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!F4)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F4)</f>
         <v/>
       </c>
       <c r="G4" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!G4)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G4)</f>
         <v/>
       </c>
       <c r="H4" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!H4)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H4)</f>
         <v/>
       </c>
       <c r="I4" s="11">
@@ -1138,7 +1224,7 @@
       </c>
       <c r="AK4" s="9" t="inlineStr">
         <is>
-          <t>Edgar Camacho</t>
+          <t>EdgarCamacho</t>
         </is>
       </c>
     </row>
@@ -1149,31 +1235,31 @@
         </is>
       </c>
       <c r="B5" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!B5)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B5)</f>
         <v/>
       </c>
       <c r="C5" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!C5)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C5)</f>
         <v/>
       </c>
       <c r="D5" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!D5)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D5)</f>
         <v/>
       </c>
       <c r="E5" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!E5)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E5)</f>
         <v/>
       </c>
       <c r="F5" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!F5)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F5)</f>
         <v/>
       </c>
       <c r="G5" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!G5)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G5)</f>
         <v/>
       </c>
       <c r="H5" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!H5)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H5)</f>
         <v/>
       </c>
       <c r="I5" s="11">
@@ -1292,31 +1378,31 @@
         </is>
       </c>
       <c r="B6" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!B6)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B6)</f>
         <v/>
       </c>
       <c r="C6" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!C6)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C6)</f>
         <v/>
       </c>
       <c r="D6" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!D6)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D6)</f>
         <v/>
       </c>
       <c r="E6" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!E6)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E6)</f>
         <v/>
       </c>
       <c r="F6" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!F6)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F6)</f>
         <v/>
       </c>
       <c r="G6" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!G6)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G6)</f>
         <v/>
       </c>
       <c r="H6" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!H6)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H6)</f>
         <v/>
       </c>
       <c r="I6" s="11">
@@ -1435,31 +1521,31 @@
         </is>
       </c>
       <c r="B7" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!B7)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B7)</f>
         <v/>
       </c>
       <c r="C7" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!C7)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C7)</f>
         <v/>
       </c>
       <c r="D7" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!D7)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D7)</f>
         <v/>
       </c>
       <c r="E7" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!E7)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E7)</f>
         <v/>
       </c>
       <c r="F7" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!F7)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F7)</f>
         <v/>
       </c>
       <c r="G7" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!G7)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G7)</f>
         <v/>
       </c>
       <c r="H7" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!H7)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H7)</f>
         <v/>
       </c>
       <c r="I7" s="11">
@@ -1578,31 +1664,31 @@
         </is>
       </c>
       <c r="B8" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!B8)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B8)</f>
         <v/>
       </c>
       <c r="C8" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!C8)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C8)</f>
         <v/>
       </c>
       <c r="D8" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!D8)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D8)</f>
         <v/>
       </c>
       <c r="E8" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!E8)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E8)</f>
         <v/>
       </c>
       <c r="F8" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!F8)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F8)</f>
         <v/>
       </c>
       <c r="G8" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!G8)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G8)</f>
         <v/>
       </c>
       <c r="H8" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!H8)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H8)</f>
         <v/>
       </c>
       <c r="I8" s="11">
@@ -1717,35 +1803,35 @@
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>Tigre Toño</t>
+          <t>Liz</t>
         </is>
       </c>
       <c r="B9" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!B9)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B9)</f>
         <v/>
       </c>
       <c r="C9" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!C9)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C9)</f>
         <v/>
       </c>
       <c r="D9" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!D9)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D9)</f>
         <v/>
       </c>
       <c r="E9" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!E9)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E9)</f>
         <v/>
       </c>
       <c r="F9" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!F9)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F9)</f>
         <v/>
       </c>
       <c r="G9" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!G9)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G9)</f>
         <v/>
       </c>
       <c r="H9" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!H9)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H9)</f>
         <v/>
       </c>
       <c r="I9" s="11">
@@ -1853,7 +1939,7 @@
       </c>
       <c r="AK9" s="9" t="inlineStr">
         <is>
-          <t>Tigre Toño</t>
+          <t>Liz</t>
         </is>
       </c>
     </row>
@@ -1864,31 +1950,31 @@
         </is>
       </c>
       <c r="B10" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!B10)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B10)</f>
         <v/>
       </c>
       <c r="C10" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!C10)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C10)</f>
         <v/>
       </c>
       <c r="D10" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!D10)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D10)</f>
         <v/>
       </c>
       <c r="E10" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!E10)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E10)</f>
         <v/>
       </c>
       <c r="F10" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!F10)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F10)</f>
         <v/>
       </c>
       <c r="G10" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!G10)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G10)</f>
         <v/>
       </c>
       <c r="H10" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!H10)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H10)</f>
         <v/>
       </c>
       <c r="I10" s="11">
@@ -2007,31 +2093,31 @@
         </is>
       </c>
       <c r="B11" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!B11)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B11)</f>
         <v/>
       </c>
       <c r="C11" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!C11)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C11)</f>
         <v/>
       </c>
       <c r="D11" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!D11)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D11)</f>
         <v/>
       </c>
       <c r="E11" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!E11)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E11)</f>
         <v/>
       </c>
       <c r="F11" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!F11)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F11)</f>
         <v/>
       </c>
       <c r="G11" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!G11)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G11)</f>
         <v/>
       </c>
       <c r="H11" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!H11)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H11)</f>
         <v/>
       </c>
       <c r="I11" s="11">
@@ -2150,31 +2236,31 @@
         </is>
       </c>
       <c r="B12" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!B12)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B12)</f>
         <v/>
       </c>
       <c r="C12" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!C12)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C12)</f>
         <v/>
       </c>
       <c r="D12" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!D12)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D12)</f>
         <v/>
       </c>
       <c r="E12" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!E12)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E12)</f>
         <v/>
       </c>
       <c r="F12" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!F12)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F12)</f>
         <v/>
       </c>
       <c r="G12" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!G12)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G12)</f>
         <v/>
       </c>
       <c r="H12" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!H12)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H12)</f>
         <v/>
       </c>
       <c r="I12" s="11">
@@ -2293,31 +2379,31 @@
         </is>
       </c>
       <c r="B13" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!B13)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B13)</f>
         <v/>
       </c>
       <c r="C13" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!C13)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C13)</f>
         <v/>
       </c>
       <c r="D13" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!D13)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D13)</f>
         <v/>
       </c>
       <c r="E13" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!E13)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E13)</f>
         <v/>
       </c>
       <c r="F13" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!F13)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F13)</f>
         <v/>
       </c>
       <c r="G13" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!G13)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G13)</f>
         <v/>
       </c>
       <c r="H13" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!H13)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H13)</f>
         <v/>
       </c>
       <c r="I13" s="11">
@@ -2436,31 +2522,31 @@
         </is>
       </c>
       <c r="B14" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!B14)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B14)</f>
         <v/>
       </c>
       <c r="C14" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!C14)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C14)</f>
         <v/>
       </c>
       <c r="D14" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!D14)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D14)</f>
         <v/>
       </c>
       <c r="E14" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!E14)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E14)</f>
         <v/>
       </c>
       <c r="F14" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!F14)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F14)</f>
         <v/>
       </c>
       <c r="G14" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!G14)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G14)</f>
         <v/>
       </c>
       <c r="H14" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!H14)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H14)</f>
         <v/>
       </c>
       <c r="I14" s="11">
@@ -2579,31 +2665,31 @@
         </is>
       </c>
       <c r="B15" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!B15)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B15)</f>
         <v/>
       </c>
       <c r="C15" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!C15)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C15)</f>
         <v/>
       </c>
       <c r="D15" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!D15)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D15)</f>
         <v/>
       </c>
       <c r="E15" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!E15)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E15)</f>
         <v/>
       </c>
       <c r="F15" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!F15)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F15)</f>
         <v/>
       </c>
       <c r="G15" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!G15)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G15)</f>
         <v/>
       </c>
       <c r="H15" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!H15)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H15)</f>
         <v/>
       </c>
       <c r="I15" s="11">
@@ -2722,31 +2808,31 @@
         </is>
       </c>
       <c r="B16" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!B16)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!B16)</f>
         <v/>
       </c>
       <c r="C16" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!C16)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!C16)</f>
         <v/>
       </c>
       <c r="D16" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!D16)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!D16)</f>
         <v/>
       </c>
       <c r="E16" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!E16)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!E16)</f>
         <v/>
       </c>
       <c r="F16" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!F16)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!F16)</f>
         <v/>
       </c>
       <c r="G16" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!G16)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!G16)</f>
         <v/>
       </c>
       <c r="H16" s="20">
-        <f>SUM('CortlandEstates1:WindwoodCondo'!H16)</f>
+        <f>SUM('COorMtElandEstatesJBNA:WindwoodCondo'!H16)</f>
         <v/>
       </c>
       <c r="I16" s="11">
@@ -3154,6 +3240,243 @@
       <c r="AI19" s="10" t="n"/>
       <c r="AJ19" s="10" t="n"/>
       <c r="AK19" s="3" t="n"/>
+    </row>
+    <row r="21">
+      <c r="B21" s="23" t="inlineStr">
+        <is>
+          <t># Timesheet</t>
+        </is>
+      </c>
+      <c r="C21" s="23" t="inlineStr">
+        <is>
+          <t>Día</t>
+        </is>
+      </c>
+      <c r="D21" s="23" t="inlineStr">
+        <is>
+          <t>Horas</t>
+        </is>
+      </c>
+      <c r="E21" s="23" t="inlineStr">
+        <is>
+          <t>Trabajo</t>
+        </is>
+      </c>
+      <c r="F21" s="3" t="n"/>
+    </row>
+    <row r="22">
+      <c r="B22" s="23" t="inlineStr">
+        <is>
+          <t>#1</t>
+        </is>
+      </c>
+      <c r="C22" s="24" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D22" s="25">
+        <f>1.0</f>
+        <v/>
+      </c>
+      <c r="E22" s="23" t="inlineStr">
+        <is>
+          <t>COorMtElandEstatesJBNA</t>
+        </is>
+      </c>
+      <c r="F22" s="26">
+        <f>68.0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" s="23" t="inlineStr">
+        <is>
+          <t>#2</t>
+        </is>
+      </c>
+      <c r="C23" s="24" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D23" s="25">
+        <f>8.5</f>
+        <v/>
+      </c>
+      <c r="E23" s="23" t="inlineStr">
+        <is>
+          <t>CortlandEstates</t>
+        </is>
+      </c>
+      <c r="F23" s="27">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" s="23" t="inlineStr">
+        <is>
+          <t>#3</t>
+        </is>
+      </c>
+      <c r="C24" s="24" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D24" s="25">
+        <f>36.0</f>
+        <v/>
+      </c>
+      <c r="E24" s="23" t="inlineStr">
+        <is>
+          <t>ParkAstorCondo</t>
+        </is>
+      </c>
+      <c r="F24" s="28">
+        <f>18.0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" s="23" t="inlineStr">
+        <is>
+          <t>#4</t>
+        </is>
+      </c>
+      <c r="C25" s="29" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D25" s="25">
+        <f>18.0</f>
+        <v/>
+      </c>
+      <c r="E25" s="23" t="inlineStr">
+        <is>
+          <t>POARMKASTORCONDOSJBNAE</t>
+        </is>
+      </c>
+      <c r="F25" s="30">
+        <f>99.0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" s="23" t="inlineStr">
+        <is>
+          <t>#5</t>
+        </is>
+      </c>
+      <c r="C26" s="24" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D26" s="25">
+        <f>2.5</f>
+        <v/>
+      </c>
+      <c r="E26" s="23" t="inlineStr">
+        <is>
+          <t>SpringsAtWeber</t>
+        </is>
+      </c>
+      <c r="F26" s="31">
+        <f>42.0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" s="23" t="inlineStr">
+        <is>
+          <t>#6</t>
+        </is>
+      </c>
+      <c r="C27" s="32" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D27" s="25">
+        <f>68.0</f>
+        <v/>
+      </c>
+      <c r="E27" s="23" t="inlineStr">
+        <is>
+          <t>WindwoodCondo</t>
+        </is>
+      </c>
+      <c r="F27" s="33">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" s="23" t="inlineStr">
+        <is>
+          <t>#7</t>
+        </is>
+      </c>
+      <c r="C28" s="24" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D28" s="25">
+        <f>51.0</f>
+        <v/>
+      </c>
+      <c r="E28" s="23" t="inlineStr">
+        <is>
+          <t>WindwoodCondo</t>
+        </is>
+      </c>
+      <c r="F28" s="34">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" s="23" t="inlineStr">
+        <is>
+          <t>#8</t>
+        </is>
+      </c>
+      <c r="C29" s="35" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D29" s="25">
+        <f>42.0</f>
+        <v/>
+      </c>
+      <c r="E29" s="23" t="inlineStr">
+        <is>
+          <t>WindwoodCondo</t>
+        </is>
+      </c>
+      <c r="F29" s="36">
+        <f>SUM(F22:F28)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" s="3" t="n"/>
+      <c r="C30" s="37" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="D30" s="36">
+        <f>SUM(D22:D29)</f>
+        <v/>
+      </c>
+      <c r="E30" s="3" t="n"/>
+      <c r="F30" s="3" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3199,7 +3522,7 @@
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>CortlandEstates1-101107056</t>
+          <t>COorMtElandEstatesJBNA-101107056</t>
         </is>
       </c>
       <c r="C1" s="18" t="n"/>
@@ -3272,7 +3595,7 @@
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>Claudia Gil</t>
+          <t>ClaudiaGil</t>
         </is>
       </c>
       <c r="B3" s="20">
@@ -3319,7 +3642,7 @@
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>Edgar Camacho</t>
+          <t>EdgarCamacho</t>
         </is>
       </c>
       <c r="B4" s="20">
@@ -3554,7 +3877,7 @@
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>Tigre Toño</t>
+          <t>Liz</t>
         </is>
       </c>
       <c r="B9" s="20">
@@ -4188,7 +4511,7 @@
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>Claudia Gil</t>
+          <t>ClaudiaGil</t>
         </is>
       </c>
       <c r="B3" s="20">
@@ -4235,7 +4558,7 @@
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>Edgar Camacho</t>
+          <t>EdgarCamacho</t>
         </is>
       </c>
       <c r="B4" s="20">
@@ -4470,7 +4793,7 @@
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>Tigre Toño</t>
+          <t>Liz</t>
         </is>
       </c>
       <c r="B9" s="20">
@@ -5104,7 +5427,7 @@
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>Claudia Gil</t>
+          <t>ClaudiaGil</t>
         </is>
       </c>
       <c r="B3" s="20">
@@ -5151,7 +5474,7 @@
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>Edgar Camacho</t>
+          <t>EdgarCamacho</t>
         </is>
       </c>
       <c r="B4" s="20">
@@ -5163,7 +5486,7 @@
         <v/>
       </c>
       <c r="D4" s="20">
-        <f>0+4.50</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="E4" s="20">
@@ -5386,7 +5709,7 @@
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>Tigre Toño</t>
+          <t>Liz</t>
         </is>
       </c>
       <c r="B9" s="20">
@@ -5492,7 +5815,7 @@
         <v/>
       </c>
       <c r="D11" s="20">
-        <f>0+4.50</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="E11" s="20">
@@ -5539,7 +5862,7 @@
         <v/>
       </c>
       <c r="D12" s="20">
-        <f>0+4.50</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="E12" s="20">
@@ -5633,7 +5956,7 @@
         <v/>
       </c>
       <c r="D14" s="20">
-        <f>0+4.50</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="E14" s="20">
@@ -5947,7 +6270,7 @@
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>SpringsAtWeber-101107046</t>
+          <t>POARMKASTORCONDOSJBNAE-101107060</t>
         </is>
       </c>
       <c r="C1" s="18" t="n"/>
@@ -6020,7 +6343,7 @@
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>Claudia Gil</t>
+          <t>ClaudiaGil</t>
         </is>
       </c>
       <c r="B3" s="20">
@@ -6067,7 +6390,7 @@
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>Edgar Camacho</t>
+          <t>EdgarCamacho</t>
         </is>
       </c>
       <c r="B4" s="20">
@@ -6079,7 +6402,7 @@
         <v/>
       </c>
       <c r="D4" s="20">
-        <f>0</f>
+        <f>4.50</f>
         <v/>
       </c>
       <c r="E4" s="20">
@@ -6302,7 +6625,7 @@
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>Tigre Toño</t>
+          <t>Liz</t>
         </is>
       </c>
       <c r="B9" s="20">
@@ -6408,7 +6731,7 @@
         <v/>
       </c>
       <c r="D11" s="20">
-        <f>0</f>
+        <f>4.50</f>
         <v/>
       </c>
       <c r="E11" s="20">
@@ -6455,7 +6778,7 @@
         <v/>
       </c>
       <c r="D12" s="20">
-        <f>0</f>
+        <f>4.50</f>
         <v/>
       </c>
       <c r="E12" s="20">
@@ -6549,11 +6872,11 @@
         <v/>
       </c>
       <c r="D14" s="20">
-        <f>0</f>
+        <f>4.50</f>
         <v/>
       </c>
       <c r="E14" s="20">
-        <f>2.50</f>
+        <f>0</f>
         <v/>
       </c>
       <c r="F14" s="20">
@@ -6863,7 +7186,7 @@
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>WindwoodCondo-101107012</t>
+          <t>SpringsAtWeber-101107046</t>
         </is>
       </c>
       <c r="C1" s="18" t="n"/>
@@ -6936,7 +7259,923 @@
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>Claudia Gil</t>
+          <t>ClaudiaGil</t>
+        </is>
+      </c>
+      <c r="B3" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C3" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D3" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E3" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F3" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G3" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H3" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I3" s="11">
+        <f>SUM(B3:H3)</f>
+        <v/>
+      </c>
+      <c r="J3" s="12">
+        <f>I3-K3</f>
+        <v/>
+      </c>
+      <c r="K3" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="9" t="inlineStr">
+        <is>
+          <t>EdgarCamacho</t>
+        </is>
+      </c>
+      <c r="B4" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C4" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D4" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E4" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F4" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G4" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H4" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I4" s="11">
+        <f>SUM(B4:H4)</f>
+        <v/>
+      </c>
+      <c r="J4" s="12">
+        <f>I4-K4</f>
+        <v/>
+      </c>
+      <c r="K4" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="9" t="inlineStr">
+        <is>
+          <t>EduardodeSouza</t>
+        </is>
+      </c>
+      <c r="B5" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C5" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D5" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E5" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F5" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G5" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H5" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I5" s="11">
+        <f>SUM(B5:H5)</f>
+        <v/>
+      </c>
+      <c r="J5" s="12">
+        <f>I5-K5</f>
+        <v/>
+      </c>
+      <c r="K5" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="9" t="inlineStr">
+        <is>
+          <t>EdwardoSauca</t>
+        </is>
+      </c>
+      <c r="B6" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C6" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D6" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E6" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F6" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G6" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H6" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I6" s="11">
+        <f>SUM(B6:H6)</f>
+        <v/>
+      </c>
+      <c r="J6" s="12">
+        <f>I6-K6</f>
+        <v/>
+      </c>
+      <c r="K6" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="9" t="inlineStr">
+        <is>
+          <t>GermanCastro</t>
+        </is>
+      </c>
+      <c r="B7" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C7" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D7" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E7" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F7" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G7" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H7" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I7" s="11">
+        <f>SUM(B7:H7)</f>
+        <v/>
+      </c>
+      <c r="J7" s="12">
+        <f>I7-K7</f>
+        <v/>
+      </c>
+      <c r="K7" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="9" t="inlineStr">
+        <is>
+          <t>IsabelaArturo</t>
+        </is>
+      </c>
+      <c r="B8" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C8" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D8" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E8" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F8" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G8" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H8" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I8" s="11">
+        <f>SUM(B8:H8)</f>
+        <v/>
+      </c>
+      <c r="J8" s="12">
+        <f>I8-K8</f>
+        <v/>
+      </c>
+      <c r="K8" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="9" t="inlineStr">
+        <is>
+          <t>Liz</t>
+        </is>
+      </c>
+      <c r="B9" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C9" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D9" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E9" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F9" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G9" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H9" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I9" s="11">
+        <f>SUM(B9:H9)</f>
+        <v/>
+      </c>
+      <c r="J9" s="12">
+        <f>I9-K9</f>
+        <v/>
+      </c>
+      <c r="K9" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="9" t="inlineStr">
+        <is>
+          <t>LuisJimenez</t>
+        </is>
+      </c>
+      <c r="B10" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C10" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D10" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E10" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F10" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G10" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H10" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I10" s="11">
+        <f>SUM(B10:H10)</f>
+        <v/>
+      </c>
+      <c r="J10" s="12">
+        <f>I10-K10</f>
+        <v/>
+      </c>
+      <c r="K10" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="A11" s="9" t="inlineStr">
+        <is>
+          <t>ManuelLopez</t>
+        </is>
+      </c>
+      <c r="B11" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C11" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D11" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E11" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F11" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G11" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H11" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I11" s="11">
+        <f>SUM(B11:H11)</f>
+        <v/>
+      </c>
+      <c r="J11" s="12">
+        <f>I11-K11</f>
+        <v/>
+      </c>
+      <c r="K11" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="9" t="inlineStr">
+        <is>
+          <t>MateoLaverde</t>
+        </is>
+      </c>
+      <c r="B12" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C12" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D12" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E12" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F12" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G12" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H12" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I12" s="11">
+        <f>SUM(B12:H12)</f>
+        <v/>
+      </c>
+      <c r="J12" s="12">
+        <f>I12-K12</f>
+        <v/>
+      </c>
+      <c r="K12" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="9" t="inlineStr">
+        <is>
+          <t>MateoMarverde</t>
+        </is>
+      </c>
+      <c r="B13" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C13" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D13" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E13" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F13" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G13" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H13" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I13" s="11">
+        <f>SUM(B13:H13)</f>
+        <v/>
+      </c>
+      <c r="J13" s="12">
+        <f>I13-K13</f>
+        <v/>
+      </c>
+      <c r="K13" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1">
+      <c r="A14" s="9" t="inlineStr">
+        <is>
+          <t>PedroForrero</t>
+        </is>
+      </c>
+      <c r="B14" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C14" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D14" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E14" s="20">
+        <f>2.50</f>
+        <v/>
+      </c>
+      <c r="F14" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G14" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H14" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I14" s="11">
+        <f>SUM(B14:H14)</f>
+        <v/>
+      </c>
+      <c r="J14" s="12">
+        <f>I14-K14</f>
+        <v/>
+      </c>
+      <c r="K14" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="A15" s="9" t="inlineStr">
+        <is>
+          <t>SaraOrtiz</t>
+        </is>
+      </c>
+      <c r="B15" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C15" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D15" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E15" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F15" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G15" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H15" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I15" s="11">
+        <f>SUM(B15:H15)</f>
+        <v/>
+      </c>
+      <c r="J15" s="12">
+        <f>I15-K15</f>
+        <v/>
+      </c>
+      <c r="K15" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1">
+      <c r="A16" s="9" t="inlineStr">
+        <is>
+          <t>YuniorOrtiz</t>
+        </is>
+      </c>
+      <c r="B16" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C16" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D16" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E16" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F16" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G16" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H16" s="20">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I16" s="11">
+        <f>SUM(B16:H16)</f>
+        <v/>
+      </c>
+      <c r="J16" s="12">
+        <f>I16-K16</f>
+        <v/>
+      </c>
+      <c r="K16" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" ht="33" customHeight="1">
+      <c r="A17" s="5" t="inlineStr">
+        <is>
+          <t>TOTAL HOURS DAY - DAILY</t>
+        </is>
+      </c>
+      <c r="B17" s="11">
+        <f>SUM(B3:B16)</f>
+        <v/>
+      </c>
+      <c r="C17" s="11">
+        <f>SUM(C3:C16)</f>
+        <v/>
+      </c>
+      <c r="D17" s="11">
+        <f>SUM(D3:D16)</f>
+        <v/>
+      </c>
+      <c r="E17" s="11">
+        <f>SUM(E3:E16)</f>
+        <v/>
+      </c>
+      <c r="F17" s="11">
+        <f>SUM(F3:F16)</f>
+        <v/>
+      </c>
+      <c r="G17" s="11">
+        <f>SUM(G3:G16)</f>
+        <v/>
+      </c>
+      <c r="H17" s="11">
+        <f>SUM(H3:H16)</f>
+        <v/>
+      </c>
+      <c r="I17" s="15">
+        <f>SUM(I3:I16)</f>
+        <v/>
+      </c>
+      <c r="J17" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K17" s="13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="33" customHeight="1">
+      <c r="A18" s="6" t="inlineStr">
+        <is>
+          <t>TOTAL REGULAR HOURS - DAILY</t>
+        </is>
+      </c>
+      <c r="B18" s="12">
+        <f>B17-B19</f>
+        <v/>
+      </c>
+      <c r="C18" s="12">
+        <f>C17-C19</f>
+        <v/>
+      </c>
+      <c r="D18" s="12">
+        <f>D17-D19</f>
+        <v/>
+      </c>
+      <c r="E18" s="12">
+        <f>E17-E19</f>
+        <v/>
+      </c>
+      <c r="F18" s="12">
+        <f>F17-F19</f>
+        <v/>
+      </c>
+      <c r="G18" s="12">
+        <f>G17-G19</f>
+        <v/>
+      </c>
+      <c r="H18" s="12">
+        <f>H17-H19</f>
+        <v/>
+      </c>
+      <c r="I18" s="12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J18" s="16">
+        <f>SUM(J3:J16)</f>
+        <v/>
+      </c>
+      <c r="K18" s="13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="33" customHeight="1">
+      <c r="A19" s="7" t="inlineStr">
+        <is>
+          <t>TOTAL OVERTIME HOURS - DAILY</t>
+        </is>
+      </c>
+      <c r="B19" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="C19" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="D19" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="E19" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="F19" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G19" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="H19" s="13">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="I19" s="13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J19" s="13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K19" s="17">
+        <f>SUM(K3:K16)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="23" customWidth="1" min="1" max="1"/>
+    <col width="11.86" customWidth="1" min="2" max="2"/>
+    <col width="11.86" customWidth="1" min="3" max="3"/>
+    <col width="11.86" customWidth="1" min="4" max="4"/>
+    <col width="11.86" customWidth="1" min="5" max="5"/>
+    <col width="11.86" customWidth="1" min="6" max="6"/>
+    <col width="11.86" customWidth="1" min="7" max="7"/>
+    <col width="11.86" customWidth="1" min="8" max="8"/>
+    <col width="11.86" customWidth="1" min="9" max="9"/>
+    <col width="11.86" customWidth="1" min="10" max="10"/>
+    <col width="11.86" customWidth="1" min="11" max="11"/>
+    <col width="11.86" customWidth="1" min="12" max="12"/>
+    <col width="11.86" customWidth="1" min="13" max="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="56.25" customHeight="1">
+      <c r="A1" s="1" t="n"/>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>WindwoodCondo-101107012</t>
+        </is>
+      </c>
+      <c r="C1" s="18" t="n"/>
+      <c r="D1" s="18" t="n"/>
+      <c r="E1" s="18" t="n"/>
+      <c r="F1" s="18" t="n"/>
+      <c r="G1" s="18" t="n"/>
+      <c r="H1" s="18" t="n"/>
+      <c r="I1" s="18" t="n"/>
+      <c r="J1" s="18" t="n"/>
+      <c r="K1" s="19" t="n"/>
+    </row>
+    <row r="2" ht="56.25" customHeight="1">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>Names</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>Friday 5</t>
+        </is>
+      </c>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>Saturday 6</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>Sunday 7</t>
+        </is>
+      </c>
+      <c r="E2" s="4" t="inlineStr">
+        <is>
+          <t>Monday 8</t>
+        </is>
+      </c>
+      <c r="F2" s="4" t="inlineStr">
+        <is>
+          <t>Tuesday 9</t>
+        </is>
+      </c>
+      <c r="G2" s="4" t="inlineStr">
+        <is>
+          <t>Wednesday 10</t>
+        </is>
+      </c>
+      <c r="H2" s="4" t="inlineStr">
+        <is>
+          <t>Thursday 11</t>
+        </is>
+      </c>
+      <c r="I2" s="5" t="inlineStr">
+        <is>
+          <t>TOTAL HOURS - WEEKLY</t>
+        </is>
+      </c>
+      <c r="J2" s="6" t="inlineStr">
+        <is>
+          <t>TOTAL REGULAR HOURS - WEEKLY</t>
+        </is>
+      </c>
+      <c r="K2" s="7" t="inlineStr">
+        <is>
+          <t>TOTAL OVERTIME HOURS - WEEKLY</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="9" t="inlineStr">
+        <is>
+          <t>ClaudiaGil</t>
         </is>
       </c>
       <c r="B3" s="20">
@@ -6983,7 +8222,7 @@
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>Edgar Camacho</t>
+          <t>EdgarCamacho</t>
         </is>
       </c>
       <c r="B4" s="20">
@@ -7218,7 +8457,7 @@
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>Tigre Toño</t>
+          <t>Liz</t>
         </is>
       </c>
       <c r="B9" s="20">

</xml_diff>